<commit_message>
fixed timer condition in detect-update; changed get data code for daily pos rate; removed trends data collection from build-data
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1260,10 +1260,10 @@
         <v>1730</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="E21" t="n">
         <v>45</v>
@@ -1518,10 +1518,10 @@
         <v>2603</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>2602</v>
+        <v>2603</v>
       </c>
       <c r="E27" t="n">
         <v>303</v>
@@ -1819,10 +1819,10 @@
         <v>2689</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>2688</v>
+        <v>2689</v>
       </c>
       <c r="E34" t="n">
         <v>396</v>
@@ -1991,10 +1991,10 @@
         <v>2416</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="E38" t="n">
         <v>557</v>
@@ -2163,10 +2163,10 @@
         <v>2717</v>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>2715</v>
+        <v>2717</v>
       </c>
       <c r="E42" t="n">
         <v>515</v>
@@ -2206,10 +2206,10 @@
         <v>1518</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>1516</v>
+        <v>1518</v>
       </c>
       <c r="E43" t="n">
         <v>486</v>
@@ -2292,10 +2292,10 @@
         <v>3458</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>3457</v>
+        <v>3458</v>
       </c>
       <c r="E45" t="n">
         <v>292</v>
@@ -2375,13 +2375,13 @@
         </is>
       </c>
       <c r="B47" t="n">
+        <v>3262</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="n">
         <v>3261</v>
-      </c>
-      <c r="C47" t="n">
-        <v>3</v>
-      </c>
-      <c r="D47" t="n">
-        <v>3258</v>
       </c>
       <c r="E47" t="n">
         <v>580</v>
@@ -2408,7 +2408,7 @@
         <v>562</v>
       </c>
       <c r="M47" t="n">
-        <v>62104</v>
+        <v>62105</v>
       </c>
     </row>
     <row r="48">
@@ -2421,10 +2421,10 @@
         <v>3907</v>
       </c>
       <c r="C48" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>3901</v>
+        <v>3907</v>
       </c>
       <c r="E48" t="n">
         <v>600</v>
@@ -2451,7 +2451,7 @@
         <v>596</v>
       </c>
       <c r="M48" t="n">
-        <v>66011</v>
+        <v>66012</v>
       </c>
     </row>
     <row r="49">
@@ -2464,10 +2464,10 @@
         <v>4022</v>
       </c>
       <c r="C49" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4016</v>
+        <v>4022</v>
       </c>
       <c r="E49" t="n">
         <v>505</v>
@@ -2494,7 +2494,7 @@
         <v>631</v>
       </c>
       <c r="M49" t="n">
-        <v>70033</v>
+        <v>70034</v>
       </c>
     </row>
     <row r="50">
@@ -2537,7 +2537,7 @@
         <v>659</v>
       </c>
       <c r="M50" t="n">
-        <v>71737</v>
+        <v>71738</v>
       </c>
     </row>
     <row r="51">
@@ -2550,10 +2550,10 @@
         <v>1098</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E51" t="n">
         <v>479</v>
@@ -2580,7 +2580,7 @@
         <v>694</v>
       </c>
       <c r="M51" t="n">
-        <v>72835</v>
+        <v>72836</v>
       </c>
     </row>
     <row r="52">
@@ -2593,10 +2593,10 @@
         <v>4287</v>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>4286</v>
+        <v>4287</v>
       </c>
       <c r="E52" t="n">
         <v>386</v>
@@ -2623,7 +2623,7 @@
         <v>731</v>
       </c>
       <c r="M52" t="n">
-        <v>77122</v>
+        <v>77123</v>
       </c>
     </row>
     <row r="53">
@@ -2636,10 +2636,10 @@
         <v>3825</v>
       </c>
       <c r="C53" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>3814</v>
+        <v>3825</v>
       </c>
       <c r="E53" t="n">
         <v>379</v>
@@ -2666,7 +2666,7 @@
         <v>778</v>
       </c>
       <c r="M53" t="n">
-        <v>80947</v>
+        <v>80948</v>
       </c>
     </row>
     <row r="54">
@@ -2679,10 +2679,10 @@
         <v>3705</v>
       </c>
       <c r="C54" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>3697</v>
+        <v>3705</v>
       </c>
       <c r="E54" t="n">
         <v>605</v>
@@ -2709,7 +2709,7 @@
         <v>826</v>
       </c>
       <c r="M54" t="n">
-        <v>84652</v>
+        <v>84653</v>
       </c>
     </row>
     <row r="55">
@@ -2719,13 +2719,13 @@
         </is>
       </c>
       <c r="B55" t="n">
+        <v>4239</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="n">
         <v>4238</v>
-      </c>
-      <c r="C55" t="n">
-        <v>47</v>
-      </c>
-      <c r="D55" t="n">
-        <v>4191</v>
       </c>
       <c r="E55" t="n">
         <v>644</v>
@@ -2752,7 +2752,7 @@
         <v>864</v>
       </c>
       <c r="M55" t="n">
-        <v>88890</v>
+        <v>88892</v>
       </c>
     </row>
     <row r="56">
@@ -2765,10 +2765,10 @@
         <v>3491</v>
       </c>
       <c r="C56" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>3472</v>
+        <v>3491</v>
       </c>
       <c r="E56" t="n">
         <v>700</v>
@@ -2795,7 +2795,7 @@
         <v>899</v>
       </c>
       <c r="M56" t="n">
-        <v>92381</v>
+        <v>92383</v>
       </c>
     </row>
     <row r="57">
@@ -2808,10 +2808,10 @@
         <v>2216</v>
       </c>
       <c r="C57" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>2212</v>
+        <v>2216</v>
       </c>
       <c r="E57" t="n">
         <v>626</v>
@@ -2838,7 +2838,7 @@
         <v>940</v>
       </c>
       <c r="M57" t="n">
-        <v>94597</v>
+        <v>94599</v>
       </c>
     </row>
     <row r="58">
@@ -2851,10 +2851,10 @@
         <v>1785</v>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>1782</v>
+        <v>1785</v>
       </c>
       <c r="E58" t="n">
         <v>950</v>
@@ -2881,7 +2881,7 @@
         <v>974</v>
       </c>
       <c r="M58" t="n">
-        <v>96382</v>
+        <v>96384</v>
       </c>
     </row>
     <row r="59">
@@ -2894,10 +2894,10 @@
         <v>4274</v>
       </c>
       <c r="C59" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>4210</v>
+        <v>4274</v>
       </c>
       <c r="E59" t="n">
         <v>622</v>
@@ -2924,7 +2924,7 @@
         <v>1015</v>
       </c>
       <c r="M59" t="n">
-        <v>100656</v>
+        <v>100658</v>
       </c>
     </row>
     <row r="60">
@@ -2934,13 +2934,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4540</v>
+        <v>4570</v>
       </c>
       <c r="C60" t="n">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="D60" t="n">
-        <v>4469</v>
+        <v>4541</v>
       </c>
       <c r="E60" t="n">
         <v>595</v>
@@ -2967,7 +2967,7 @@
         <v>1049</v>
       </c>
       <c r="M60" t="n">
-        <v>105196</v>
+        <v>105228</v>
       </c>
     </row>
     <row r="61">
@@ -2977,13 +2977,13 @@
         </is>
       </c>
       <c r="B61" t="n">
+        <v>4637</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="n">
         <v>4636</v>
-      </c>
-      <c r="C61" t="n">
-        <v>68</v>
-      </c>
-      <c r="D61" t="n">
-        <v>4568</v>
       </c>
       <c r="E61" t="n">
         <v>654</v>
@@ -3010,7 +3010,7 @@
         <v>1089</v>
       </c>
       <c r="M61" t="n">
-        <v>109832</v>
+        <v>109865</v>
       </c>
     </row>
     <row r="62">
@@ -3020,13 +3020,13 @@
         </is>
       </c>
       <c r="B62" t="n">
+        <v>4686</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="n">
         <v>4685</v>
-      </c>
-      <c r="C62" t="n">
-        <v>11</v>
-      </c>
-      <c r="D62" t="n">
-        <v>4674</v>
       </c>
       <c r="E62" t="n">
         <v>795</v>
@@ -3053,7 +3053,7 @@
         <v>1134</v>
       </c>
       <c r="M62" t="n">
-        <v>114517</v>
+        <v>114551</v>
       </c>
     </row>
     <row r="63">
@@ -3063,13 +3063,13 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>5751</v>
+        <v>5760</v>
       </c>
       <c r="C63" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
-        <v>5745</v>
+        <v>5752</v>
       </c>
       <c r="E63" t="n">
         <v>654</v>
@@ -3096,7 +3096,7 @@
         <v>1167</v>
       </c>
       <c r="M63" t="n">
-        <v>120268</v>
+        <v>120311</v>
       </c>
     </row>
     <row r="64">
@@ -3106,10 +3106,10 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2823</v>
+        <v>2837</v>
       </c>
       <c r="C64" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D64" t="n">
         <v>2822</v>
@@ -3139,7 +3139,7 @@
         <v>1207</v>
       </c>
       <c r="M64" t="n">
-        <v>123091</v>
+        <v>123148</v>
       </c>
     </row>
     <row r="65">
@@ -3182,7 +3182,7 @@
         <v>1237</v>
       </c>
       <c r="M65" t="n">
-        <v>124746</v>
+        <v>124803</v>
       </c>
     </row>
     <row r="66">
@@ -3192,13 +3192,13 @@
         </is>
       </c>
       <c r="B66" t="n">
+        <v>5212</v>
+      </c>
+      <c r="C66" t="n">
+        <v>3</v>
+      </c>
+      <c r="D66" t="n">
         <v>5209</v>
-      </c>
-      <c r="C66" t="n">
-        <v>11</v>
-      </c>
-      <c r="D66" t="n">
-        <v>5198</v>
       </c>
       <c r="E66" t="n">
         <v>526</v>
@@ -3225,7 +3225,7 @@
         <v>1272</v>
       </c>
       <c r="M66" t="n">
-        <v>129955</v>
+        <v>130015</v>
       </c>
     </row>
     <row r="67">
@@ -3235,13 +3235,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5773</v>
+        <v>5797</v>
       </c>
       <c r="C67" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D67" t="n">
-        <v>5729</v>
+        <v>5772</v>
       </c>
       <c r="E67" t="n">
         <v>838</v>
@@ -3268,7 +3268,7 @@
         <v>1308</v>
       </c>
       <c r="M67" t="n">
-        <v>135728</v>
+        <v>135812</v>
       </c>
     </row>
     <row r="68">
@@ -3278,13 +3278,13 @@
         </is>
       </c>
       <c r="B68" t="n">
+        <v>5580</v>
+      </c>
+      <c r="C68" t="n">
+        <v>10</v>
+      </c>
+      <c r="D68" t="n">
         <v>5570</v>
-      </c>
-      <c r="C68" t="n">
-        <v>21</v>
-      </c>
-      <c r="D68" t="n">
-        <v>5549</v>
       </c>
       <c r="E68" t="n">
         <v>624</v>
@@ -3299,10 +3299,10 @@
         <v>39</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K68" t="n">
         <v>22437</v>
@@ -3311,7 +3311,7 @@
         <v>1347</v>
       </c>
       <c r="M68" t="n">
-        <v>141298</v>
+        <v>141392</v>
       </c>
     </row>
     <row r="69">
@@ -3321,40 +3321,40 @@
         </is>
       </c>
       <c r="B69" t="n">
+        <v>5800</v>
+      </c>
+      <c r="C69" t="n">
+        <v>17</v>
+      </c>
+      <c r="D69" t="n">
         <v>5783</v>
       </c>
-      <c r="C69" t="n">
-        <v>37</v>
-      </c>
-      <c r="D69" t="n">
-        <v>5746</v>
-      </c>
       <c r="E69" t="n">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H69" t="n">
         <v>33</v>
       </c>
       <c r="I69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K69" t="n">
-        <v>23081</v>
+        <v>23079</v>
       </c>
       <c r="L69" t="n">
         <v>1380</v>
       </c>
       <c r="M69" t="n">
-        <v>147081</v>
+        <v>147192</v>
       </c>
     </row>
     <row r="70">
@@ -3364,22 +3364,22 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5821</v>
+        <v>5832</v>
       </c>
       <c r="C70" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D70" t="n">
-        <v>5773</v>
+        <v>5820</v>
       </c>
       <c r="E70" t="n">
         <v>593</v>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H70" t="n">
         <v>20</v>
@@ -3391,13 +3391,13 @@
         <v>20</v>
       </c>
       <c r="K70" t="n">
-        <v>23674</v>
+        <v>23672</v>
       </c>
       <c r="L70" t="n">
         <v>1400</v>
       </c>
       <c r="M70" t="n">
-        <v>152902</v>
+        <v>153024</v>
       </c>
     </row>
     <row r="71">
@@ -3407,13 +3407,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3087</v>
+        <v>3100</v>
       </c>
       <c r="C71" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D71" t="n">
-        <v>3056</v>
+        <v>3086</v>
       </c>
       <c r="E71" t="n">
         <v>389</v>
@@ -3428,19 +3428,19 @@
         <v>25</v>
       </c>
       <c r="I71" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K71" t="n">
-        <v>24063</v>
+        <v>24061</v>
       </c>
       <c r="L71" t="n">
         <v>1425</v>
       </c>
       <c r="M71" t="n">
-        <v>155989</v>
+        <v>156124</v>
       </c>
     </row>
     <row r="72">
@@ -3453,16 +3453,16 @@
         <v>1227</v>
       </c>
       <c r="C72" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>1214</v>
+        <v>1227</v>
       </c>
       <c r="E72" t="n">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G72" t="n">
         <v>463</v>
@@ -3477,13 +3477,13 @@
         <v>27</v>
       </c>
       <c r="K72" t="n">
-        <v>24527</v>
+        <v>24526</v>
       </c>
       <c r="L72" t="n">
         <v>1452</v>
       </c>
       <c r="M72" t="n">
-        <v>157216</v>
+        <v>157351</v>
       </c>
     </row>
     <row r="73">
@@ -3493,19 +3493,19 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6237</v>
+        <v>6395</v>
       </c>
       <c r="C73" t="n">
-        <v>478</v>
+        <v>156</v>
       </c>
       <c r="D73" t="n">
-        <v>5759</v>
+        <v>6239</v>
       </c>
       <c r="E73" t="n">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
         <v>522</v>
@@ -3514,19 +3514,19 @@
         <v>37</v>
       </c>
       <c r="I73" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K73" t="n">
-        <v>25050</v>
+        <v>25048</v>
       </c>
       <c r="L73" t="n">
         <v>1489</v>
       </c>
       <c r="M73" t="n">
-        <v>163453</v>
+        <v>163746</v>
       </c>
     </row>
     <row r="74">
@@ -3536,40 +3536,40 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>4998</v>
+        <v>5559</v>
       </c>
       <c r="C74" t="n">
-        <v>2668</v>
+        <v>557</v>
       </c>
       <c r="D74" t="n">
-        <v>2330</v>
+        <v>5002</v>
       </c>
       <c r="E74" t="n">
         <v>376</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H74" t="n">
         <v>35</v>
       </c>
       <c r="I74" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K74" t="n">
-        <v>25426</v>
+        <v>25424</v>
       </c>
       <c r="L74" t="n">
         <v>1524</v>
       </c>
       <c r="M74" t="n">
-        <v>168451</v>
+        <v>169305</v>
       </c>
     </row>
     <row r="75">
@@ -3579,40 +3579,40 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2126</v>
+        <v>4217</v>
       </c>
       <c r="C75" t="n">
-        <v>1627</v>
+        <v>2109</v>
       </c>
       <c r="D75" t="n">
-        <v>499</v>
+        <v>2108</v>
       </c>
       <c r="E75" t="n">
         <v>609</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H75" t="n">
         <v>21</v>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K75" t="n">
-        <v>26035</v>
+        <v>26033</v>
       </c>
       <c r="L75" t="n">
         <v>1545</v>
       </c>
       <c r="M75" t="n">
-        <v>170577</v>
+        <v>173522</v>
       </c>
     </row>
     <row r="76">
@@ -3622,40 +3622,40 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>663</v>
+        <v>2803</v>
       </c>
       <c r="C76" t="n">
-        <v>572</v>
+        <v>2151</v>
       </c>
       <c r="D76" t="n">
-        <v>91</v>
+        <v>652</v>
       </c>
       <c r="E76" t="n">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F76" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="H76" t="n">
+        <v>38</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
         <v>37</v>
       </c>
-      <c r="I76" t="n">
-        <v>17</v>
-      </c>
-      <c r="J76" t="n">
-        <v>20</v>
-      </c>
       <c r="K76" t="n">
-        <v>26629</v>
+        <v>26625</v>
       </c>
       <c r="L76" t="n">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="M76" t="n">
-        <v>171240</v>
+        <v>176325</v>
       </c>
     </row>
     <row r="77">
@@ -3665,40 +3665,83 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>118</v>
+        <v>855</v>
       </c>
       <c r="C77" t="n">
-        <v>118</v>
+        <v>739</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E77" t="n">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F77" t="n">
-        <v>649</v>
+        <v>6</v>
       </c>
       <c r="G77" t="n">
-        <v>2</v>
+        <v>642</v>
       </c>
       <c r="H77" t="n">
+        <v>18</v>
+      </c>
+      <c r="I77" t="n">
+        <v>4</v>
+      </c>
+      <c r="J77" t="n">
         <v>14</v>
       </c>
-      <c r="I77" t="n">
-        <v>14</v>
-      </c>
-      <c r="J77" t="n">
-        <v>0</v>
-      </c>
       <c r="K77" t="n">
-        <v>27280</v>
+        <v>27273</v>
       </c>
       <c r="L77" t="n">
-        <v>1596</v>
+        <v>1601</v>
       </c>
       <c r="M77" t="n">
-        <v>171358</v>
+        <v>177180</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2020-05-16</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>63</v>
+      </c>
+      <c r="C78" t="n">
+        <v>63</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>505</v>
+      </c>
+      <c r="F78" t="n">
+        <v>502</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3</v>
+      </c>
+      <c r="H78" t="n">
+        <v>6</v>
+      </c>
+      <c r="I78" t="n">
+        <v>6</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="n">
+        <v>27778</v>
+      </c>
+      <c r="L78" t="n">
+        <v>1607</v>
+      </c>
+      <c r="M78" t="n">
+        <v>177243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comment edit in pos-rate
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1386,13 +1386,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="E24" t="n">
         <v>105</v>
@@ -1419,7 +1419,7 @@
         <v>24</v>
       </c>
       <c r="M24" t="n">
-        <v>9267</v>
+        <v>9266</v>
       </c>
     </row>
     <row r="25">
@@ -1462,7 +1462,7 @@
         <v>29</v>
       </c>
       <c r="M25" t="n">
-        <v>10869</v>
+        <v>10868</v>
       </c>
     </row>
     <row r="26">
@@ -1505,7 +1505,7 @@
         <v>35</v>
       </c>
       <c r="M26" t="n">
-        <v>13181</v>
+        <v>13180</v>
       </c>
     </row>
     <row r="27">
@@ -1548,7 +1548,7 @@
         <v>44</v>
       </c>
       <c r="M27" t="n">
-        <v>15784</v>
+        <v>15783</v>
       </c>
     </row>
     <row r="28">
@@ -1591,7 +1591,7 @@
         <v>47</v>
       </c>
       <c r="M28" t="n">
-        <v>17943</v>
+        <v>17942</v>
       </c>
     </row>
     <row r="29">
@@ -1601,13 +1601,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E29" t="n">
         <v>288</v>
@@ -1634,7 +1634,7 @@
         <v>58</v>
       </c>
       <c r="M29" t="n">
-        <v>19214</v>
+        <v>19212</v>
       </c>
     </row>
     <row r="30">
@@ -1677,7 +1677,7 @@
         <v>76</v>
       </c>
       <c r="M30" t="n">
-        <v>20846</v>
+        <v>20844</v>
       </c>
     </row>
     <row r="31">
@@ -1720,7 +1720,7 @@
         <v>91</v>
       </c>
       <c r="M31" t="n">
-        <v>22804</v>
+        <v>22802</v>
       </c>
     </row>
     <row r="32">
@@ -1763,7 +1763,7 @@
         <v>113</v>
       </c>
       <c r="M32" t="n">
-        <v>25117</v>
+        <v>25115</v>
       </c>
     </row>
     <row r="33">
@@ -1806,7 +1806,7 @@
         <v>135</v>
       </c>
       <c r="M33" t="n">
-        <v>27650</v>
+        <v>27648</v>
       </c>
     </row>
     <row r="34">
@@ -1816,13 +1816,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="E34" t="n">
         <v>396</v>
@@ -1849,7 +1849,7 @@
         <v>157</v>
       </c>
       <c r="M34" t="n">
-        <v>30339</v>
+        <v>30336</v>
       </c>
     </row>
     <row r="35">
@@ -1892,7 +1892,7 @@
         <v>189</v>
       </c>
       <c r="M35" t="n">
-        <v>33128</v>
+        <v>33125</v>
       </c>
     </row>
     <row r="36">
@@ -1935,7 +1935,7 @@
         <v>214</v>
       </c>
       <c r="M36" t="n">
-        <v>34764</v>
+        <v>34761</v>
       </c>
     </row>
     <row r="37">
@@ -1978,7 +1978,7 @@
         <v>248</v>
       </c>
       <c r="M37" t="n">
-        <v>35859</v>
+        <v>35856</v>
       </c>
     </row>
     <row r="38">
@@ -1988,10 +1988,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2416</v>
+        <v>2417</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
         <v>2416</v>
@@ -2021,7 +2021,7 @@
         <v>273</v>
       </c>
       <c r="M38" t="n">
-        <v>38275</v>
+        <v>38273</v>
       </c>
     </row>
     <row r="39">
@@ -2031,13 +2031,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2770</v>
+        <v>2769</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>2770</v>
+        <v>2769</v>
       </c>
       <c r="E39" t="n">
         <v>422</v>
@@ -2064,7 +2064,7 @@
         <v>309</v>
       </c>
       <c r="M39" t="n">
-        <v>41045</v>
+        <v>41042</v>
       </c>
     </row>
     <row r="40">
@@ -2077,10 +2077,10 @@
         <v>3071</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>3071</v>
+        <v>3070</v>
       </c>
       <c r="E40" t="n">
         <v>422</v>
@@ -2107,7 +2107,7 @@
         <v>337</v>
       </c>
       <c r="M40" t="n">
-        <v>44116</v>
+        <v>44113</v>
       </c>
     </row>
     <row r="41">
@@ -2117,13 +2117,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="E41" t="n">
         <v>558</v>
@@ -2150,7 +2150,7 @@
         <v>372</v>
       </c>
       <c r="M41" t="n">
-        <v>46856</v>
+        <v>46852</v>
       </c>
     </row>
     <row r="42">
@@ -2160,13 +2160,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>2717</v>
+        <v>2715</v>
       </c>
       <c r="E42" t="n">
         <v>515</v>
@@ -2193,7 +2193,7 @@
         <v>397</v>
       </c>
       <c r="M42" t="n">
-        <v>49573</v>
+        <v>49568</v>
       </c>
     </row>
     <row r="43">
@@ -2206,19 +2206,19 @@
         <v>1527</v>
       </c>
       <c r="C43" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>1518</v>
+        <v>1527</v>
       </c>
       <c r="E43" t="n">
         <v>486</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H43" t="n">
         <v>20</v>
@@ -2236,7 +2236,7 @@
         <v>417</v>
       </c>
       <c r="M43" t="n">
-        <v>51100</v>
+        <v>51095</v>
       </c>
     </row>
     <row r="44">
@@ -2258,10 +2258,10 @@
         <v>319</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H44" t="n">
         <v>29</v>
@@ -2279,7 +2279,7 @@
         <v>446</v>
       </c>
       <c r="M44" t="n">
-        <v>51798</v>
+        <v>51793</v>
       </c>
     </row>
     <row r="45">
@@ -2289,13 +2289,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3458</v>
+        <v>3457</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>3458</v>
+        <v>3457</v>
       </c>
       <c r="E45" t="n">
         <v>292</v>
@@ -2322,7 +2322,7 @@
         <v>480</v>
       </c>
       <c r="M45" t="n">
-        <v>55256</v>
+        <v>55250</v>
       </c>
     </row>
     <row r="46">
@@ -2365,7 +2365,7 @@
         <v>525</v>
       </c>
       <c r="M46" t="n">
-        <v>58849</v>
+        <v>58843</v>
       </c>
     </row>
     <row r="47">
@@ -2408,7 +2408,7 @@
         <v>562</v>
       </c>
       <c r="M47" t="n">
-        <v>62111</v>
+        <v>62105</v>
       </c>
     </row>
     <row r="48">
@@ -2418,10 +2418,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>3908</v>
+        <v>3907</v>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
         <v>3906</v>
@@ -2451,7 +2451,7 @@
         <v>596</v>
       </c>
       <c r="M48" t="n">
-        <v>66019</v>
+        <v>66012</v>
       </c>
     </row>
     <row r="49">
@@ -2464,10 +2464,10 @@
         <v>4022</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4021</v>
+        <v>4022</v>
       </c>
       <c r="E49" t="n">
         <v>505</v>
@@ -2479,10 +2479,10 @@
         <v>505</v>
       </c>
       <c r="H49" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
         <v>35</v>
@@ -2491,10 +2491,10 @@
         <v>10598</v>
       </c>
       <c r="L49" t="n">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="M49" t="n">
-        <v>70041</v>
+        <v>70034</v>
       </c>
     </row>
     <row r="50">
@@ -2513,13 +2513,13 @@
         <v>1704</v>
       </c>
       <c r="E50" t="n">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H50" t="n">
         <v>28</v>
@@ -2531,13 +2531,13 @@
         <v>28</v>
       </c>
       <c r="K50" t="n">
-        <v>11156</v>
+        <v>11155</v>
       </c>
       <c r="L50" t="n">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="M50" t="n">
-        <v>71745</v>
+        <v>71738</v>
       </c>
     </row>
     <row r="51">
@@ -2547,10 +2547,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
         <v>1098</v>
@@ -2565,22 +2565,22 @@
         <v>479</v>
       </c>
       <c r="H51" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
         <v>35</v>
       </c>
       <c r="K51" t="n">
-        <v>11635</v>
+        <v>11634</v>
       </c>
       <c r="L51" t="n">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="M51" t="n">
-        <v>72844</v>
+        <v>72838</v>
       </c>
     </row>
     <row r="52">
@@ -2593,37 +2593,37 @@
         <v>4286</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>4286</v>
+        <v>4285</v>
       </c>
       <c r="E52" t="n">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H52" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
         <v>37</v>
       </c>
       <c r="K52" t="n">
-        <v>12021</v>
+        <v>12019</v>
       </c>
       <c r="L52" t="n">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="M52" t="n">
-        <v>77130</v>
+        <v>77124</v>
       </c>
     </row>
     <row r="53">
@@ -2636,10 +2636,10 @@
         <v>3827</v>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>3825</v>
+        <v>3826</v>
       </c>
       <c r="E53" t="n">
         <v>379</v>
@@ -2651,22 +2651,22 @@
         <v>379</v>
       </c>
       <c r="H53" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="n">
         <v>47</v>
       </c>
       <c r="K53" t="n">
-        <v>12400</v>
+        <v>12398</v>
       </c>
       <c r="L53" t="n">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="M53" t="n">
-        <v>80957</v>
+        <v>80951</v>
       </c>
     </row>
     <row r="54">
@@ -2676,40 +2676,40 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3705</v>
+        <v>3710</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>3705</v>
+        <v>3704</v>
       </c>
       <c r="E54" t="n">
         <v>605</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="H54" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J54" t="n">
         <v>48</v>
       </c>
       <c r="K54" t="n">
-        <v>13005</v>
+        <v>13003</v>
       </c>
       <c r="L54" t="n">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c r="M54" t="n">
-        <v>84662</v>
+        <v>84661</v>
       </c>
     </row>
     <row r="55">
@@ -2719,13 +2719,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4239</v>
+        <v>4266</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D55" t="n">
-        <v>4239</v>
+        <v>4240</v>
       </c>
       <c r="E55" t="n">
         <v>644</v>
@@ -2746,13 +2746,13 @@
         <v>38</v>
       </c>
       <c r="K55" t="n">
-        <v>13649</v>
+        <v>13647</v>
       </c>
       <c r="L55" t="n">
-        <v>864</v>
+        <v>870</v>
       </c>
       <c r="M55" t="n">
-        <v>88901</v>
+        <v>88927</v>
       </c>
     </row>
     <row r="56">
@@ -2762,40 +2762,40 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3492</v>
+        <v>3493</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>3491</v>
+        <v>3493</v>
       </c>
       <c r="E56" t="n">
         <v>700</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H56" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="n">
         <v>35</v>
       </c>
       <c r="K56" t="n">
-        <v>14349</v>
+        <v>14347</v>
       </c>
       <c r="L56" t="n">
-        <v>899</v>
+        <v>906</v>
       </c>
       <c r="M56" t="n">
-        <v>92393</v>
+        <v>92420</v>
       </c>
     </row>
     <row r="57">
@@ -2805,22 +2805,22 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="C57" t="n">
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="E57" t="n">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H57" t="n">
         <v>41</v>
@@ -2832,13 +2832,13 @@
         <v>41</v>
       </c>
       <c r="K57" t="n">
-        <v>14975</v>
+        <v>14971</v>
       </c>
       <c r="L57" t="n">
-        <v>940</v>
+        <v>947</v>
       </c>
       <c r="M57" t="n">
-        <v>94610</v>
+        <v>94636</v>
       </c>
     </row>
     <row r="58">
@@ -2848,13 +2848,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" t="n">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="E58" t="n">
         <v>950</v>
@@ -2875,13 +2875,13 @@
         <v>34</v>
       </c>
       <c r="K58" t="n">
-        <v>15925</v>
+        <v>15921</v>
       </c>
       <c r="L58" t="n">
-        <v>974</v>
+        <v>981</v>
       </c>
       <c r="M58" t="n">
-        <v>96396</v>
+        <v>96421</v>
       </c>
     </row>
     <row r="59">
@@ -2891,13 +2891,13 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>4287</v>
+        <v>4338</v>
       </c>
       <c r="C59" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D59" t="n">
-        <v>4274</v>
+        <v>4288</v>
       </c>
       <c r="E59" t="n">
         <v>621</v>
@@ -2918,13 +2918,13 @@
         <v>41</v>
       </c>
       <c r="K59" t="n">
-        <v>16546</v>
+        <v>16542</v>
       </c>
       <c r="L59" t="n">
-        <v>1015</v>
+        <v>1022</v>
       </c>
       <c r="M59" t="n">
-        <v>100683</v>
+        <v>100759</v>
       </c>
     </row>
     <row r="60">
@@ -2934,13 +2934,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4573</v>
+        <v>4686</v>
       </c>
       <c r="C60" t="n">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="D60" t="n">
-        <v>4570</v>
+        <v>4594</v>
       </c>
       <c r="E60" t="n">
         <v>595</v>
@@ -2961,13 +2961,13 @@
         <v>34</v>
       </c>
       <c r="K60" t="n">
-        <v>17141</v>
+        <v>17137</v>
       </c>
       <c r="L60" t="n">
-        <v>1049</v>
+        <v>1056</v>
       </c>
       <c r="M60" t="n">
-        <v>105256</v>
+        <v>105445</v>
       </c>
     </row>
     <row r="61">
@@ -2977,13 +2977,13 @@
         </is>
       </c>
       <c r="B61" t="n">
+        <v>4717</v>
+      </c>
+      <c r="C61" t="n">
+        <v>76</v>
+      </c>
+      <c r="D61" t="n">
         <v>4641</v>
-      </c>
-      <c r="C61" t="n">
-        <v>4</v>
-      </c>
-      <c r="D61" t="n">
-        <v>4637</v>
       </c>
       <c r="E61" t="n">
         <v>654</v>
@@ -3004,13 +3004,13 @@
         <v>40</v>
       </c>
       <c r="K61" t="n">
-        <v>17795</v>
+        <v>17791</v>
       </c>
       <c r="L61" t="n">
-        <v>1089</v>
+        <v>1096</v>
       </c>
       <c r="M61" t="n">
-        <v>109897</v>
+        <v>110162</v>
       </c>
     </row>
     <row r="62">
@@ -3020,13 +3020,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>4690</v>
+        <v>4737</v>
       </c>
       <c r="C62" t="n">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D62" t="n">
-        <v>4686</v>
+        <v>4689</v>
       </c>
       <c r="E62" t="n">
         <v>795</v>
@@ -3047,13 +3047,13 @@
         <v>45</v>
       </c>
       <c r="K62" t="n">
-        <v>18590</v>
+        <v>18586</v>
       </c>
       <c r="L62" t="n">
-        <v>1134</v>
+        <v>1141</v>
       </c>
       <c r="M62" t="n">
-        <v>114587</v>
+        <v>114899</v>
       </c>
     </row>
     <row r="63">
@@ -3063,22 +3063,22 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>5760</v>
+        <v>5764</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>5760</v>
+        <v>5758</v>
       </c>
       <c r="E63" t="n">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H63" t="n">
         <v>33</v>
@@ -3090,13 +3090,13 @@
         <v>33</v>
       </c>
       <c r="K63" t="n">
-        <v>19244</v>
+        <v>19239</v>
       </c>
       <c r="L63" t="n">
-        <v>1167</v>
+        <v>1174</v>
       </c>
       <c r="M63" t="n">
-        <v>120347</v>
+        <v>120663</v>
       </c>
     </row>
     <row r="64">
@@ -3106,19 +3106,19 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2843</v>
+        <v>2850</v>
       </c>
       <c r="C64" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D64" t="n">
-        <v>2837</v>
+        <v>2842</v>
       </c>
       <c r="E64" t="n">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" t="n">
         <v>634</v>
@@ -3133,13 +3133,13 @@
         <v>40</v>
       </c>
       <c r="K64" t="n">
-        <v>19878</v>
+        <v>19874</v>
       </c>
       <c r="L64" t="n">
-        <v>1207</v>
+        <v>1214</v>
       </c>
       <c r="M64" t="n">
-        <v>123190</v>
+        <v>123513</v>
       </c>
     </row>
     <row r="65">
@@ -3149,13 +3149,13 @@
         </is>
       </c>
       <c r="B65" t="n">
+        <v>1658</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="n">
         <v>1654</v>
-      </c>
-      <c r="C65" t="n">
-        <v>1</v>
-      </c>
-      <c r="D65" t="n">
-        <v>1653</v>
       </c>
       <c r="E65" t="n">
         <v>570</v>
@@ -3176,13 +3176,13 @@
         <v>30</v>
       </c>
       <c r="K65" t="n">
-        <v>20448</v>
+        <v>20444</v>
       </c>
       <c r="L65" t="n">
-        <v>1237</v>
+        <v>1244</v>
       </c>
       <c r="M65" t="n">
-        <v>124844</v>
+        <v>125171</v>
       </c>
     </row>
     <row r="66">
@@ -3192,13 +3192,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>5212</v>
+        <v>5277</v>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="D66" t="n">
-        <v>5211</v>
+        <v>5210</v>
       </c>
       <c r="E66" t="n">
         <v>526</v>
@@ -3219,13 +3219,13 @@
         <v>35</v>
       </c>
       <c r="K66" t="n">
-        <v>20974</v>
+        <v>20970</v>
       </c>
       <c r="L66" t="n">
-        <v>1272</v>
+        <v>1279</v>
       </c>
       <c r="M66" t="n">
-        <v>130056</v>
+        <v>130448</v>
       </c>
     </row>
     <row r="67">
@@ -3235,13 +3235,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5801</v>
+        <v>5866</v>
       </c>
       <c r="C67" t="n">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D67" t="n">
-        <v>5797</v>
+        <v>5799</v>
       </c>
       <c r="E67" t="n">
         <v>838</v>
@@ -3262,13 +3262,13 @@
         <v>36</v>
       </c>
       <c r="K67" t="n">
-        <v>21812</v>
+        <v>21808</v>
       </c>
       <c r="L67" t="n">
-        <v>1308</v>
+        <v>1315</v>
       </c>
       <c r="M67" t="n">
-        <v>135857</v>
+        <v>136314</v>
       </c>
     </row>
     <row r="68">
@@ -3278,40 +3278,40 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>5588</v>
+        <v>5584</v>
       </c>
       <c r="C68" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D68" t="n">
-        <v>5579</v>
+        <v>5580</v>
       </c>
       <c r="E68" t="n">
         <v>624</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H68" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J68" t="n">
         <v>39</v>
       </c>
       <c r="K68" t="n">
-        <v>22436</v>
+        <v>22432</v>
       </c>
       <c r="L68" t="n">
-        <v>1347</v>
+        <v>1355</v>
       </c>
       <c r="M68" t="n">
-        <v>141445</v>
+        <v>141898</v>
       </c>
     </row>
     <row r="69">
@@ -3321,40 +3321,40 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>5800</v>
+        <v>5831</v>
       </c>
       <c r="C69" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D69" t="n">
-        <v>5798</v>
+        <v>5792</v>
       </c>
       <c r="E69" t="n">
         <v>642</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" t="n">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="H69" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="n">
         <v>33</v>
       </c>
       <c r="K69" t="n">
-        <v>23078</v>
+        <v>23074</v>
       </c>
       <c r="L69" t="n">
-        <v>1380</v>
+        <v>1389</v>
       </c>
       <c r="M69" t="n">
-        <v>147245</v>
+        <v>147729</v>
       </c>
     </row>
     <row r="70">
@@ -3364,22 +3364,22 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5836</v>
+        <v>5990</v>
       </c>
       <c r="C70" t="n">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="D70" t="n">
-        <v>5831</v>
+        <v>5835</v>
       </c>
       <c r="E70" t="n">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H70" t="n">
         <v>20</v>
@@ -3391,13 +3391,13 @@
         <v>20</v>
       </c>
       <c r="K70" t="n">
-        <v>23671</v>
+        <v>23666</v>
       </c>
       <c r="L70" t="n">
-        <v>1400</v>
+        <v>1409</v>
       </c>
       <c r="M70" t="n">
-        <v>153081</v>
+        <v>153719</v>
       </c>
     </row>
     <row r="71">
@@ -3407,13 +3407,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3119</v>
+        <v>3131</v>
       </c>
       <c r="C71" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D71" t="n">
-        <v>3099</v>
+        <v>3116</v>
       </c>
       <c r="E71" t="n">
         <v>388</v>
@@ -3425,22 +3425,22 @@
         <v>388</v>
       </c>
       <c r="H71" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J71" t="n">
         <v>25</v>
       </c>
       <c r="K71" t="n">
-        <v>24059</v>
+        <v>24054</v>
       </c>
       <c r="L71" t="n">
-        <v>1425</v>
+        <v>1437</v>
       </c>
       <c r="M71" t="n">
-        <v>156200</v>
+        <v>156850</v>
       </c>
     </row>
     <row r="72">
@@ -3450,13 +3450,13 @@
         </is>
       </c>
       <c r="B72" t="n">
+        <v>1231</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" t="n">
         <v>1230</v>
-      </c>
-      <c r="C72" t="n">
-        <v>3</v>
-      </c>
-      <c r="D72" t="n">
-        <v>1227</v>
       </c>
       <c r="E72" t="n">
         <v>464</v>
@@ -3477,13 +3477,13 @@
         <v>27</v>
       </c>
       <c r="K72" t="n">
-        <v>24523</v>
+        <v>24518</v>
       </c>
       <c r="L72" t="n">
-        <v>1452</v>
+        <v>1464</v>
       </c>
       <c r="M72" t="n">
-        <v>157430</v>
+        <v>158081</v>
       </c>
     </row>
     <row r="73">
@@ -3493,22 +3493,22 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6411</v>
+        <v>6522</v>
       </c>
       <c r="C73" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D73" t="n">
-        <v>6394</v>
+        <v>6403</v>
       </c>
       <c r="E73" t="n">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H73" t="n">
         <v>37</v>
@@ -3520,13 +3520,13 @@
         <v>37</v>
       </c>
       <c r="K73" t="n">
-        <v>25044</v>
+        <v>25038</v>
       </c>
       <c r="L73" t="n">
-        <v>1489</v>
+        <v>1501</v>
       </c>
       <c r="M73" t="n">
-        <v>163841</v>
+        <v>164603</v>
       </c>
     </row>
     <row r="74">
@@ -3536,13 +3536,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>5623</v>
+        <v>5773</v>
       </c>
       <c r="C74" t="n">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="D74" t="n">
-        <v>5568</v>
+        <v>5617</v>
       </c>
       <c r="E74" t="n">
         <v>376</v>
@@ -3563,13 +3563,13 @@
         <v>35</v>
       </c>
       <c r="K74" t="n">
-        <v>25420</v>
+        <v>25414</v>
       </c>
       <c r="L74" t="n">
-        <v>1524</v>
+        <v>1536</v>
       </c>
       <c r="M74" t="n">
-        <v>169464</v>
+        <v>170376</v>
       </c>
     </row>
     <row r="75">
@@ -3579,22 +3579,22 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>5474</v>
+        <v>5827</v>
       </c>
       <c r="C75" t="n">
-        <v>1243</v>
+        <v>373</v>
       </c>
       <c r="D75" t="n">
-        <v>4231</v>
+        <v>5454</v>
       </c>
       <c r="E75" t="n">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H75" t="n">
         <v>21</v>
@@ -3606,13 +3606,13 @@
         <v>21</v>
       </c>
       <c r="K75" t="n">
-        <v>26029</v>
+        <v>26021</v>
       </c>
       <c r="L75" t="n">
-        <v>1545</v>
+        <v>1557</v>
       </c>
       <c r="M75" t="n">
-        <v>174938</v>
+        <v>176203</v>
       </c>
     </row>
     <row r="76">
@@ -3622,40 +3622,40 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>4861</v>
+        <v>5477</v>
       </c>
       <c r="C76" t="n">
-        <v>2090</v>
+        <v>637</v>
       </c>
       <c r="D76" t="n">
-        <v>2771</v>
+        <v>4840</v>
       </c>
       <c r="E76" t="n">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="H76" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76" t="n">
         <v>38</v>
       </c>
       <c r="K76" t="n">
-        <v>26621</v>
+        <v>26610</v>
       </c>
       <c r="L76" t="n">
-        <v>1583</v>
+        <v>1596</v>
       </c>
       <c r="M76" t="n">
-        <v>179799</v>
+        <v>181680</v>
       </c>
     </row>
     <row r="77">
@@ -3665,40 +3665,40 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>3595</v>
+        <v>5762</v>
       </c>
       <c r="C77" t="n">
-        <v>2743</v>
+        <v>2177</v>
       </c>
       <c r="D77" t="n">
-        <v>852</v>
+        <v>3585</v>
       </c>
       <c r="E77" t="n">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" t="n">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="H77" t="n">
+        <v>24</v>
+      </c>
+      <c r="I77" t="n">
+        <v>5</v>
+      </c>
+      <c r="J77" t="n">
         <v>19</v>
       </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="n">
-        <v>18</v>
-      </c>
       <c r="K77" t="n">
-        <v>27267</v>
+        <v>27253</v>
       </c>
       <c r="L77" t="n">
-        <v>1602</v>
+        <v>1620</v>
       </c>
       <c r="M77" t="n">
-        <v>183394</v>
+        <v>187442</v>
       </c>
     </row>
     <row r="78">
@@ -3708,40 +3708,40 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>428</v>
+        <v>1409</v>
       </c>
       <c r="C78" t="n">
-        <v>365</v>
+        <v>983</v>
       </c>
       <c r="D78" t="n">
-        <v>63</v>
+        <v>426</v>
       </c>
       <c r="E78" t="n">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H78" t="n">
+        <v>22</v>
+      </c>
+      <c r="I78" t="n">
+        <v>10</v>
+      </c>
+      <c r="J78" t="n">
         <v>12</v>
       </c>
-      <c r="I78" t="n">
-        <v>6</v>
-      </c>
-      <c r="J78" t="n">
-        <v>6</v>
-      </c>
       <c r="K78" t="n">
-        <v>27766</v>
+        <v>27749</v>
       </c>
       <c r="L78" t="n">
-        <v>1614</v>
+        <v>1642</v>
       </c>
       <c r="M78" t="n">
-        <v>183822</v>
+        <v>188851</v>
       </c>
     </row>
     <row r="79">
@@ -3751,40 +3751,83 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>90</v>
+        <v>327</v>
       </c>
       <c r="C79" t="n">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="E79" t="n">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F79" t="n">
-        <v>489</v>
+        <v>2</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="H79" t="n">
+        <v>21</v>
+      </c>
+      <c r="I79" t="n">
+        <v>14</v>
+      </c>
+      <c r="J79" t="n">
         <v>7</v>
       </c>
-      <c r="I79" t="n">
-        <v>7</v>
-      </c>
-      <c r="J79" t="n">
-        <v>0</v>
-      </c>
       <c r="K79" t="n">
-        <v>28255</v>
+        <v>28234</v>
       </c>
       <c r="L79" t="n">
-        <v>1621</v>
+        <v>1663</v>
       </c>
       <c r="M79" t="n">
-        <v>183912</v>
+        <v>189178</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2020-05-18</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>152</v>
+      </c>
+      <c r="C80" t="n">
+        <v>152</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>471</v>
+      </c>
+      <c r="F80" t="n">
+        <v>471</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>15</v>
+      </c>
+      <c r="I80" t="n">
+        <v>15</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="n">
+        <v>28705</v>
+      </c>
+      <c r="L80" t="n">
+        <v>1678</v>
+      </c>
+      <c r="M80" t="n">
+        <v>189330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pos rate: changed window from 3 to 7; adjusted to docs.
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2461,13 +2461,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4178</v>
+        <v>4176</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>4178</v>
+        <v>4176</v>
       </c>
       <c r="E49" t="n">
         <v>505</v>
@@ -2494,7 +2494,7 @@
         <v>638</v>
       </c>
       <c r="M49" t="n">
-        <v>70552</v>
+        <v>70550</v>
       </c>
     </row>
     <row r="50">
@@ -2537,7 +2537,7 @@
         <v>666</v>
       </c>
       <c r="M50" t="n">
-        <v>72322</v>
+        <v>72320</v>
       </c>
     </row>
     <row r="51">
@@ -2580,7 +2580,7 @@
         <v>703</v>
       </c>
       <c r="M51" t="n">
-        <v>73436</v>
+        <v>73434</v>
       </c>
     </row>
     <row r="52">
@@ -2623,7 +2623,7 @@
         <v>741</v>
       </c>
       <c r="M52" t="n">
-        <v>77818</v>
+        <v>77816</v>
       </c>
     </row>
     <row r="53">
@@ -2666,7 +2666,7 @@
         <v>790</v>
       </c>
       <c r="M53" t="n">
-        <v>81718</v>
+        <v>81716</v>
       </c>
     </row>
     <row r="54">
@@ -2709,7 +2709,7 @@
         <v>840</v>
       </c>
       <c r="M54" t="n">
-        <v>85632</v>
+        <v>85630</v>
       </c>
     </row>
     <row r="55">
@@ -2752,7 +2752,7 @@
         <v>878</v>
       </c>
       <c r="M55" t="n">
-        <v>90079</v>
+        <v>90077</v>
       </c>
     </row>
     <row r="56">
@@ -2795,7 +2795,7 @@
         <v>915</v>
       </c>
       <c r="M56" t="n">
-        <v>93714</v>
+        <v>93712</v>
       </c>
     </row>
     <row r="57">
@@ -2838,7 +2838,7 @@
         <v>956</v>
       </c>
       <c r="M57" t="n">
-        <v>96084</v>
+        <v>96082</v>
       </c>
     </row>
     <row r="58">
@@ -2881,7 +2881,7 @@
         <v>990</v>
       </c>
       <c r="M58" t="n">
-        <v>97935</v>
+        <v>97933</v>
       </c>
     </row>
     <row r="59">
@@ -2924,7 +2924,7 @@
         <v>1032</v>
       </c>
       <c r="M59" t="n">
-        <v>102739</v>
+        <v>102737</v>
       </c>
     </row>
     <row r="60">
@@ -2967,7 +2967,7 @@
         <v>1066</v>
       </c>
       <c r="M60" t="n">
-        <v>107796</v>
+        <v>107794</v>
       </c>
     </row>
     <row r="61">
@@ -3010,7 +3010,7 @@
         <v>1109</v>
       </c>
       <c r="M61" t="n">
-        <v>113192</v>
+        <v>113190</v>
       </c>
     </row>
     <row r="62">
@@ -3053,7 +3053,7 @@
         <v>1154</v>
       </c>
       <c r="M62" t="n">
-        <v>119020</v>
+        <v>119018</v>
       </c>
     </row>
     <row r="63">
@@ -3096,7 +3096,7 @@
         <v>1190</v>
       </c>
       <c r="M63" t="n">
-        <v>125739</v>
+        <v>125737</v>
       </c>
     </row>
     <row r="64">
@@ -3139,7 +3139,7 @@
         <v>1234</v>
       </c>
       <c r="M64" t="n">
-        <v>129070</v>
+        <v>129068</v>
       </c>
     </row>
     <row r="65">
@@ -3182,7 +3182,7 @@
         <v>1266</v>
       </c>
       <c r="M65" t="n">
-        <v>130907</v>
+        <v>130905</v>
       </c>
     </row>
     <row r="66">
@@ -3225,7 +3225,7 @@
         <v>1304</v>
       </c>
       <c r="M66" t="n">
-        <v>136746</v>
+        <v>136744</v>
       </c>
     </row>
     <row r="67">
@@ -3268,7 +3268,7 @@
         <v>1342</v>
       </c>
       <c r="M67" t="n">
-        <v>143327</v>
+        <v>143325</v>
       </c>
     </row>
     <row r="68">
@@ -3311,7 +3311,7 @@
         <v>1385</v>
       </c>
       <c r="M68" t="n">
-        <v>149333</v>
+        <v>149331</v>
       </c>
     </row>
     <row r="69">
@@ -3354,7 +3354,7 @@
         <v>1419</v>
       </c>
       <c r="M69" t="n">
-        <v>155994</v>
+        <v>155992</v>
       </c>
     </row>
     <row r="70">
@@ -3397,7 +3397,7 @@
         <v>1444</v>
       </c>
       <c r="M70" t="n">
-        <v>162713</v>
+        <v>162711</v>
       </c>
     </row>
     <row r="71">
@@ -3440,7 +3440,7 @@
         <v>1476</v>
       </c>
       <c r="M71" t="n">
-        <v>166060</v>
+        <v>166058</v>
       </c>
     </row>
     <row r="72">
@@ -3483,7 +3483,7 @@
         <v>1510</v>
       </c>
       <c r="M72" t="n">
-        <v>167381</v>
+        <v>167379</v>
       </c>
     </row>
     <row r="73">
@@ -3493,13 +3493,13 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>7167</v>
+        <v>7165</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>7167</v>
+        <v>7165</v>
       </c>
       <c r="E73" t="n">
         <v>507</v>
@@ -3526,7 +3526,7 @@
         <v>1551</v>
       </c>
       <c r="M73" t="n">
-        <v>174548</v>
+        <v>174544</v>
       </c>
     </row>
     <row r="74">
@@ -3536,13 +3536,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>7041</v>
+        <v>7040</v>
       </c>
       <c r="C74" t="n">
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>7041</v>
+        <v>7040</v>
       </c>
       <c r="E74" t="n">
         <v>373</v>
@@ -3569,7 +3569,7 @@
         <v>1589</v>
       </c>
       <c r="M74" t="n">
-        <v>181589</v>
+        <v>181584</v>
       </c>
     </row>
     <row r="75">
@@ -3579,13 +3579,13 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>7316</v>
+        <v>7313</v>
       </c>
       <c r="C75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>7314</v>
+        <v>7313</v>
       </c>
       <c r="E75" t="n">
         <v>601</v>
@@ -3612,7 +3612,7 @@
         <v>1616</v>
       </c>
       <c r="M75" t="n">
-        <v>188905</v>
+        <v>188897</v>
       </c>
     </row>
     <row r="76">
@@ -3622,13 +3622,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>8195</v>
+        <v>8194</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>8195</v>
+        <v>8194</v>
       </c>
       <c r="E76" t="n">
         <v>585</v>
@@ -3655,7 +3655,7 @@
         <v>1658</v>
       </c>
       <c r="M76" t="n">
-        <v>197100</v>
+        <v>197091</v>
       </c>
     </row>
     <row r="77">
@@ -3665,13 +3665,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>9792</v>
+        <v>9790</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>9792</v>
+        <v>9790</v>
       </c>
       <c r="E77" t="n">
         <v>633</v>
@@ -3698,7 +3698,7 @@
         <v>1690</v>
       </c>
       <c r="M77" t="n">
-        <v>206892</v>
+        <v>206881</v>
       </c>
     </row>
     <row r="78">
@@ -3741,7 +3741,7 @@
         <v>1718</v>
       </c>
       <c r="M78" t="n">
-        <v>210082</v>
+        <v>210071</v>
       </c>
     </row>
     <row r="79">
@@ -3784,7 +3784,7 @@
         <v>1748</v>
       </c>
       <c r="M79" t="n">
-        <v>212007</v>
+        <v>211996</v>
       </c>
     </row>
     <row r="80">
@@ -3827,7 +3827,7 @@
         <v>1787</v>
       </c>
       <c r="M80" t="n">
-        <v>220386</v>
+        <v>220375</v>
       </c>
     </row>
     <row r="81">
@@ -3870,7 +3870,7 @@
         <v>1816</v>
       </c>
       <c r="M81" t="n">
-        <v>227523</v>
+        <v>227512</v>
       </c>
     </row>
     <row r="82">
@@ -3880,13 +3880,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>6783</v>
+        <v>6782</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>6783</v>
+        <v>6782</v>
       </c>
       <c r="E82" t="n">
         <v>643</v>
@@ -3913,7 +3913,7 @@
         <v>1846</v>
       </c>
       <c r="M82" t="n">
-        <v>234306</v>
+        <v>234294</v>
       </c>
     </row>
     <row r="83">
@@ -3923,13 +3923,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>7709</v>
+        <v>7708</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>7709</v>
+        <v>7708</v>
       </c>
       <c r="E83" t="n">
         <v>459</v>
@@ -3956,7 +3956,7 @@
         <v>1883</v>
       </c>
       <c r="M83" t="n">
-        <v>242015</v>
+        <v>242002</v>
       </c>
     </row>
     <row r="84">
@@ -3999,7 +3999,7 @@
         <v>1900</v>
       </c>
       <c r="M84" t="n">
-        <v>250364</v>
+        <v>250351</v>
       </c>
     </row>
     <row r="85">
@@ -4042,7 +4042,7 @@
         <v>1924</v>
       </c>
       <c r="M85" t="n">
-        <v>253221</v>
+        <v>253208</v>
       </c>
     </row>
     <row r="86">
@@ -4085,7 +4085,7 @@
         <v>1939</v>
       </c>
       <c r="M86" t="n">
-        <v>255093</v>
+        <v>255080</v>
       </c>
     </row>
     <row r="87">
@@ -4128,7 +4128,7 @@
         <v>1960</v>
       </c>
       <c r="M87" t="n">
-        <v>256917</v>
+        <v>256904</v>
       </c>
     </row>
     <row r="88">
@@ -4138,10 +4138,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>7988</v>
+        <v>7989</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" t="n">
         <v>7988</v>
@@ -4171,7 +4171,7 @@
         <v>1979</v>
       </c>
       <c r="M88" t="n">
-        <v>264905</v>
+        <v>264893</v>
       </c>
     </row>
     <row r="89">
@@ -4181,13 +4181,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>6515</v>
+        <v>6517</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>6515</v>
+        <v>6517</v>
       </c>
       <c r="E89" t="n">
         <v>597</v>
@@ -4214,7 +4214,7 @@
         <v>1993</v>
       </c>
       <c r="M89" t="n">
-        <v>271420</v>
+        <v>271410</v>
       </c>
     </row>
     <row r="90">
@@ -4224,13 +4224,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>7174</v>
+        <v>7180</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>7174</v>
+        <v>7180</v>
       </c>
       <c r="E90" t="n">
         <v>478</v>
@@ -4257,7 +4257,7 @@
         <v>2011</v>
       </c>
       <c r="M90" t="n">
-        <v>278594</v>
+        <v>278590</v>
       </c>
     </row>
     <row r="91">
@@ -4267,13 +4267,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>7832</v>
+        <v>7835</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>7832</v>
+        <v>7834</v>
       </c>
       <c r="E91" t="n">
         <v>559</v>
@@ -4300,7 +4300,7 @@
         <v>2032</v>
       </c>
       <c r="M91" t="n">
-        <v>286426</v>
+        <v>286425</v>
       </c>
     </row>
     <row r="92">
@@ -4343,7 +4343,7 @@
         <v>2053</v>
       </c>
       <c r="M92" t="n">
-        <v>289320</v>
+        <v>289319</v>
       </c>
     </row>
     <row r="93">
@@ -4353,13 +4353,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E93" t="n">
         <v>281</v>
@@ -4386,7 +4386,7 @@
         <v>2069</v>
       </c>
       <c r="M93" t="n">
-        <v>291142</v>
+        <v>291140</v>
       </c>
     </row>
     <row r="94">
@@ -4396,13 +4396,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>8141</v>
+        <v>8131</v>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>8140</v>
+        <v>8131</v>
       </c>
       <c r="E94" t="n">
         <v>412</v>
@@ -4429,7 +4429,7 @@
         <v>2089</v>
       </c>
       <c r="M94" t="n">
-        <v>299283</v>
+        <v>299271</v>
       </c>
     </row>
     <row r="95">
@@ -4472,7 +4472,7 @@
         <v>2104</v>
       </c>
       <c r="M95" t="n">
-        <v>304998</v>
+        <v>304986</v>
       </c>
     </row>
     <row r="96">
@@ -4482,13 +4482,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>6757</v>
+        <v>6756</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>6757</v>
+        <v>6755</v>
       </c>
       <c r="E96" t="n">
         <v>426</v>
@@ -4515,7 +4515,7 @@
         <v>2128</v>
       </c>
       <c r="M96" t="n">
-        <v>311755</v>
+        <v>311742</v>
       </c>
     </row>
     <row r="97">
@@ -4528,10 +4528,10 @@
         <v>6972</v>
       </c>
       <c r="C97" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>6969</v>
+        <v>6972</v>
       </c>
       <c r="E97" t="n">
         <v>501</v>
@@ -4558,7 +4558,7 @@
         <v>2150</v>
       </c>
       <c r="M97" t="n">
-        <v>318727</v>
+        <v>318714</v>
       </c>
     </row>
     <row r="98">
@@ -4601,7 +4601,7 @@
         <v>2171</v>
       </c>
       <c r="M98" t="n">
-        <v>326665</v>
+        <v>326652</v>
       </c>
     </row>
     <row r="99">
@@ -4644,7 +4644,7 @@
         <v>2179</v>
       </c>
       <c r="M99" t="n">
-        <v>330380</v>
+        <v>330367</v>
       </c>
     </row>
     <row r="100">
@@ -4687,7 +4687,7 @@
         <v>2194</v>
       </c>
       <c r="M100" t="n">
-        <v>332370</v>
+        <v>332357</v>
       </c>
     </row>
     <row r="101">
@@ -4700,10 +4700,10 @@
         <v>9705</v>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>9704</v>
+        <v>9705</v>
       </c>
       <c r="E101" t="n">
         <v>386</v>
@@ -4730,7 +4730,7 @@
         <v>2210</v>
       </c>
       <c r="M101" t="n">
-        <v>342075</v>
+        <v>342062</v>
       </c>
     </row>
     <row r="102">
@@ -4773,7 +4773,7 @@
         <v>2234</v>
       </c>
       <c r="M102" t="n">
-        <v>348674</v>
+        <v>348661</v>
       </c>
     </row>
     <row r="103">
@@ -4783,10 +4783,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>8026</v>
+        <v>8027</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
         <v>8026</v>
@@ -4816,7 +4816,7 @@
         <v>2251</v>
       </c>
       <c r="M103" t="n">
-        <v>356700</v>
+        <v>356688</v>
       </c>
     </row>
     <row r="104">
@@ -4859,7 +4859,7 @@
         <v>2266</v>
       </c>
       <c r="M104" t="n">
-        <v>366545</v>
+        <v>366533</v>
       </c>
     </row>
     <row r="105">
@@ -4869,13 +4869,13 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>10091</v>
+        <v>10089</v>
       </c>
       <c r="C105" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>10085</v>
+        <v>10089</v>
       </c>
       <c r="E105" t="n">
         <v>405</v>
@@ -4902,7 +4902,7 @@
         <v>2279</v>
       </c>
       <c r="M105" t="n">
-        <v>376636</v>
+        <v>376622</v>
       </c>
     </row>
     <row r="106">
@@ -4912,13 +4912,13 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>4938</v>
+        <v>4937</v>
       </c>
       <c r="C106" t="n">
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>4938</v>
+        <v>4937</v>
       </c>
       <c r="E106" t="n">
         <v>389</v>
@@ -4945,7 +4945,7 @@
         <v>2288</v>
       </c>
       <c r="M106" t="n">
-        <v>381574</v>
+        <v>381559</v>
       </c>
     </row>
     <row r="107">
@@ -4988,7 +4988,7 @@
         <v>2308</v>
       </c>
       <c r="M107" t="n">
-        <v>383466</v>
+        <v>383451</v>
       </c>
     </row>
     <row r="108">
@@ -5031,7 +5031,7 @@
         <v>2321</v>
       </c>
       <c r="M108" t="n">
-        <v>394857</v>
+        <v>394842</v>
       </c>
     </row>
     <row r="109">
@@ -5044,10 +5044,10 @@
         <v>9809</v>
       </c>
       <c r="C109" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>9799</v>
+        <v>9809</v>
       </c>
       <c r="E109" t="n">
         <v>237</v>
@@ -5074,7 +5074,7 @@
         <v>2334</v>
       </c>
       <c r="M109" t="n">
-        <v>404666</v>
+        <v>404651</v>
       </c>
     </row>
     <row r="110">
@@ -5084,13 +5084,13 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>10144</v>
+        <v>10143</v>
       </c>
       <c r="C110" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>10128</v>
+        <v>10143</v>
       </c>
       <c r="E110" t="n">
         <v>550</v>
@@ -5117,7 +5117,7 @@
         <v>2351</v>
       </c>
       <c r="M110" t="n">
-        <v>414810</v>
+        <v>414794</v>
       </c>
     </row>
     <row r="111">
@@ -5127,13 +5127,13 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>10128</v>
+        <v>10127</v>
       </c>
       <c r="C111" t="n">
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>10128</v>
+        <v>10127</v>
       </c>
       <c r="E111" t="n">
         <v>368</v>
@@ -5160,7 +5160,7 @@
         <v>2374</v>
       </c>
       <c r="M111" t="n">
-        <v>424938</v>
+        <v>424921</v>
       </c>
     </row>
     <row r="112">
@@ -5170,13 +5170,13 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>10214</v>
+        <v>10212</v>
       </c>
       <c r="C112" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>10186</v>
+        <v>10212</v>
       </c>
       <c r="E112" t="n">
         <v>381</v>
@@ -5203,7 +5203,7 @@
         <v>2383</v>
       </c>
       <c r="M112" t="n">
-        <v>435152</v>
+        <v>435133</v>
       </c>
     </row>
     <row r="113">
@@ -5216,10 +5216,10 @@
         <v>4389</v>
       </c>
       <c r="C113" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>4387</v>
+        <v>4389</v>
       </c>
       <c r="E113" t="n">
         <v>371</v>
@@ -5231,10 +5231,10 @@
         <v>371</v>
       </c>
       <c r="H113" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
         <v>9</v>
@@ -5243,10 +5243,10 @@
         <v>42293</v>
       </c>
       <c r="L113" t="n">
-        <v>2392</v>
+        <v>2393</v>
       </c>
       <c r="M113" t="n">
-        <v>439541</v>
+        <v>439522</v>
       </c>
     </row>
     <row r="114">
@@ -5274,10 +5274,10 @@
         <v>248</v>
       </c>
       <c r="H114" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" t="n">
         <v>10</v>
@@ -5286,10 +5286,10 @@
         <v>42541</v>
       </c>
       <c r="L114" t="n">
-        <v>2402</v>
+        <v>2404</v>
       </c>
       <c r="M114" t="n">
-        <v>441371</v>
+        <v>441352</v>
       </c>
     </row>
     <row r="115">
@@ -5299,13 +5299,13 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>10623</v>
+        <v>10626</v>
       </c>
       <c r="C115" t="n">
         <v>4</v>
       </c>
       <c r="D115" t="n">
-        <v>10619</v>
+        <v>10622</v>
       </c>
       <c r="E115" t="n">
         <v>304</v>
@@ -5329,10 +5329,10 @@
         <v>42845</v>
       </c>
       <c r="L115" t="n">
-        <v>2416</v>
+        <v>2418</v>
       </c>
       <c r="M115" t="n">
-        <v>451994</v>
+        <v>451978</v>
       </c>
     </row>
     <row r="116">
@@ -5342,10 +5342,10 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>9639</v>
+        <v>9640</v>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116" t="n">
         <v>9639</v>
@@ -5372,10 +5372,10 @@
         <v>43118</v>
       </c>
       <c r="L116" t="n">
-        <v>2421</v>
+        <v>2423</v>
       </c>
       <c r="M116" t="n">
-        <v>461633</v>
+        <v>461618</v>
       </c>
     </row>
     <row r="117">
@@ -5385,13 +5385,13 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>9062</v>
+        <v>9071</v>
       </c>
       <c r="C117" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>9054</v>
+        <v>9065</v>
       </c>
       <c r="E117" t="n">
         <v>511</v>
@@ -5403,10 +5403,10 @@
         <v>511</v>
       </c>
       <c r="H117" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J117" t="n">
         <v>8</v>
@@ -5415,10 +5415,10 @@
         <v>43629</v>
       </c>
       <c r="L117" t="n">
-        <v>2429</v>
+        <v>2432</v>
       </c>
       <c r="M117" t="n">
-        <v>470695</v>
+        <v>470689</v>
       </c>
     </row>
     <row r="118">
@@ -5428,22 +5428,22 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>9168</v>
+        <v>9266</v>
       </c>
       <c r="C118" t="n">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="D118" t="n">
-        <v>9039</v>
+        <v>9172</v>
       </c>
       <c r="E118" t="n">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F118" t="n">
         <v>0</v>
       </c>
       <c r="G118" t="n">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H118" t="n">
         <v>12</v>
@@ -5455,13 +5455,13 @@
         <v>12</v>
       </c>
       <c r="K118" t="n">
-        <v>44075</v>
+        <v>44074</v>
       </c>
       <c r="L118" t="n">
-        <v>2441</v>
+        <v>2444</v>
       </c>
       <c r="M118" t="n">
-        <v>479863</v>
+        <v>479955</v>
       </c>
     </row>
     <row r="119">
@@ -5471,13 +5471,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>9070</v>
+        <v>9315</v>
       </c>
       <c r="C119" t="n">
-        <v>44</v>
+        <v>240</v>
       </c>
       <c r="D119" t="n">
-        <v>9026</v>
+        <v>9075</v>
       </c>
       <c r="E119" t="n">
         <v>478</v>
@@ -5492,19 +5492,19 @@
         <v>11</v>
       </c>
       <c r="I119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K119" t="n">
-        <v>44553</v>
+        <v>44552</v>
       </c>
       <c r="L119" t="n">
-        <v>2452</v>
+        <v>2455</v>
       </c>
       <c r="M119" t="n">
-        <v>488933</v>
+        <v>489270</v>
       </c>
     </row>
     <row r="120">
@@ -5514,13 +5514,13 @@
         </is>
       </c>
       <c r="B120" t="n">
+        <v>3454</v>
+      </c>
+      <c r="C120" t="n">
+        <v>12</v>
+      </c>
+      <c r="D120" t="n">
         <v>3442</v>
-      </c>
-      <c r="C120" t="n">
-        <v>7</v>
-      </c>
-      <c r="D120" t="n">
-        <v>3435</v>
       </c>
       <c r="E120" t="n">
         <v>348</v>
@@ -5532,22 +5532,22 @@
         <v>348</v>
       </c>
       <c r="H120" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I120" t="n">
         <v>1</v>
       </c>
       <c r="J120" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K120" t="n">
-        <v>44901</v>
+        <v>44900</v>
       </c>
       <c r="L120" t="n">
-        <v>2461</v>
+        <v>2465</v>
       </c>
       <c r="M120" t="n">
-        <v>492375</v>
+        <v>492724</v>
       </c>
     </row>
     <row r="121">
@@ -5557,13 +5557,13 @@
         </is>
       </c>
       <c r="B121" t="n">
+        <v>2356</v>
+      </c>
+      <c r="C121" t="n">
+        <v>5</v>
+      </c>
+      <c r="D121" t="n">
         <v>2351</v>
-      </c>
-      <c r="C121" t="n">
-        <v>51</v>
-      </c>
-      <c r="D121" t="n">
-        <v>2300</v>
       </c>
       <c r="E121" t="n">
         <v>300</v>
@@ -5575,22 +5575,22 @@
         <v>300</v>
       </c>
       <c r="H121" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121" t="n">
         <v>8</v>
       </c>
       <c r="K121" t="n">
-        <v>45201</v>
+        <v>45200</v>
       </c>
       <c r="L121" t="n">
-        <v>2469</v>
+        <v>2474</v>
       </c>
       <c r="M121" t="n">
-        <v>494726</v>
+        <v>495080</v>
       </c>
     </row>
     <row r="122">
@@ -5600,22 +5600,22 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>8753</v>
+        <v>8977</v>
       </c>
       <c r="C122" t="n">
-        <v>22</v>
+        <v>221</v>
       </c>
       <c r="D122" t="n">
-        <v>8731</v>
+        <v>8756</v>
       </c>
       <c r="E122" t="n">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H122" t="n">
         <v>7</v>
@@ -5627,13 +5627,13 @@
         <v>7</v>
       </c>
       <c r="K122" t="n">
-        <v>45575</v>
+        <v>45571</v>
       </c>
       <c r="L122" t="n">
-        <v>2476</v>
+        <v>2481</v>
       </c>
       <c r="M122" t="n">
-        <v>503479</v>
+        <v>504057</v>
       </c>
     </row>
     <row r="123">
@@ -5643,13 +5643,13 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>7570</v>
+        <v>8052</v>
       </c>
       <c r="C123" t="n">
-        <v>218</v>
+        <v>478</v>
       </c>
       <c r="D123" t="n">
-        <v>7352</v>
+        <v>7574</v>
       </c>
       <c r="E123" t="n">
         <v>357</v>
@@ -5661,22 +5661,22 @@
         <v>357</v>
       </c>
       <c r="H123" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J123" t="n">
         <v>6</v>
       </c>
       <c r="K123" t="n">
-        <v>45932</v>
+        <v>45928</v>
       </c>
       <c r="L123" t="n">
-        <v>2482</v>
+        <v>2488</v>
       </c>
       <c r="M123" t="n">
-        <v>511049</v>
+        <v>512109</v>
       </c>
     </row>
     <row r="124">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>6341</v>
+        <v>6711</v>
       </c>
       <c r="C124" t="n">
-        <v>232</v>
+        <v>377</v>
       </c>
       <c r="D124" t="n">
-        <v>6109</v>
+        <v>6334</v>
       </c>
       <c r="E124" t="n">
         <v>442</v>
@@ -5713,13 +5713,13 @@
         <v>10</v>
       </c>
       <c r="K124" t="n">
-        <v>46374</v>
+        <v>46370</v>
       </c>
       <c r="L124" t="n">
-        <v>2492</v>
+        <v>2498</v>
       </c>
       <c r="M124" t="n">
-        <v>517390</v>
+        <v>518820</v>
       </c>
     </row>
     <row r="125">
@@ -5729,13 +5729,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>7006</v>
+        <v>7819</v>
       </c>
       <c r="C125" t="n">
-        <v>715</v>
+        <v>826</v>
       </c>
       <c r="D125" t="n">
-        <v>6291</v>
+        <v>6993</v>
       </c>
       <c r="E125" t="n">
         <v>531</v>
@@ -5747,22 +5747,22 @@
         <v>531</v>
       </c>
       <c r="H125" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I125" t="n">
         <v>1</v>
       </c>
       <c r="J125" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K125" t="n">
-        <v>46905</v>
+        <v>46901</v>
       </c>
       <c r="L125" t="n">
-        <v>2498</v>
+        <v>2505</v>
       </c>
       <c r="M125" t="n">
-        <v>524396</v>
+        <v>526639</v>
       </c>
     </row>
     <row r="126">
@@ -5772,40 +5772,40 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>3384</v>
+        <v>3921</v>
       </c>
       <c r="C126" t="n">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="D126" t="n">
-        <v>2816</v>
+        <v>3378</v>
       </c>
       <c r="E126" t="n">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F126" t="n">
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H126" t="n">
         <v>5</v>
       </c>
       <c r="I126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K126" t="n">
-        <v>47404</v>
+        <v>47399</v>
       </c>
       <c r="L126" t="n">
-        <v>2503</v>
+        <v>2510</v>
       </c>
       <c r="M126" t="n">
-        <v>527780</v>
+        <v>530560</v>
       </c>
     </row>
     <row r="127">
@@ -5815,13 +5815,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>1398</v>
+        <v>1600</v>
       </c>
       <c r="C127" t="n">
-        <v>754</v>
+        <v>205</v>
       </c>
       <c r="D127" t="n">
-        <v>644</v>
+        <v>1395</v>
       </c>
       <c r="E127" t="n">
         <v>590</v>
@@ -5836,19 +5836,19 @@
         <v>6</v>
       </c>
       <c r="I127" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J127" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K127" t="n">
-        <v>47994</v>
+        <v>47989</v>
       </c>
       <c r="L127" t="n">
-        <v>2509</v>
+        <v>2516</v>
       </c>
       <c r="M127" t="n">
-        <v>529178</v>
+        <v>532160</v>
       </c>
     </row>
     <row r="128">
@@ -5858,40 +5858,40 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>663</v>
+        <v>1457</v>
       </c>
       <c r="C128" t="n">
-        <v>512</v>
+        <v>796</v>
       </c>
       <c r="D128" t="n">
-        <v>151</v>
+        <v>661</v>
       </c>
       <c r="E128" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F128" t="n">
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H128" t="n">
+        <v>12</v>
+      </c>
+      <c r="I128" t="n">
+        <v>2</v>
+      </c>
+      <c r="J128" t="n">
         <v>10</v>
       </c>
-      <c r="I128" t="n">
-        <v>7</v>
-      </c>
-      <c r="J128" t="n">
-        <v>3</v>
-      </c>
       <c r="K128" t="n">
-        <v>48312</v>
+        <v>48306</v>
       </c>
       <c r="L128" t="n">
-        <v>2519</v>
+        <v>2528</v>
       </c>
       <c r="M128" t="n">
-        <v>529841</v>
+        <v>533617</v>
       </c>
     </row>
     <row r="129">
@@ -5901,40 +5901,83 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>234</v>
+        <v>2080</v>
       </c>
       <c r="C129" t="n">
-        <v>234</v>
+        <v>1850</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="E129" t="n">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F129" t="n">
-        <v>314</v>
+        <v>0</v>
       </c>
       <c r="G129" t="n">
-        <v>0</v>
+        <v>302</v>
       </c>
       <c r="H129" t="n">
+        <v>9</v>
+      </c>
+      <c r="I129" t="n">
+        <v>4</v>
+      </c>
+      <c r="J129" t="n">
         <v>5</v>
       </c>
-      <c r="I129" t="n">
-        <v>5</v>
-      </c>
-      <c r="J129" t="n">
-        <v>0</v>
-      </c>
       <c r="K129" t="n">
-        <v>48626</v>
+        <v>48608</v>
       </c>
       <c r="L129" t="n">
-        <v>2524</v>
+        <v>2537</v>
       </c>
       <c r="M129" t="n">
-        <v>530075</v>
+        <v>535697</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2020-07-07</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>160</v>
+      </c>
+      <c r="C130" t="n">
+        <v>160</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="n">
+        <v>455</v>
+      </c>
+      <c r="F130" t="n">
+        <v>455</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" t="n">
+        <v>2</v>
+      </c>
+      <c r="I130" t="n">
+        <v>2</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="n">
+        <v>49063</v>
+      </c>
+      <c r="L130" t="n">
+        <v>2539</v>
+      </c>
+      <c r="M130" t="n">
+        <v>535857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
indy hub changed col names again
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M135"/>
+  <dimension ref="A1:M136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,67 +369,67 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>COVID_TEST</t>
+          <t>m1e_covid_tests</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_DELTA_TESTS</t>
+          <t>m1e_daily_delta_tests</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_BASE_TESTS</t>
+          <t>m1e_daily_base_tests</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>COVID_DEATHS</t>
+          <t>m1e_covid_deaths</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_DELTA_DEATHS</t>
+          <t>m1e_daily_delta_deaths</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_BASE_DEATHS</t>
+          <t>m1e_daily_base_deaths</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>COVID_COUNT</t>
+          <t>m1e_covid_cases</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_DELTA_CASES</t>
+          <t>m1e_daily_delta_cases</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>DAILY_BASE_CASES</t>
+          <t>m1e_daily_base_cases</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>COVID_COUNT_CUMSUM</t>
+          <t>m1e_cumsum_covid_cases</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>COVID_DEATHS_CUMSUM</t>
+          <t>m1e_cumsum_covid_deaths</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>COVID_TEST_CUMSUM</t>
+          <t>m1e_cumsum_covid_tests</t>
         </is>
       </c>
     </row>
@@ -4396,13 +4396,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>8130</v>
+        <v>8129</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>8130</v>
+        <v>8129</v>
       </c>
       <c r="E94" t="n">
         <v>20</v>
@@ -4429,7 +4429,7 @@
         <v>2089</v>
       </c>
       <c r="M94" t="n">
-        <v>299319</v>
+        <v>299318</v>
       </c>
     </row>
     <row r="95">
@@ -4472,7 +4472,7 @@
         <v>2104</v>
       </c>
       <c r="M95" t="n">
-        <v>305034</v>
+        <v>305033</v>
       </c>
     </row>
     <row r="96">
@@ -4515,7 +4515,7 @@
         <v>2128</v>
       </c>
       <c r="M96" t="n">
-        <v>311790</v>
+        <v>311789</v>
       </c>
     </row>
     <row r="97">
@@ -4558,7 +4558,7 @@
         <v>2150</v>
       </c>
       <c r="M97" t="n">
-        <v>318763</v>
+        <v>318762</v>
       </c>
     </row>
     <row r="98">
@@ -4601,7 +4601,7 @@
         <v>2171</v>
       </c>
       <c r="M98" t="n">
-        <v>326701</v>
+        <v>326700</v>
       </c>
     </row>
     <row r="99">
@@ -4644,7 +4644,7 @@
         <v>2179</v>
       </c>
       <c r="M99" t="n">
-        <v>330416</v>
+        <v>330415</v>
       </c>
     </row>
     <row r="100">
@@ -4687,7 +4687,7 @@
         <v>2194</v>
       </c>
       <c r="M100" t="n">
-        <v>332406</v>
+        <v>332405</v>
       </c>
     </row>
     <row r="101">
@@ -4730,7 +4730,7 @@
         <v>2210</v>
       </c>
       <c r="M101" t="n">
-        <v>342109</v>
+        <v>342108</v>
       </c>
     </row>
     <row r="102">
@@ -4740,10 +4740,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>6598</v>
+        <v>6599</v>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102" t="n">
         <v>6598</v>
@@ -5041,10 +5041,10 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>9810</v>
+        <v>9812</v>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D109" t="n">
         <v>9810</v>
@@ -5074,7 +5074,7 @@
         <v>2334</v>
       </c>
       <c r="M109" t="n">
-        <v>404701</v>
+        <v>404703</v>
       </c>
     </row>
     <row r="110">
@@ -5084,10 +5084,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>10144</v>
+        <v>10147</v>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D110" t="n">
         <v>10144</v>
@@ -5117,7 +5117,7 @@
         <v>2351</v>
       </c>
       <c r="M110" t="n">
-        <v>414845</v>
+        <v>414850</v>
       </c>
     </row>
     <row r="111">
@@ -5160,7 +5160,7 @@
         <v>2374</v>
       </c>
       <c r="M111" t="n">
-        <v>424972</v>
+        <v>424977</v>
       </c>
     </row>
     <row r="112">
@@ -5170,10 +5170,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>10212</v>
+        <v>10219</v>
       </c>
       <c r="C112" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D112" t="n">
         <v>10212</v>
@@ -5203,7 +5203,7 @@
         <v>2384</v>
       </c>
       <c r="M112" t="n">
-        <v>435184</v>
+        <v>435196</v>
       </c>
     </row>
     <row r="113">
@@ -5213,10 +5213,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>4390</v>
+        <v>4391</v>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113" t="n">
         <v>4390</v>
@@ -5246,7 +5246,7 @@
         <v>2394</v>
       </c>
       <c r="M113" t="n">
-        <v>439574</v>
+        <v>439587</v>
       </c>
     </row>
     <row r="114">
@@ -5256,10 +5256,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1831</v>
+        <v>1834</v>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D114" t="n">
         <v>1831</v>
@@ -5289,7 +5289,7 @@
         <v>2405</v>
       </c>
       <c r="M114" t="n">
-        <v>441405</v>
+        <v>441421</v>
       </c>
     </row>
     <row r="115">
@@ -5299,13 +5299,13 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>10627</v>
+        <v>10631</v>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D115" t="n">
-        <v>10627</v>
+        <v>10628</v>
       </c>
       <c r="E115" t="n">
         <v>14</v>
@@ -5332,7 +5332,7 @@
         <v>2419</v>
       </c>
       <c r="M115" t="n">
-        <v>452032</v>
+        <v>452052</v>
       </c>
     </row>
     <row r="116">
@@ -5342,10 +5342,10 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>9639</v>
+        <v>9642</v>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D116" t="n">
         <v>9639</v>
@@ -5375,7 +5375,7 @@
         <v>2424</v>
       </c>
       <c r="M116" t="n">
-        <v>461671</v>
+        <v>461694</v>
       </c>
     </row>
     <row r="117">
@@ -5385,10 +5385,10 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>9080</v>
+        <v>9082</v>
       </c>
       <c r="C117" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D117" t="n">
         <v>9080</v>
@@ -5418,7 +5418,7 @@
         <v>2433</v>
       </c>
       <c r="M117" t="n">
-        <v>470751</v>
+        <v>470776</v>
       </c>
     </row>
     <row r="118">
@@ -5461,7 +5461,7 @@
         <v>2445</v>
       </c>
       <c r="M118" t="n">
-        <v>480029</v>
+        <v>480054</v>
       </c>
     </row>
     <row r="119">
@@ -5471,13 +5471,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>9706</v>
+        <v>9712</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D119" t="n">
-        <v>9706</v>
+        <v>9708</v>
       </c>
       <c r="E119" t="n">
         <v>11</v>
@@ -5504,7 +5504,7 @@
         <v>2456</v>
       </c>
       <c r="M119" t="n">
-        <v>489735</v>
+        <v>489766</v>
       </c>
     </row>
     <row r="120">
@@ -5514,13 +5514,13 @@
         </is>
       </c>
       <c r="B120" t="n">
+        <v>3975</v>
+      </c>
+      <c r="C120" t="n">
+        <v>13</v>
+      </c>
+      <c r="D120" t="n">
         <v>3962</v>
-      </c>
-      <c r="C120" t="n">
-        <v>1</v>
-      </c>
-      <c r="D120" t="n">
-        <v>3961</v>
       </c>
       <c r="E120" t="n">
         <v>10</v>
@@ -5547,7 +5547,7 @@
         <v>2466</v>
       </c>
       <c r="M120" t="n">
-        <v>493697</v>
+        <v>493741</v>
       </c>
     </row>
     <row r="121">
@@ -5560,10 +5560,10 @@
         <v>2534</v>
       </c>
       <c r="C121" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D121" t="n">
-        <v>2513</v>
+        <v>2531</v>
       </c>
       <c r="E121" t="n">
         <v>9</v>
@@ -5590,7 +5590,7 @@
         <v>2475</v>
       </c>
       <c r="M121" t="n">
-        <v>496231</v>
+        <v>496275</v>
       </c>
     </row>
     <row r="122">
@@ -5600,13 +5600,13 @@
         </is>
       </c>
       <c r="B122" t="n">
+        <v>9341</v>
+      </c>
+      <c r="C122" t="n">
+        <v>55</v>
+      </c>
+      <c r="D122" t="n">
         <v>9286</v>
-      </c>
-      <c r="C122" t="n">
-        <v>115</v>
-      </c>
-      <c r="D122" t="n">
-        <v>9171</v>
       </c>
       <c r="E122" t="n">
         <v>7</v>
@@ -5633,7 +5633,7 @@
         <v>2482</v>
       </c>
       <c r="M122" t="n">
-        <v>505517</v>
+        <v>505616</v>
       </c>
     </row>
     <row r="123">
@@ -5643,13 +5643,13 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>8486</v>
+        <v>8524</v>
       </c>
       <c r="C123" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D123" t="n">
-        <v>8458</v>
+        <v>8487</v>
       </c>
       <c r="E123" t="n">
         <v>7</v>
@@ -5676,7 +5676,7 @@
         <v>2489</v>
       </c>
       <c r="M123" t="n">
-        <v>514003</v>
+        <v>514140</v>
       </c>
     </row>
     <row r="124">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>6910</v>
+        <v>6983</v>
       </c>
       <c r="C124" t="n">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="D124" t="n">
-        <v>6886</v>
+        <v>6913</v>
       </c>
       <c r="E124" t="n">
         <v>10</v>
@@ -5704,22 +5704,22 @@
         <v>10</v>
       </c>
       <c r="H124" t="n">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I124" t="n">
         <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K124" t="n">
-        <v>46365</v>
+        <v>46364</v>
       </c>
       <c r="L124" t="n">
         <v>2499</v>
       </c>
       <c r="M124" t="n">
-        <v>520913</v>
+        <v>521123</v>
       </c>
     </row>
     <row r="125">
@@ -5729,13 +5729,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>8076</v>
+        <v>8097</v>
       </c>
       <c r="C125" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D125" t="n">
-        <v>8054</v>
+        <v>8081</v>
       </c>
       <c r="E125" t="n">
         <v>7</v>
@@ -5756,13 +5756,13 @@
         <v>528</v>
       </c>
       <c r="K125" t="n">
-        <v>46893</v>
+        <v>46892</v>
       </c>
       <c r="L125" t="n">
         <v>2506</v>
       </c>
       <c r="M125" t="n">
-        <v>528989</v>
+        <v>529220</v>
       </c>
     </row>
     <row r="126">
@@ -5772,19 +5772,19 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>4534</v>
+        <v>4639</v>
       </c>
       <c r="C126" t="n">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="D126" t="n">
-        <v>4505</v>
+        <v>4542</v>
       </c>
       <c r="E126" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" t="n">
         <v>6</v>
@@ -5799,13 +5799,13 @@
         <v>497</v>
       </c>
       <c r="K126" t="n">
-        <v>47390</v>
+        <v>47389</v>
       </c>
       <c r="L126" t="n">
-        <v>2512</v>
+        <v>2513</v>
       </c>
       <c r="M126" t="n">
-        <v>533523</v>
+        <v>533859</v>
       </c>
     </row>
     <row r="127">
@@ -5815,13 +5815,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>2022</v>
+        <v>2031</v>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D127" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E127" t="n">
         <v>6</v>
@@ -5842,13 +5842,13 @@
         <v>589</v>
       </c>
       <c r="K127" t="n">
-        <v>47979</v>
+        <v>47978</v>
       </c>
       <c r="L127" t="n">
-        <v>2518</v>
+        <v>2519</v>
       </c>
       <c r="M127" t="n">
-        <v>535545</v>
+        <v>535890</v>
       </c>
     </row>
     <row r="128">
@@ -5858,13 +5858,13 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>2184</v>
+        <v>2191</v>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D128" t="n">
-        <v>2183</v>
+        <v>2186</v>
       </c>
       <c r="E128" t="n">
         <v>12</v>
@@ -5885,13 +5885,13 @@
         <v>315</v>
       </c>
       <c r="K128" t="n">
-        <v>48294</v>
+        <v>48293</v>
       </c>
       <c r="L128" t="n">
-        <v>2530</v>
+        <v>2531</v>
       </c>
       <c r="M128" t="n">
-        <v>537729</v>
+        <v>538081</v>
       </c>
     </row>
     <row r="129">
@@ -5901,13 +5901,13 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>10047</v>
+        <v>10118</v>
       </c>
       <c r="C129" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="D129" t="n">
-        <v>10025</v>
+        <v>10058</v>
       </c>
       <c r="E129" t="n">
         <v>11</v>
@@ -5928,13 +5928,13 @@
         <v>301</v>
       </c>
       <c r="K129" t="n">
-        <v>48595</v>
+        <v>48594</v>
       </c>
       <c r="L129" t="n">
-        <v>2541</v>
+        <v>2542</v>
       </c>
       <c r="M129" t="n">
-        <v>547776</v>
+        <v>548199</v>
       </c>
     </row>
     <row r="130">
@@ -5944,19 +5944,19 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>8113</v>
+        <v>8441</v>
       </c>
       <c r="C130" t="n">
-        <v>134</v>
+        <v>327</v>
       </c>
       <c r="D130" t="n">
-        <v>7979</v>
+        <v>8114</v>
       </c>
       <c r="E130" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130" t="n">
         <v>5</v>
@@ -5971,13 +5971,13 @@
         <v>445</v>
       </c>
       <c r="K130" t="n">
-        <v>49040</v>
+        <v>49039</v>
       </c>
       <c r="L130" t="n">
-        <v>2546</v>
+        <v>2548</v>
       </c>
       <c r="M130" t="n">
-        <v>555889</v>
+        <v>556640</v>
       </c>
     </row>
     <row r="131">
@@ -5987,13 +5987,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>6783</v>
+        <v>7496</v>
       </c>
       <c r="C131" t="n">
-        <v>1382</v>
+        <v>666</v>
       </c>
       <c r="D131" t="n">
-        <v>5401</v>
+        <v>6830</v>
       </c>
       <c r="E131" t="n">
         <v>7</v>
@@ -6014,13 +6014,13 @@
         <v>499</v>
       </c>
       <c r="K131" t="n">
-        <v>49539</v>
+        <v>49538</v>
       </c>
       <c r="L131" t="n">
-        <v>2553</v>
+        <v>2555</v>
       </c>
       <c r="M131" t="n">
-        <v>562672</v>
+        <v>564136</v>
       </c>
     </row>
     <row r="132">
@@ -6030,13 +6030,13 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>4568</v>
+        <v>6286</v>
       </c>
       <c r="C132" t="n">
-        <v>2445</v>
+        <v>1772</v>
       </c>
       <c r="D132" t="n">
-        <v>2123</v>
+        <v>4514</v>
       </c>
       <c r="E132" t="n">
         <v>8</v>
@@ -6048,22 +6048,22 @@
         <v>8</v>
       </c>
       <c r="H132" t="n">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I132" t="n">
         <v>0</v>
       </c>
       <c r="J132" t="n">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="K132" t="n">
-        <v>50266</v>
+        <v>50264</v>
       </c>
       <c r="L132" t="n">
-        <v>2561</v>
+        <v>2563</v>
       </c>
       <c r="M132" t="n">
-        <v>567240</v>
+        <v>570422</v>
       </c>
     </row>
     <row r="133">
@@ -6073,40 +6073,40 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>2200</v>
+        <v>5323</v>
       </c>
       <c r="C133" t="n">
-        <v>869</v>
+        <v>3138</v>
       </c>
       <c r="D133" t="n">
-        <v>1331</v>
+        <v>2185</v>
       </c>
       <c r="E133" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G133" t="n">
         <v>3</v>
       </c>
       <c r="H133" t="n">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="I133" t="n">
         <v>0</v>
       </c>
       <c r="J133" t="n">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="K133" t="n">
-        <v>51034</v>
+        <v>51027</v>
       </c>
       <c r="L133" t="n">
-        <v>2564</v>
+        <v>2568</v>
       </c>
       <c r="M133" t="n">
-        <v>569440</v>
+        <v>575745</v>
       </c>
     </row>
     <row r="134">
@@ -6116,40 +6116,40 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>848</v>
+        <v>1540</v>
       </c>
       <c r="C134" t="n">
-        <v>630</v>
+        <v>715</v>
       </c>
       <c r="D134" t="n">
-        <v>218</v>
+        <v>825</v>
       </c>
       <c r="E134" t="n">
+        <v>6</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1</v>
+      </c>
+      <c r="G134" t="n">
         <v>5</v>
       </c>
-      <c r="F134" t="n">
-        <v>2</v>
-      </c>
-      <c r="G134" t="n">
-        <v>3</v>
-      </c>
       <c r="H134" t="n">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I134" t="n">
         <v>0</v>
       </c>
       <c r="J134" t="n">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K134" t="n">
-        <v>51585</v>
+        <v>51577</v>
       </c>
       <c r="L134" t="n">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="M134" t="n">
-        <v>570288</v>
+        <v>577285</v>
       </c>
     </row>
     <row r="135">
@@ -6159,40 +6159,83 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>121</v>
+        <v>945</v>
       </c>
       <c r="C135" t="n">
-        <v>121</v>
+        <v>829</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F135" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G135" t="n">
         <v>0</v>
       </c>
       <c r="H135" t="n">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="I135" t="n">
-        <v>452</v>
+        <v>1</v>
       </c>
       <c r="J135" t="n">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="K135" t="n">
-        <v>52037</v>
+        <v>52024</v>
       </c>
       <c r="L135" t="n">
-        <v>2569</v>
+        <v>2580</v>
       </c>
       <c r="M135" t="n">
-        <v>570409</v>
+        <v>578230</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2020-07-13</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>179</v>
+      </c>
+      <c r="C136" t="n">
+        <v>179</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" t="n">
+        <v>2</v>
+      </c>
+      <c r="F136" t="n">
+        <v>2</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" t="n">
+        <v>661</v>
+      </c>
+      <c r="I136" t="n">
+        <v>661</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="n">
+        <v>52685</v>
+      </c>
+      <c r="L136" t="n">
+        <v>2582</v>
+      </c>
+      <c r="M136" t="n">
+        <v>578409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manual update of charts; gh actions failing at the moment
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,11 @@
           <t>COVID_TEST_CUMSUM</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>POSITIVITY_RATE</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -475,6 +480,9 @@
       <c r="M2" t="n">
         <v>1</v>
       </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,6 +526,9 @@
       <c r="M3" t="n">
         <v>2</v>
       </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -561,6 +572,9 @@
       <c r="M4" t="n">
         <v>3</v>
       </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -604,6 +618,9 @@
       <c r="M5" t="n">
         <v>5</v>
       </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -647,6 +664,9 @@
       <c r="M6" t="n">
         <v>9</v>
       </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -690,6 +710,9 @@
       <c r="M7" t="n">
         <v>13</v>
       </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -733,6 +756,9 @@
       <c r="M8" t="n">
         <v>15</v>
       </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -776,6 +802,9 @@
       <c r="M9" t="n">
         <v>21</v>
       </c>
+      <c r="N9" t="n">
+        <v>16.66666666666666</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -819,6 +848,9 @@
       <c r="M10" t="n">
         <v>26</v>
       </c>
+      <c r="N10" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -862,6 +894,9 @@
       <c r="M11" t="n">
         <v>35</v>
       </c>
+      <c r="N11" t="n">
+        <v>22.22222222222222</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -905,6 +940,9 @@
       <c r="M12" t="n">
         <v>60</v>
       </c>
+      <c r="N12" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -948,6 +986,9 @@
       <c r="M13" t="n">
         <v>112</v>
       </c>
+      <c r="N13" t="n">
+        <v>1.923076923076923</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -991,6 +1032,9 @@
       <c r="M14" t="n">
         <v>172</v>
       </c>
+      <c r="N14" t="n">
+        <v>6.666666666666667</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1034,6 +1078,9 @@
       <c r="M15" t="n">
         <v>370</v>
       </c>
+      <c r="N15" t="n">
+        <v>8.585858585858585</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1077,6 +1124,9 @@
       <c r="M16" t="n">
         <v>617</v>
       </c>
+      <c r="N16" t="n">
+        <v>8.502024291497975</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1120,6 +1170,9 @@
       <c r="M17" t="n">
         <v>895</v>
       </c>
+      <c r="N17" t="n">
+        <v>8.273381294964029</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1163,6 +1216,9 @@
       <c r="M18" t="n">
         <v>1040</v>
       </c>
+      <c r="N18" t="n">
+        <v>14.48275862068966</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1206,6 +1262,9 @@
       <c r="M19" t="n">
         <v>1692</v>
       </c>
+      <c r="N19" t="n">
+        <v>10.88957055214724</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1249,6 +1308,9 @@
       <c r="M20" t="n">
         <v>2433</v>
       </c>
+      <c r="N20" t="n">
+        <v>13.36032388663968</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1292,6 +1354,9 @@
       <c r="M21" t="n">
         <v>3304</v>
       </c>
+      <c r="N21" t="n">
+        <v>12.9735935706085</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1335,6 +1400,9 @@
       <c r="M22" t="n">
         <v>4386</v>
       </c>
+      <c r="N22" t="n">
+        <v>14.51016635859519</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1378,6 +1446,9 @@
       <c r="M23" t="n">
         <v>6125</v>
       </c>
+      <c r="N23" t="n">
+        <v>13.80103507763082</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1421,6 +1492,9 @@
       <c r="M24" t="n">
         <v>6822</v>
       </c>
+      <c r="N24" t="n">
+        <v>20.94691535150645</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1464,6 +1538,9 @@
       <c r="M25" t="n">
         <v>7845</v>
       </c>
+      <c r="N25" t="n">
+        <v>13.97849462365591</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1507,6 +1584,9 @@
       <c r="M26" t="n">
         <v>9303</v>
       </c>
+      <c r="N26" t="n">
+        <v>22.97668038408779</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1550,6 +1630,9 @@
       <c r="M27" t="n">
         <v>10912</v>
       </c>
+      <c r="N27" t="n">
+        <v>24.67371037911746</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1593,6 +1676,9 @@
       <c r="M28" t="n">
         <v>13238</v>
       </c>
+      <c r="N28" t="n">
+        <v>18.18572656921754</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1636,6 +1722,9 @@
       <c r="M29" t="n">
         <v>15847</v>
       </c>
+      <c r="N29" t="n">
+        <v>17.63127635109237</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1679,6 +1768,9 @@
       <c r="M30" t="n">
         <v>18010</v>
       </c>
+      <c r="N30" t="n">
+        <v>21.40545538603791</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1722,6 +1814,9 @@
       <c r="M31" t="n">
         <v>19288</v>
       </c>
+      <c r="N31" t="n">
+        <v>25.35211267605634</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1765,6 +1860,9 @@
       <c r="M32" t="n">
         <v>20920</v>
       </c>
+      <c r="N32" t="n">
+        <v>17.27941176470588</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1808,6 +1906,9 @@
       <c r="M33" t="n">
         <v>22880</v>
       </c>
+      <c r="N33" t="n">
+        <v>23.8265306122449</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1851,6 +1952,9 @@
       <c r="M34" t="n">
         <v>25198</v>
       </c>
+      <c r="N34" t="n">
+        <v>21.48403796376186</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1894,6 +1998,9 @@
       <c r="M35" t="n">
         <v>27741</v>
       </c>
+      <c r="N35" t="n">
+        <v>18.95399134880063</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1937,6 +2044,9 @@
       <c r="M36" t="n">
         <v>30442</v>
       </c>
+      <c r="N36" t="n">
+        <v>18.99296556830803</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1980,6 +2090,9 @@
       <c r="M37" t="n">
         <v>33244</v>
       </c>
+      <c r="N37" t="n">
+        <v>17.41613133476088</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2023,6 +2136,9 @@
       <c r="M38" t="n">
         <v>34880</v>
       </c>
+      <c r="N38" t="n">
+        <v>20.35452322738386</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2066,6 +2182,9 @@
       <c r="M39" t="n">
         <v>35975</v>
       </c>
+      <c r="N39" t="n">
+        <v>21.27853881278539</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2109,6 +2228,9 @@
       <c r="M40" t="n">
         <v>38400</v>
       </c>
+      <c r="N40" t="n">
+        <v>20.61855670103093</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2152,6 +2274,9 @@
       <c r="M41" t="n">
         <v>41182</v>
       </c>
+      <c r="N41" t="n">
+        <v>20.95614665708124</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2195,6 +2320,9 @@
       <c r="M42" t="n">
         <v>44255</v>
       </c>
+      <c r="N42" t="n">
+        <v>19.58997722095672</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2238,6 +2366,9 @@
       <c r="M43" t="n">
         <v>47004</v>
       </c>
+      <c r="N43" t="n">
+        <v>16.69698072026192</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2281,6 +2412,9 @@
       <c r="M44" t="n">
         <v>49731</v>
       </c>
+      <c r="N44" t="n">
+        <v>18.59185918591859</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2324,6 +2458,9 @@
       <c r="M45" t="n">
         <v>51273</v>
       </c>
+      <c r="N45" t="n">
+        <v>19.06614785992218</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2367,6 +2504,9 @@
       <c r="M46" t="n">
         <v>51972</v>
       </c>
+      <c r="N46" t="n">
+        <v>23.89127324749642</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2410,6 +2550,9 @@
       <c r="M47" t="n">
         <v>55443</v>
       </c>
+      <c r="N47" t="n">
+        <v>18.55373091328147</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2453,6 +2596,9 @@
       <c r="M48" t="n">
         <v>59071</v>
       </c>
+      <c r="N48" t="n">
+        <v>17.69570011025358</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2496,6 +2642,9 @@
       <c r="M49" t="n">
         <v>62374</v>
       </c>
+      <c r="N49" t="n">
+        <v>17.71117166212534</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2539,6 +2688,9 @@
       <c r="M50" t="n">
         <v>66377</v>
       </c>
+      <c r="N50" t="n">
+        <v>17.46190357232076</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2582,6 +2734,9 @@
       <c r="M51" t="n">
         <v>70553</v>
       </c>
+      <c r="N51" t="n">
+        <v>18.63026819923371</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2625,6 +2780,9 @@
       <c r="M52" t="n">
         <v>72323</v>
       </c>
+      <c r="N52" t="n">
+        <v>17.74011299435028</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2668,6 +2826,9 @@
       <c r="M53" t="n">
         <v>73437</v>
       </c>
+      <c r="N53" t="n">
+        <v>20.82585278276481</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2711,6 +2872,9 @@
       <c r="M54" t="n">
         <v>77818</v>
       </c>
+      <c r="N54" t="n">
+        <v>18.0324126911664</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2754,6 +2918,9 @@
       <c r="M55" t="n">
         <v>81718</v>
       </c>
+      <c r="N55" t="n">
+        <v>18.30769230769231</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2797,6 +2964,9 @@
       <c r="M56" t="n">
         <v>85636</v>
       </c>
+      <c r="N56" t="n">
+        <v>16.23277182235835</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2840,6 +3010,9 @@
       <c r="M57" t="n">
         <v>90083</v>
       </c>
+      <c r="N57" t="n">
+        <v>30.71733753091972</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2883,6 +3056,9 @@
       <c r="M58" t="n">
         <v>93718</v>
       </c>
+      <c r="N58" t="n">
+        <v>20.90784044016506</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2926,6 +3102,9 @@
       <c r="M59" t="n">
         <v>96088</v>
       </c>
+      <c r="N59" t="n">
+        <v>17.08860759493671</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2969,6 +3148,9 @@
       <c r="M60" t="n">
         <v>97940</v>
       </c>
+      <c r="N60" t="n">
+        <v>13.33693304535637</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2977,10 +3159,10 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>4804</v>
+        <v>4805</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
         <v>4804</v>
@@ -3010,7 +3192,10 @@
         <v>1032</v>
       </c>
       <c r="M61" t="n">
-        <v>102744</v>
+        <v>102745</v>
+      </c>
+      <c r="N61" t="n">
+        <v>16.98231009365244</v>
       </c>
     </row>
     <row r="62">
@@ -3053,7 +3238,10 @@
         <v>1066</v>
       </c>
       <c r="M62" t="n">
-        <v>107801</v>
+        <v>107802</v>
+      </c>
+      <c r="N62" t="n">
+        <v>14.27723947004153</v>
       </c>
     </row>
     <row r="63">
@@ -3096,7 +3284,10 @@
         <v>1109</v>
       </c>
       <c r="M63" t="n">
-        <v>113201</v>
+        <v>113202</v>
+      </c>
+      <c r="N63" t="n">
+        <v>14.33333333333333</v>
       </c>
     </row>
     <row r="64">
@@ -3139,7 +3330,10 @@
         <v>1154</v>
       </c>
       <c r="M64" t="n">
-        <v>119029</v>
+        <v>119030</v>
+      </c>
+      <c r="N64" t="n">
+        <v>12.69732326698696</v>
       </c>
     </row>
     <row r="65">
@@ -3182,7 +3376,10 @@
         <v>1190</v>
       </c>
       <c r="M65" t="n">
-        <v>125748</v>
+        <v>125749</v>
+      </c>
+      <c r="N65" t="n">
+        <v>13.75204643548147</v>
       </c>
     </row>
     <row r="66">
@@ -3225,7 +3422,10 @@
         <v>1234</v>
       </c>
       <c r="M66" t="n">
-        <v>129079</v>
+        <v>129080</v>
+      </c>
+      <c r="N66" t="n">
+        <v>14.0198138697088</v>
       </c>
     </row>
     <row r="67">
@@ -3268,7 +3468,10 @@
         <v>1266</v>
       </c>
       <c r="M67" t="n">
-        <v>130918</v>
+        <v>130919</v>
+      </c>
+      <c r="N67" t="n">
+        <v>16.25883632408918</v>
       </c>
     </row>
     <row r="68">
@@ -3281,10 +3484,10 @@
         <v>5845</v>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>5844</v>
+        <v>5845</v>
       </c>
       <c r="E68" t="n">
         <v>38</v>
@@ -3311,7 +3514,10 @@
         <v>1304</v>
       </c>
       <c r="M68" t="n">
-        <v>136763</v>
+        <v>136764</v>
+      </c>
+      <c r="N68" t="n">
+        <v>11.65098374679213</v>
       </c>
     </row>
     <row r="69">
@@ -3324,10 +3530,10 @@
         <v>6606</v>
       </c>
       <c r="C69" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>6590</v>
+        <v>6606</v>
       </c>
       <c r="E69" t="n">
         <v>38</v>
@@ -3354,7 +3560,10 @@
         <v>1342</v>
       </c>
       <c r="M69" t="n">
-        <v>143369</v>
+        <v>143370</v>
+      </c>
+      <c r="N69" t="n">
+        <v>11.59551922494702</v>
       </c>
     </row>
     <row r="70">
@@ -3367,10 +3576,10 @@
         <v>6016</v>
       </c>
       <c r="C70" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>6012</v>
+        <v>6016</v>
       </c>
       <c r="E70" t="n">
         <v>43</v>
@@ -3397,7 +3606,10 @@
         <v>1385</v>
       </c>
       <c r="M70" t="n">
-        <v>149385</v>
+        <v>149386</v>
+      </c>
+      <c r="N70" t="n">
+        <v>9.308510638297872</v>
       </c>
     </row>
     <row r="71">
@@ -3440,7 +3652,10 @@
         <v>1419</v>
       </c>
       <c r="M71" t="n">
-        <v>156057</v>
+        <v>156058</v>
+      </c>
+      <c r="N71" t="n">
+        <v>9.15767386091127</v>
       </c>
     </row>
     <row r="72">
@@ -3483,7 +3698,10 @@
         <v>1444</v>
       </c>
       <c r="M72" t="n">
-        <v>162783</v>
+        <v>162784</v>
+      </c>
+      <c r="N72" t="n">
+        <v>8.385370205173952</v>
       </c>
     </row>
     <row r="73">
@@ -3526,7 +3744,10 @@
         <v>1476</v>
       </c>
       <c r="M73" t="n">
-        <v>166134</v>
+        <v>166135</v>
+      </c>
+      <c r="N73" t="n">
+        <v>9.877648463145331</v>
       </c>
     </row>
     <row r="74">
@@ -3569,7 +3790,10 @@
         <v>1510</v>
       </c>
       <c r="M74" t="n">
-        <v>167457</v>
+        <v>167458</v>
+      </c>
+      <c r="N74" t="n">
+        <v>10.80876795162509</v>
       </c>
     </row>
     <row r="75">
@@ -3612,7 +3836,10 @@
         <v>1551</v>
       </c>
       <c r="M75" t="n">
-        <v>174627</v>
+        <v>174628</v>
+      </c>
+      <c r="N75" t="n">
+        <v>8.117154811715482</v>
       </c>
     </row>
     <row r="76">
@@ -3655,7 +3882,10 @@
         <v>1589</v>
       </c>
       <c r="M76" t="n">
-        <v>181666</v>
+        <v>181667</v>
+      </c>
+      <c r="N76" t="n">
+        <v>9.418951555618696</v>
       </c>
     </row>
     <row r="77">
@@ -3698,7 +3928,10 @@
         <v>1616</v>
       </c>
       <c r="M77" t="n">
-        <v>188957</v>
+        <v>188958</v>
+      </c>
+      <c r="N77" t="n">
+        <v>8.105883966534083</v>
       </c>
     </row>
     <row r="78">
@@ -3741,7 +3974,10 @@
         <v>1658</v>
       </c>
       <c r="M78" t="n">
-        <v>197149</v>
+        <v>197150</v>
+      </c>
+      <c r="N78" t="n">
+        <v>6.884765625</v>
       </c>
     </row>
     <row r="79">
@@ -3784,7 +4020,10 @@
         <v>1690</v>
       </c>
       <c r="M79" t="n">
-        <v>206931</v>
+        <v>206932</v>
+      </c>
+      <c r="N79" t="n">
+        <v>8.975669597219383</v>
       </c>
     </row>
     <row r="80">
@@ -3827,7 +4066,10 @@
         <v>1718</v>
       </c>
       <c r="M80" t="n">
-        <v>210118</v>
+        <v>210119</v>
+      </c>
+      <c r="N80" t="n">
+        <v>7.405083150298086</v>
       </c>
     </row>
     <row r="81">
@@ -3870,7 +4112,10 @@
         <v>1748</v>
       </c>
       <c r="M81" t="n">
-        <v>212043</v>
+        <v>212044</v>
+      </c>
+      <c r="N81" t="n">
+        <v>10.12987012987013</v>
       </c>
     </row>
     <row r="82">
@@ -3913,7 +4158,10 @@
         <v>1787</v>
       </c>
       <c r="M82" t="n">
-        <v>220419</v>
+        <v>220420</v>
+      </c>
+      <c r="N82" t="n">
+        <v>8.034861509073544</v>
       </c>
     </row>
     <row r="83">
@@ -3956,7 +4204,10 @@
         <v>1816</v>
       </c>
       <c r="M83" t="n">
-        <v>227550</v>
+        <v>227551</v>
+      </c>
+      <c r="N83" t="n">
+        <v>8.848688823446922</v>
       </c>
     </row>
     <row r="84">
@@ -3999,7 +4250,10 @@
         <v>1847</v>
       </c>
       <c r="M84" t="n">
-        <v>234329</v>
+        <v>234330</v>
+      </c>
+      <c r="N84" t="n">
+        <v>9.086885971382209</v>
       </c>
     </row>
     <row r="85">
@@ -4042,7 +4296,10 @@
         <v>1884</v>
       </c>
       <c r="M85" t="n">
-        <v>242030</v>
+        <v>242031</v>
+      </c>
+      <c r="N85" t="n">
+        <v>8.492403583950136</v>
       </c>
     </row>
     <row r="86">
@@ -4052,13 +4309,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>8350</v>
+        <v>8351</v>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>8349</v>
+        <v>8351</v>
       </c>
       <c r="E86" t="n">
         <v>18</v>
@@ -4085,7 +4342,10 @@
         <v>1902</v>
       </c>
       <c r="M86" t="n">
-        <v>250380</v>
+        <v>250382</v>
+      </c>
+      <c r="N86" t="n">
+        <v>7.041072925398156</v>
       </c>
     </row>
     <row r="87">
@@ -4128,7 +4388,10 @@
         <v>1926</v>
       </c>
       <c r="M87" t="n">
-        <v>253236</v>
+        <v>253238</v>
+      </c>
+      <c r="N87" t="n">
+        <v>7.38795518207283</v>
       </c>
     </row>
     <row r="88">
@@ -4171,7 +4434,10 @@
         <v>1941</v>
       </c>
       <c r="M88" t="n">
-        <v>255108</v>
+        <v>255110</v>
+      </c>
+      <c r="N88" t="n">
+        <v>8.814102564102564</v>
       </c>
     </row>
     <row r="89">
@@ -4214,7 +4480,10 @@
         <v>1962</v>
       </c>
       <c r="M89" t="n">
-        <v>256932</v>
+        <v>256934</v>
+      </c>
+      <c r="N89" t="n">
+        <v>9.155701754385964</v>
       </c>
     </row>
     <row r="90">
@@ -4257,7 +4526,10 @@
         <v>1981</v>
       </c>
       <c r="M90" t="n">
-        <v>264911</v>
+        <v>264913</v>
+      </c>
+      <c r="N90" t="n">
+        <v>8.033588168943478</v>
       </c>
     </row>
     <row r="91">
@@ -4300,7 +4572,10 @@
         <v>1995</v>
       </c>
       <c r="M91" t="n">
-        <v>271433</v>
+        <v>271435</v>
+      </c>
+      <c r="N91" t="n">
+        <v>7.313707451701931</v>
       </c>
     </row>
     <row r="92">
@@ -4310,13 +4585,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>7181</v>
+        <v>7180</v>
       </c>
       <c r="C92" t="n">
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>7181</v>
+        <v>7180</v>
       </c>
       <c r="E92" t="n">
         <v>18</v>
@@ -4343,7 +4618,10 @@
         <v>2013</v>
       </c>
       <c r="M92" t="n">
-        <v>278614</v>
+        <v>278615</v>
+      </c>
+      <c r="N92" t="n">
+        <v>7.242339832869081</v>
       </c>
     </row>
     <row r="93">
@@ -4353,13 +4631,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>7826</v>
+        <v>7825</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>7826</v>
+        <v>7825</v>
       </c>
       <c r="E93" t="n">
         <v>21</v>
@@ -4388,6 +4666,9 @@
       <c r="M93" t="n">
         <v>286440</v>
       </c>
+      <c r="N93" t="n">
+        <v>7.067092651757188</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4431,6 +4712,9 @@
       <c r="M94" t="n">
         <v>289333</v>
       </c>
+      <c r="N94" t="n">
+        <v>7.258900795022467</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4474,6 +4758,9 @@
       <c r="M95" t="n">
         <v>291154</v>
       </c>
+      <c r="N95" t="n">
+        <v>7.468423942888523</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4517,6 +4804,9 @@
       <c r="M96" t="n">
         <v>299280</v>
       </c>
+      <c r="N96" t="n">
+        <v>7.371400443022397</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4560,6 +4850,9 @@
       <c r="M97" t="n">
         <v>304991</v>
       </c>
+      <c r="N97" t="n">
+        <v>7.844510593591315</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4603,6 +4896,9 @@
       <c r="M98" t="n">
         <v>311745</v>
       </c>
+      <c r="N98" t="n">
+        <v>6.588688184779389</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4646,6 +4942,9 @@
       <c r="M99" t="n">
         <v>318721</v>
       </c>
+      <c r="N99" t="n">
+        <v>6.708715596330276</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4689,6 +4988,9 @@
       <c r="M100" t="n">
         <v>326653</v>
       </c>
+      <c r="N100" t="n">
+        <v>6.064044377206254</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4732,6 +5034,9 @@
       <c r="M101" t="n">
         <v>330368</v>
       </c>
+      <c r="N101" t="n">
+        <v>4.037685060565275</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4775,6 +5080,9 @@
       <c r="M102" t="n">
         <v>332359</v>
       </c>
+      <c r="N102" t="n">
+        <v>7.885484681064792</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4783,10 +5091,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>9700</v>
+        <v>9701</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
         <v>9700</v>
@@ -4816,7 +5124,10 @@
         <v>2212</v>
       </c>
       <c r="M103" t="n">
-        <v>342059</v>
+        <v>342060</v>
+      </c>
+      <c r="N103" t="n">
+        <v>7.535305638593959</v>
       </c>
     </row>
     <row r="104">
@@ -4826,10 +5137,10 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>6600</v>
+        <v>6603</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D104" t="n">
         <v>6600</v>
@@ -4859,7 +5170,10 @@
         <v>2236</v>
       </c>
       <c r="M104" t="n">
-        <v>348659</v>
+        <v>348663</v>
+      </c>
+      <c r="N104" t="n">
+        <v>6.815084052703317</v>
       </c>
     </row>
     <row r="105">
@@ -4869,10 +5183,10 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>8027</v>
+        <v>8029</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D105" t="n">
         <v>8027</v>
@@ -4902,7 +5216,10 @@
         <v>2253</v>
       </c>
       <c r="M105" t="n">
-        <v>356686</v>
+        <v>356692</v>
+      </c>
+      <c r="N105" t="n">
+        <v>5.89114460082202</v>
       </c>
     </row>
     <row r="106">
@@ -4912,10 +5229,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>9854</v>
+        <v>9856</v>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D106" t="n">
         <v>9854</v>
@@ -4945,7 +5262,10 @@
         <v>2268</v>
       </c>
       <c r="M106" t="n">
-        <v>366540</v>
+        <v>366548</v>
+      </c>
+      <c r="N106" t="n">
+        <v>4.626623376623376</v>
       </c>
     </row>
     <row r="107">
@@ -4988,7 +5308,10 @@
         <v>2281</v>
       </c>
       <c r="M107" t="n">
-        <v>376630</v>
+        <v>376638</v>
+      </c>
+      <c r="N107" t="n">
+        <v>4.132804757185332</v>
       </c>
     </row>
     <row r="108">
@@ -5031,7 +5354,10 @@
         <v>2290</v>
       </c>
       <c r="M108" t="n">
-        <v>381566</v>
+        <v>381574</v>
+      </c>
+      <c r="N108" t="n">
+        <v>3.383306320907618</v>
       </c>
     </row>
     <row r="109">
@@ -5050,10 +5376,10 @@
         <v>1893</v>
       </c>
       <c r="E109" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" t="n">
         <v>20</v>
@@ -5071,10 +5397,13 @@
         <v>39967</v>
       </c>
       <c r="L109" t="n">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="M109" t="n">
-        <v>383459</v>
+        <v>383467</v>
+      </c>
+      <c r="N109" t="n">
+        <v>7.712625462229266</v>
       </c>
     </row>
     <row r="110">
@@ -5084,10 +5413,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>11393</v>
+        <v>11396</v>
       </c>
       <c r="C110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D110" t="n">
         <v>11393</v>
@@ -5114,10 +5443,13 @@
         <v>40381</v>
       </c>
       <c r="L110" t="n">
-        <v>2323</v>
+        <v>2324</v>
       </c>
       <c r="M110" t="n">
-        <v>394852</v>
+        <v>394863</v>
+      </c>
+      <c r="N110" t="n">
+        <v>4.440154440154441</v>
       </c>
     </row>
     <row r="111">
@@ -5127,10 +5459,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>9810</v>
+        <v>9811</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111" t="n">
         <v>9810</v>
@@ -5157,10 +5489,13 @@
         <v>40618</v>
       </c>
       <c r="L111" t="n">
-        <v>2336</v>
+        <v>2337</v>
       </c>
       <c r="M111" t="n">
-        <v>404662</v>
+        <v>404674</v>
+      </c>
+      <c r="N111" t="n">
+        <v>3.74069921516665</v>
       </c>
     </row>
     <row r="112">
@@ -5200,10 +5535,13 @@
         <v>41168</v>
       </c>
       <c r="L112" t="n">
-        <v>2353</v>
+        <v>2354</v>
       </c>
       <c r="M112" t="n">
-        <v>414807</v>
+        <v>414819</v>
+      </c>
+      <c r="N112" t="n">
+        <v>3.992114342040414</v>
       </c>
     </row>
     <row r="113">
@@ -5243,10 +5581,13 @@
         <v>41536</v>
       </c>
       <c r="L113" t="n">
-        <v>2376</v>
+        <v>2377</v>
       </c>
       <c r="M113" t="n">
-        <v>424935</v>
+        <v>424947</v>
+      </c>
+      <c r="N113" t="n">
+        <v>4.216034755134281</v>
       </c>
     </row>
     <row r="114">
@@ -5256,13 +5597,13 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>10222</v>
+        <v>10226</v>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D114" t="n">
-        <v>10222</v>
+        <v>10223</v>
       </c>
       <c r="E114" t="n">
         <v>13</v>
@@ -5286,10 +5627,13 @@
         <v>41917</v>
       </c>
       <c r="L114" t="n">
-        <v>2389</v>
+        <v>2390</v>
       </c>
       <c r="M114" t="n">
-        <v>435157</v>
+        <v>435173</v>
+      </c>
+      <c r="N114" t="n">
+        <v>3.804028945824369</v>
       </c>
     </row>
     <row r="115">
@@ -5329,10 +5673,13 @@
         <v>42288</v>
       </c>
       <c r="L115" t="n">
-        <v>2399</v>
+        <v>2400</v>
       </c>
       <c r="M115" t="n">
-        <v>439552</v>
+        <v>439568</v>
+      </c>
+      <c r="N115" t="n">
+        <v>4.209328782707622</v>
       </c>
     </row>
     <row r="116">
@@ -5372,10 +5719,13 @@
         <v>42536</v>
       </c>
       <c r="L116" t="n">
-        <v>2410</v>
+        <v>2411</v>
       </c>
       <c r="M116" t="n">
-        <v>441394</v>
+        <v>441410</v>
+      </c>
+      <c r="N116" t="n">
+        <v>7.27470141150923</v>
       </c>
     </row>
     <row r="117">
@@ -5385,10 +5735,10 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>10641</v>
+        <v>10643</v>
       </c>
       <c r="C117" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D117" t="n">
         <v>10641</v>
@@ -5415,10 +5765,13 @@
         <v>42840</v>
       </c>
       <c r="L117" t="n">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="M117" t="n">
-        <v>452035</v>
+        <v>452053</v>
+      </c>
+      <c r="N117" t="n">
+        <v>5.355632810297848</v>
       </c>
     </row>
     <row r="118">
@@ -5458,10 +5811,13 @@
         <v>43112</v>
       </c>
       <c r="L118" t="n">
-        <v>2429</v>
+        <v>2430</v>
       </c>
       <c r="M118" t="n">
-        <v>461688</v>
+        <v>461706</v>
+      </c>
+      <c r="N118" t="n">
+        <v>4.827514762250078</v>
       </c>
     </row>
     <row r="119">
@@ -5471,13 +5827,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>9090</v>
+        <v>9092</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D119" t="n">
-        <v>9090</v>
+        <v>9091</v>
       </c>
       <c r="E119" t="n">
         <v>10</v>
@@ -5501,10 +5857,13 @@
         <v>43623</v>
       </c>
       <c r="L119" t="n">
-        <v>2439</v>
+        <v>2440</v>
       </c>
       <c r="M119" t="n">
-        <v>470778</v>
+        <v>470798</v>
+      </c>
+      <c r="N119" t="n">
+        <v>4.64144302683678</v>
       </c>
     </row>
     <row r="120">
@@ -5514,13 +5873,13 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>9293</v>
+        <v>9294</v>
       </c>
       <c r="C120" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D120" t="n">
-        <v>9293</v>
+        <v>9292</v>
       </c>
       <c r="E120" t="n">
         <v>12</v>
@@ -5544,10 +5903,13 @@
         <v>44068</v>
       </c>
       <c r="L120" t="n">
-        <v>2451</v>
+        <v>2452</v>
       </c>
       <c r="M120" t="n">
-        <v>480071</v>
+        <v>480092</v>
+      </c>
+      <c r="N120" t="n">
+        <v>4.723477512373575</v>
       </c>
     </row>
     <row r="121">
@@ -5557,22 +5919,22 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>9735</v>
+        <v>9738</v>
       </c>
       <c r="C121" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D121" t="n">
-        <v>9735</v>
+        <v>9736</v>
       </c>
       <c r="E121" t="n">
         <v>12</v>
       </c>
       <c r="F121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H121" t="n">
         <v>477</v>
@@ -5587,10 +5949,13 @@
         <v>44545</v>
       </c>
       <c r="L121" t="n">
-        <v>2463</v>
+        <v>2464</v>
       </c>
       <c r="M121" t="n">
-        <v>489806</v>
+        <v>489830</v>
+      </c>
+      <c r="N121" t="n">
+        <v>5.586362702813719</v>
       </c>
     </row>
     <row r="122">
@@ -5630,10 +5995,13 @@
         <v>44893</v>
       </c>
       <c r="L122" t="n">
-        <v>2473</v>
+        <v>2474</v>
       </c>
       <c r="M122" t="n">
-        <v>493858</v>
+        <v>493882</v>
+      </c>
+      <c r="N122" t="n">
+        <v>6.04639684106614</v>
       </c>
     </row>
     <row r="123">
@@ -5643,13 +6011,13 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="E123" t="n">
         <v>10</v>
@@ -5673,10 +6041,13 @@
         <v>45193</v>
       </c>
       <c r="L123" t="n">
-        <v>2483</v>
+        <v>2484</v>
       </c>
       <c r="M123" t="n">
-        <v>496826</v>
+        <v>496849</v>
+      </c>
+      <c r="N123" t="n">
+        <v>6.740815638692283</v>
       </c>
     </row>
     <row r="124">
@@ -5686,13 +6057,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>10221</v>
+        <v>10225</v>
       </c>
       <c r="C124" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D124" t="n">
-        <v>10212</v>
+        <v>10222</v>
       </c>
       <c r="E124" t="n">
         <v>8</v>
@@ -5716,10 +6087,13 @@
         <v>45563</v>
       </c>
       <c r="L124" t="n">
-        <v>2491</v>
+        <v>2492</v>
       </c>
       <c r="M124" t="n">
-        <v>507047</v>
+        <v>507074</v>
+      </c>
+      <c r="N124" t="n">
+        <v>6.200488997555012</v>
       </c>
     </row>
     <row r="125">
@@ -5729,13 +6103,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>8769</v>
+        <v>8772</v>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D125" t="n">
-        <v>8769</v>
+        <v>8768</v>
       </c>
       <c r="E125" t="n">
         <v>7</v>
@@ -5759,10 +6133,13 @@
         <v>45919</v>
       </c>
       <c r="L125" t="n">
-        <v>2498</v>
+        <v>2499</v>
       </c>
       <c r="M125" t="n">
-        <v>515816</v>
+        <v>515846</v>
+      </c>
+      <c r="N125" t="n">
+        <v>6.452348381212951</v>
       </c>
     </row>
     <row r="126">
@@ -5772,13 +6149,13 @@
         </is>
       </c>
       <c r="B126" t="n">
+        <v>7881</v>
+      </c>
+      <c r="C126" t="n">
+        <v>8</v>
+      </c>
+      <c r="D126" t="n">
         <v>7873</v>
-      </c>
-      <c r="C126" t="n">
-        <v>1</v>
-      </c>
-      <c r="D126" t="n">
-        <v>7872</v>
       </c>
       <c r="E126" t="n">
         <v>11</v>
@@ -5802,10 +6179,13 @@
         <v>46359</v>
       </c>
       <c r="L126" t="n">
-        <v>2509</v>
+        <v>2510</v>
       </c>
       <c r="M126" t="n">
-        <v>523689</v>
+        <v>523727</v>
+      </c>
+      <c r="N126" t="n">
+        <v>6.407816266971196</v>
       </c>
     </row>
     <row r="127">
@@ -5815,13 +6195,13 @@
         </is>
       </c>
       <c r="B127" t="n">
+        <v>9102</v>
+      </c>
+      <c r="C127" t="n">
+        <v>2</v>
+      </c>
+      <c r="D127" t="n">
         <v>9100</v>
-      </c>
-      <c r="C127" t="n">
-        <v>1</v>
-      </c>
-      <c r="D127" t="n">
-        <v>9099</v>
       </c>
       <c r="E127" t="n">
         <v>8</v>
@@ -5845,10 +6225,13 @@
         <v>46887</v>
       </c>
       <c r="L127" t="n">
-        <v>2517</v>
+        <v>2518</v>
       </c>
       <c r="M127" t="n">
-        <v>532789</v>
+        <v>532829</v>
+      </c>
+      <c r="N127" t="n">
+        <v>6.877609316633706</v>
       </c>
     </row>
     <row r="128">
@@ -5861,10 +6244,10 @@
         <v>5187</v>
       </c>
       <c r="C128" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>5184</v>
+        <v>5187</v>
       </c>
       <c r="E128" t="n">
         <v>9</v>
@@ -5888,10 +6271,13 @@
         <v>47383</v>
       </c>
       <c r="L128" t="n">
-        <v>2526</v>
+        <v>2527</v>
       </c>
       <c r="M128" t="n">
-        <v>537976</v>
+        <v>538016</v>
+      </c>
+      <c r="N128" t="n">
+        <v>5.764411027568922</v>
       </c>
     </row>
     <row r="129">
@@ -5931,10 +6317,13 @@
         <v>47972</v>
       </c>
       <c r="L129" t="n">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="M129" t="n">
-        <v>540067</v>
+        <v>540107</v>
+      </c>
+      <c r="N129" t="n">
+        <v>7.269249163079866</v>
       </c>
     </row>
     <row r="130">
@@ -5974,10 +6363,13 @@
         <v>48287</v>
       </c>
       <c r="L130" t="n">
-        <v>2545</v>
+        <v>2546</v>
       </c>
       <c r="M130" t="n">
-        <v>542762</v>
+        <v>542802</v>
+      </c>
+      <c r="N130" t="n">
+        <v>10.27829313543599</v>
       </c>
     </row>
     <row r="131">
@@ -5987,13 +6379,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>11209</v>
+        <v>11212</v>
       </c>
       <c r="C131" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D131" t="n">
-        <v>11196</v>
+        <v>11208</v>
       </c>
       <c r="E131" t="n">
         <v>14</v>
@@ -6017,10 +6409,13 @@
         <v>48587</v>
       </c>
       <c r="L131" t="n">
-        <v>2559</v>
+        <v>2560</v>
       </c>
       <c r="M131" t="n">
-        <v>553971</v>
+        <v>554014</v>
+      </c>
+      <c r="N131" t="n">
+        <v>7.367106671423475</v>
       </c>
     </row>
     <row r="132">
@@ -6030,13 +6425,13 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>9768</v>
+        <v>9792</v>
       </c>
       <c r="C132" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D132" t="n">
-        <v>9758</v>
+        <v>9770</v>
       </c>
       <c r="E132" t="n">
         <v>6</v>
@@ -6060,10 +6455,13 @@
         <v>49032</v>
       </c>
       <c r="L132" t="n">
-        <v>2565</v>
+        <v>2566</v>
       </c>
       <c r="M132" t="n">
-        <v>563739</v>
+        <v>563806</v>
+      </c>
+      <c r="N132" t="n">
+        <v>7.792075163398692</v>
       </c>
     </row>
     <row r="133">
@@ -6073,13 +6471,13 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>8671</v>
+        <v>8690</v>
       </c>
       <c r="C133" t="n">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D133" t="n">
-        <v>8627</v>
+        <v>8676</v>
       </c>
       <c r="E133" t="n">
         <v>7</v>
@@ -6103,10 +6501,13 @@
         <v>49531</v>
       </c>
       <c r="L133" t="n">
-        <v>2572</v>
+        <v>2573</v>
       </c>
       <c r="M133" t="n">
-        <v>572410</v>
+        <v>572496</v>
+      </c>
+      <c r="N133" t="n">
+        <v>7.456846950517837</v>
       </c>
     </row>
     <row r="134">
@@ -6116,13 +6517,13 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>8590</v>
+        <v>8588</v>
       </c>
       <c r="C134" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D134" t="n">
-        <v>8572</v>
+        <v>8584</v>
       </c>
       <c r="E134" t="n">
         <v>10</v>
@@ -6146,10 +6547,13 @@
         <v>50251</v>
       </c>
       <c r="L134" t="n">
-        <v>2582</v>
+        <v>2583</v>
       </c>
       <c r="M134" t="n">
-        <v>581000</v>
+        <v>581084</v>
+      </c>
+      <c r="N134" t="n">
+        <v>6.904983698183512</v>
       </c>
     </row>
     <row r="135">
@@ -6159,13 +6563,13 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>9818</v>
+        <v>9826</v>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D135" t="n">
-        <v>9818</v>
+        <v>9815</v>
       </c>
       <c r="E135" t="n">
         <v>7</v>
@@ -6189,10 +6593,13 @@
         <v>51008</v>
       </c>
       <c r="L135" t="n">
-        <v>2589</v>
+        <v>2590</v>
       </c>
       <c r="M135" t="n">
-        <v>590818</v>
+        <v>590910</v>
+      </c>
+      <c r="N135" t="n">
+        <v>6.228373702422145</v>
       </c>
     </row>
     <row r="136">
@@ -6202,13 +6609,13 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>4560</v>
+        <v>4567</v>
       </c>
       <c r="C136" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D136" t="n">
-        <v>4547</v>
+        <v>4561</v>
       </c>
       <c r="E136" t="n">
         <v>8</v>
@@ -6232,10 +6639,13 @@
         <v>51554</v>
       </c>
       <c r="L136" t="n">
-        <v>2597</v>
+        <v>2598</v>
       </c>
       <c r="M136" t="n">
-        <v>595378</v>
+        <v>595477</v>
+      </c>
+      <c r="N136" t="n">
+        <v>6.875410553974162</v>
       </c>
     </row>
     <row r="137">
@@ -6245,13 +6655,13 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>3004</v>
+        <v>3140</v>
       </c>
       <c r="C137" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D137" t="n">
-        <v>2898</v>
+        <v>3029</v>
       </c>
       <c r="E137" t="n">
         <v>13</v>
@@ -6275,10 +6685,13 @@
         <v>52000</v>
       </c>
       <c r="L137" t="n">
-        <v>2610</v>
+        <v>2611</v>
       </c>
       <c r="M137" t="n">
-        <v>598382</v>
+        <v>598617</v>
+      </c>
+      <c r="N137" t="n">
+        <v>8.980891719745223</v>
       </c>
     </row>
     <row r="138">
@@ -6288,13 +6701,13 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>11545</v>
+        <v>11745</v>
       </c>
       <c r="C138" t="n">
-        <v>23</v>
+        <v>186</v>
       </c>
       <c r="D138" t="n">
-        <v>11522</v>
+        <v>11559</v>
       </c>
       <c r="E138" t="n">
         <v>9</v>
@@ -6318,10 +6731,13 @@
         <v>52645</v>
       </c>
       <c r="L138" t="n">
-        <v>2619</v>
+        <v>2620</v>
       </c>
       <c r="M138" t="n">
-        <v>609927</v>
+        <v>610362</v>
+      </c>
+      <c r="N138" t="n">
+        <v>7.441464452958706</v>
       </c>
     </row>
     <row r="139">
@@ -6331,13 +6747,13 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>10906</v>
+        <v>11076</v>
       </c>
       <c r="C139" t="n">
-        <v>309</v>
+        <v>162</v>
       </c>
       <c r="D139" t="n">
-        <v>10597</v>
+        <v>10914</v>
       </c>
       <c r="E139" t="n">
         <v>5</v>
@@ -6361,10 +6777,13 @@
         <v>53323</v>
       </c>
       <c r="L139" t="n">
-        <v>2624</v>
+        <v>2625</v>
       </c>
       <c r="M139" t="n">
-        <v>620833</v>
+        <v>621438</v>
+      </c>
+      <c r="N139" t="n">
+        <v>6.644998194293969</v>
       </c>
     </row>
     <row r="140">
@@ -6374,13 +6793,13 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>10354</v>
+        <v>10742</v>
       </c>
       <c r="C140" t="n">
-        <v>171</v>
+        <v>368</v>
       </c>
       <c r="D140" t="n">
-        <v>10183</v>
+        <v>10374</v>
       </c>
       <c r="E140" t="n">
         <v>10</v>
@@ -6404,10 +6823,13 @@
         <v>54044</v>
       </c>
       <c r="L140" t="n">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="M140" t="n">
-        <v>631187</v>
+        <v>632180</v>
+      </c>
+      <c r="N140" t="n">
+        <v>6.86091975423571</v>
       </c>
     </row>
     <row r="141">
@@ -6417,10 +6839,10 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>11628</v>
+        <v>11705</v>
       </c>
       <c r="C141" t="n">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D141" t="n">
         <v>11619</v>
@@ -6447,10 +6869,13 @@
         <v>54782</v>
       </c>
       <c r="L141" t="n">
-        <v>2643</v>
+        <v>2644</v>
       </c>
       <c r="M141" t="n">
-        <v>642815</v>
+        <v>643885</v>
+      </c>
+      <c r="N141" t="n">
+        <v>6.655275523280649</v>
       </c>
     </row>
     <row r="142">
@@ -6460,13 +6885,13 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>12024</v>
+        <v>12026</v>
       </c>
       <c r="C142" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D142" t="n">
-        <v>12018</v>
+        <v>12013</v>
       </c>
       <c r="E142" t="n">
         <v>8</v>
@@ -6490,10 +6915,13 @@
         <v>55616</v>
       </c>
       <c r="L142" t="n">
-        <v>2651</v>
+        <v>2652</v>
       </c>
       <c r="M142" t="n">
-        <v>654839</v>
+        <v>655911</v>
+      </c>
+      <c r="N142" t="n">
+        <v>6.053550640279394</v>
       </c>
     </row>
     <row r="143">
@@ -6503,13 +6931,13 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>4769</v>
+        <v>4770</v>
       </c>
       <c r="C143" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D143" t="n">
-        <v>4767</v>
+        <v>4764</v>
       </c>
       <c r="E143" t="n">
         <v>6</v>
@@ -6533,10 +6961,13 @@
         <v>56526</v>
       </c>
       <c r="L143" t="n">
-        <v>2657</v>
+        <v>2658</v>
       </c>
       <c r="M143" t="n">
-        <v>659608</v>
+        <v>660681</v>
+      </c>
+      <c r="N143" t="n">
+        <v>5.828092243186583</v>
       </c>
     </row>
     <row r="144">
@@ -6546,40 +6977,43 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>2926</v>
+        <v>2931</v>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="E144" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G144" t="n">
         <v>7</v>
       </c>
       <c r="H144" t="n">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I144" t="n">
         <v>0</v>
       </c>
       <c r="J144" t="n">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K144" t="n">
-        <v>57167</v>
+        <v>57166</v>
       </c>
       <c r="L144" t="n">
-        <v>2664</v>
+        <v>2666</v>
       </c>
       <c r="M144" t="n">
-        <v>662534</v>
+        <v>663612</v>
+      </c>
+      <c r="N144" t="n">
+        <v>8.836574547935857</v>
       </c>
     </row>
     <row r="145">
@@ -6589,13 +7023,13 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>12375</v>
+        <v>12378</v>
       </c>
       <c r="C145" t="n">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="D145" t="n">
-        <v>12291</v>
+        <v>12368</v>
       </c>
       <c r="E145" t="n">
         <v>13</v>
@@ -6616,13 +7050,16 @@
         <v>715</v>
       </c>
       <c r="K145" t="n">
-        <v>57882</v>
+        <v>57881</v>
       </c>
       <c r="L145" t="n">
-        <v>2677</v>
+        <v>2679</v>
       </c>
       <c r="M145" t="n">
-        <v>674909</v>
+        <v>675990</v>
+      </c>
+      <c r="N145" t="n">
+        <v>6.745839392470512</v>
       </c>
     </row>
     <row r="146">
@@ -6632,13 +7069,13 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>11950</v>
+        <v>12005</v>
       </c>
       <c r="C146" t="n">
-        <v>323</v>
+        <v>63</v>
       </c>
       <c r="D146" t="n">
-        <v>11627</v>
+        <v>11942</v>
       </c>
       <c r="E146" t="n">
         <v>8</v>
@@ -6659,13 +7096,16 @@
         <v>736</v>
       </c>
       <c r="K146" t="n">
-        <v>58618</v>
+        <v>58617</v>
       </c>
       <c r="L146" t="n">
-        <v>2685</v>
+        <v>2687</v>
       </c>
       <c r="M146" t="n">
-        <v>686859</v>
+        <v>687995</v>
+      </c>
+      <c r="N146" t="n">
+        <v>6.913785922532279</v>
       </c>
     </row>
     <row r="147">
@@ -6675,13 +7115,13 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>10959</v>
+        <v>11054</v>
       </c>
       <c r="C147" t="n">
-        <v>551</v>
+        <v>110</v>
       </c>
       <c r="D147" t="n">
-        <v>10408</v>
+        <v>10944</v>
       </c>
       <c r="E147" t="n">
         <v>12</v>
@@ -6693,22 +7133,25 @@
         <v>12</v>
       </c>
       <c r="H147" t="n">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="I147" t="n">
         <v>0</v>
       </c>
       <c r="J147" t="n">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="K147" t="n">
-        <v>59557</v>
+        <v>59553</v>
       </c>
       <c r="L147" t="n">
-        <v>2697</v>
+        <v>2699</v>
       </c>
       <c r="M147" t="n">
-        <v>697818</v>
+        <v>699049</v>
+      </c>
+      <c r="N147" t="n">
+        <v>7.083408720825041</v>
       </c>
     </row>
     <row r="148">
@@ -6718,40 +7161,43 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>10491</v>
+        <v>10938</v>
       </c>
       <c r="C148" t="n">
-        <v>736</v>
+        <v>455</v>
       </c>
       <c r="D148" t="n">
-        <v>9755</v>
+        <v>10483</v>
       </c>
       <c r="E148" t="n">
         <v>10</v>
       </c>
       <c r="F148" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H148" t="n">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I148" t="n">
         <v>0</v>
       </c>
       <c r="J148" t="n">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="K148" t="n">
-        <v>60556</v>
+        <v>60551</v>
       </c>
       <c r="L148" t="n">
-        <v>2707</v>
+        <v>2709</v>
       </c>
       <c r="M148" t="n">
-        <v>708309</v>
+        <v>709987</v>
+      </c>
+      <c r="N148" t="n">
+        <v>6.920826476503931</v>
       </c>
     </row>
     <row r="149">
@@ -6761,22 +7207,22 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>10241</v>
+        <v>11027</v>
       </c>
       <c r="C149" t="n">
-        <v>2204</v>
+        <v>801</v>
       </c>
       <c r="D149" t="n">
-        <v>8037</v>
+        <v>10226</v>
       </c>
       <c r="E149" t="n">
+        <v>9</v>
+      </c>
+      <c r="F149" t="n">
+        <v>1</v>
+      </c>
+      <c r="G149" t="n">
         <v>8</v>
-      </c>
-      <c r="F149" t="n">
-        <v>2</v>
-      </c>
-      <c r="G149" t="n">
-        <v>6</v>
       </c>
       <c r="H149" t="n">
         <v>916</v>
@@ -6788,14 +7234,15 @@
         <v>916</v>
       </c>
       <c r="K149" t="n">
-        <v>61472</v>
+        <v>61467</v>
       </c>
       <c r="L149" t="n">
-        <v>2715</v>
+        <v>2718</v>
       </c>
       <c r="M149" t="n">
-        <v>718550</v>
-      </c>
+        <v>721014</v>
+      </c>
+      <c r="N149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6804,41 +7251,42 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>2641</v>
+        <v>3900</v>
       </c>
       <c r="C150" t="n">
-        <v>668</v>
+        <v>1263</v>
       </c>
       <c r="D150" t="n">
-        <v>1973</v>
+        <v>2637</v>
       </c>
       <c r="E150" t="n">
         <v>7</v>
       </c>
       <c r="F150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G150" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H150" t="n">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="K150" t="n">
-        <v>62311</v>
+        <v>62304</v>
       </c>
       <c r="L150" t="n">
-        <v>2722</v>
+        <v>2725</v>
       </c>
       <c r="M150" t="n">
-        <v>721191</v>
-      </c>
+        <v>724914</v>
+      </c>
+      <c r="N150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6847,13 +7295,13 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>1280</v>
+        <v>1964</v>
       </c>
       <c r="C151" t="n">
-        <v>531</v>
+        <v>687</v>
       </c>
       <c r="D151" t="n">
-        <v>749</v>
+        <v>1277</v>
       </c>
       <c r="E151" t="n">
         <v>8</v>
@@ -6874,14 +7322,15 @@
         <v>552</v>
       </c>
       <c r="K151" t="n">
-        <v>62863</v>
+        <v>62856</v>
       </c>
       <c r="L151" t="n">
-        <v>2730</v>
+        <v>2733</v>
       </c>
       <c r="M151" t="n">
-        <v>722471</v>
-      </c>
+        <v>726878</v>
+      </c>
+      <c r="N151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6890,22 +7339,22 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>1651</v>
+        <v>7082</v>
       </c>
       <c r="C152" t="n">
-        <v>1491</v>
+        <v>5442</v>
       </c>
       <c r="D152" t="n">
-        <v>160</v>
+        <v>1640</v>
       </c>
       <c r="E152" t="n">
+        <v>4</v>
+      </c>
+      <c r="F152" t="n">
         <v>2</v>
       </c>
-      <c r="F152" t="n">
-        <v>1</v>
-      </c>
       <c r="G152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H152" t="n">
         <v>804</v>
@@ -6917,14 +7366,15 @@
         <v>804</v>
       </c>
       <c r="K152" t="n">
-        <v>63667</v>
+        <v>63660</v>
       </c>
       <c r="L152" t="n">
-        <v>2732</v>
+        <v>2737</v>
       </c>
       <c r="M152" t="n">
-        <v>724122</v>
-      </c>
+        <v>733960</v>
+      </c>
+      <c r="N152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6933,41 +7383,86 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>116</v>
+        <v>1702</v>
       </c>
       <c r="C153" t="n">
-        <v>116</v>
+        <v>1588</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="E153" t="n">
+        <v>4</v>
+      </c>
+      <c r="F153" t="n">
+        <v>3</v>
+      </c>
+      <c r="G153" t="n">
         <v>1</v>
       </c>
-      <c r="F153" t="n">
-        <v>1</v>
-      </c>
-      <c r="G153" t="n">
-        <v>0</v>
-      </c>
       <c r="H153" t="n">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="I153" t="n">
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="J153" t="n">
-        <v>2</v>
+        <v>623</v>
       </c>
       <c r="K153" t="n">
-        <v>64299</v>
+        <v>64283</v>
       </c>
       <c r="L153" t="n">
-        <v>2733</v>
+        <v>2741</v>
       </c>
       <c r="M153" t="n">
-        <v>724238</v>
-      </c>
+        <v>735662</v>
+      </c>
+      <c r="N153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2020-07-29</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>186</v>
+      </c>
+      <c r="C154" t="n">
+        <v>186</v>
+      </c>
+      <c r="D154" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" t="n">
+        <v>5</v>
+      </c>
+      <c r="F154" t="n">
+        <v>5</v>
+      </c>
+      <c r="G154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" t="n">
+        <v>970</v>
+      </c>
+      <c r="I154" t="n">
+        <v>970</v>
+      </c>
+      <c r="J154" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="n">
+        <v>65253</v>
+      </c>
+      <c r="L154" t="n">
+        <v>2746</v>
+      </c>
+      <c r="M154" t="n">
+        <v>735848</v>
+      </c>
+      <c r="N154" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
updated case-trend because it happened with a script I was messing with
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M164"/>
+  <dimension ref="A1:M165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2203,13 +2203,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="E43" t="n">
         <v>37</v>
@@ -2236,7 +2236,7 @@
         <v>375</v>
       </c>
       <c r="M43" t="n">
-        <v>47197</v>
+        <v>47196</v>
       </c>
     </row>
     <row r="44">
@@ -2279,7 +2279,7 @@
         <v>400</v>
       </c>
       <c r="M44" t="n">
-        <v>49928</v>
+        <v>49927</v>
       </c>
     </row>
     <row r="45">
@@ -2322,7 +2322,7 @@
         <v>420</v>
       </c>
       <c r="M45" t="n">
-        <v>51471</v>
+        <v>51470</v>
       </c>
     </row>
     <row r="46">
@@ -2365,7 +2365,7 @@
         <v>449</v>
       </c>
       <c r="M46" t="n">
-        <v>52181</v>
+        <v>52180</v>
       </c>
     </row>
     <row r="47">
@@ -2378,10 +2378,10 @@
         <v>3494</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>3493</v>
+        <v>3494</v>
       </c>
       <c r="E47" t="n">
         <v>35</v>
@@ -2408,7 +2408,7 @@
         <v>484</v>
       </c>
       <c r="M47" t="n">
-        <v>55675</v>
+        <v>55674</v>
       </c>
     </row>
     <row r="48">
@@ -2451,7 +2451,7 @@
         <v>530</v>
       </c>
       <c r="M48" t="n">
-        <v>59319</v>
+        <v>59318</v>
       </c>
     </row>
     <row r="49">
@@ -2494,7 +2494,7 @@
         <v>568</v>
       </c>
       <c r="M49" t="n">
-        <v>62642</v>
+        <v>62641</v>
       </c>
     </row>
     <row r="50">
@@ -2537,7 +2537,7 @@
         <v>602</v>
       </c>
       <c r="M50" t="n">
-        <v>66664</v>
+        <v>66663</v>
       </c>
     </row>
     <row r="51">
@@ -2580,7 +2580,7 @@
         <v>638</v>
       </c>
       <c r="M51" t="n">
-        <v>70859</v>
+        <v>70858</v>
       </c>
     </row>
     <row r="52">
@@ -2623,7 +2623,7 @@
         <v>666</v>
       </c>
       <c r="M52" t="n">
-        <v>72644</v>
+        <v>72643</v>
       </c>
     </row>
     <row r="53">
@@ -2666,7 +2666,7 @@
         <v>703</v>
       </c>
       <c r="M53" t="n">
-        <v>73781</v>
+        <v>73780</v>
       </c>
     </row>
     <row r="54">
@@ -2709,7 +2709,7 @@
         <v>741</v>
       </c>
       <c r="M54" t="n">
-        <v>78186</v>
+        <v>78185</v>
       </c>
     </row>
     <row r="55">
@@ -2752,7 +2752,7 @@
         <v>790</v>
       </c>
       <c r="M55" t="n">
-        <v>82113</v>
+        <v>82112</v>
       </c>
     </row>
     <row r="56">
@@ -2795,7 +2795,7 @@
         <v>840</v>
       </c>
       <c r="M56" t="n">
-        <v>86056</v>
+        <v>86055</v>
       </c>
     </row>
     <row r="57">
@@ -2838,7 +2838,7 @@
         <v>878</v>
       </c>
       <c r="M57" t="n">
-        <v>90575</v>
+        <v>90574</v>
       </c>
     </row>
     <row r="58">
@@ -2881,7 +2881,7 @@
         <v>915</v>
       </c>
       <c r="M58" t="n">
-        <v>94262</v>
+        <v>94261</v>
       </c>
     </row>
     <row r="59">
@@ -2924,7 +2924,7 @@
         <v>956</v>
       </c>
       <c r="M59" t="n">
-        <v>96654</v>
+        <v>96653</v>
       </c>
     </row>
     <row r="60">
@@ -2967,7 +2967,7 @@
         <v>990</v>
       </c>
       <c r="M60" t="n">
-        <v>98515</v>
+        <v>98514</v>
       </c>
     </row>
     <row r="61">
@@ -2977,13 +2977,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>4843</v>
+        <v>4841</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>4843</v>
+        <v>4841</v>
       </c>
       <c r="E61" t="n">
         <v>42</v>
@@ -3010,7 +3010,7 @@
         <v>1032</v>
       </c>
       <c r="M61" t="n">
-        <v>103358</v>
+        <v>103355</v>
       </c>
     </row>
     <row r="62">
@@ -3053,7 +3053,7 @@
         <v>1066</v>
       </c>
       <c r="M62" t="n">
-        <v>108453</v>
+        <v>108450</v>
       </c>
     </row>
     <row r="63">
@@ -3096,7 +3096,7 @@
         <v>1109</v>
       </c>
       <c r="M63" t="n">
-        <v>113871</v>
+        <v>113868</v>
       </c>
     </row>
     <row r="64">
@@ -3139,7 +3139,7 @@
         <v>1154</v>
       </c>
       <c r="M64" t="n">
-        <v>119702</v>
+        <v>119699</v>
       </c>
     </row>
     <row r="65">
@@ -3182,7 +3182,7 @@
         <v>1190</v>
       </c>
       <c r="M65" t="n">
-        <v>126440</v>
+        <v>126437</v>
       </c>
     </row>
     <row r="66">
@@ -3195,10 +3195,10 @@
         <v>3336</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>3336</v>
+        <v>3335</v>
       </c>
       <c r="E66" t="n">
         <v>44</v>
@@ -3225,7 +3225,7 @@
         <v>1234</v>
       </c>
       <c r="M66" t="n">
-        <v>129776</v>
+        <v>129773</v>
       </c>
     </row>
     <row r="67">
@@ -3268,7 +3268,7 @@
         <v>1266</v>
       </c>
       <c r="M67" t="n">
-        <v>131617</v>
+        <v>131614</v>
       </c>
     </row>
     <row r="68">
@@ -3311,7 +3311,7 @@
         <v>1304</v>
       </c>
       <c r="M68" t="n">
-        <v>137478</v>
+        <v>137475</v>
       </c>
     </row>
     <row r="69">
@@ -3354,7 +3354,7 @@
         <v>1342</v>
       </c>
       <c r="M69" t="n">
-        <v>144093</v>
+        <v>144090</v>
       </c>
     </row>
     <row r="70">
@@ -3397,7 +3397,7 @@
         <v>1385</v>
       </c>
       <c r="M70" t="n">
-        <v>150136</v>
+        <v>150133</v>
       </c>
     </row>
     <row r="71">
@@ -3410,10 +3410,10 @@
         <v>6705</v>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>6704</v>
+        <v>6705</v>
       </c>
       <c r="E71" t="n">
         <v>34</v>
@@ -3440,7 +3440,7 @@
         <v>1419</v>
       </c>
       <c r="M71" t="n">
-        <v>156841</v>
+        <v>156838</v>
       </c>
     </row>
     <row r="72">
@@ -3483,7 +3483,7 @@
         <v>1444</v>
       </c>
       <c r="M72" t="n">
-        <v>163592</v>
+        <v>163589</v>
       </c>
     </row>
     <row r="73">
@@ -3526,7 +3526,7 @@
         <v>1476</v>
       </c>
       <c r="M73" t="n">
-        <v>166949</v>
+        <v>166946</v>
       </c>
     </row>
     <row r="74">
@@ -3569,7 +3569,7 @@
         <v>1510</v>
       </c>
       <c r="M74" t="n">
-        <v>168274</v>
+        <v>168271</v>
       </c>
     </row>
     <row r="75">
@@ -3612,7 +3612,7 @@
         <v>1551</v>
       </c>
       <c r="M75" t="n">
-        <v>175498</v>
+        <v>175495</v>
       </c>
     </row>
     <row r="76">
@@ -3655,7 +3655,7 @@
         <v>1589</v>
       </c>
       <c r="M76" t="n">
-        <v>182558</v>
+        <v>182555</v>
       </c>
     </row>
     <row r="77">
@@ -3698,7 +3698,7 @@
         <v>1616</v>
       </c>
       <c r="M77" t="n">
-        <v>189861</v>
+        <v>189858</v>
       </c>
     </row>
     <row r="78">
@@ -3741,7 +3741,7 @@
         <v>1658</v>
       </c>
       <c r="M78" t="n">
-        <v>198057</v>
+        <v>198054</v>
       </c>
     </row>
     <row r="79">
@@ -3784,7 +3784,7 @@
         <v>1690</v>
       </c>
       <c r="M79" t="n">
-        <v>207845</v>
+        <v>207842</v>
       </c>
     </row>
     <row r="80">
@@ -3797,10 +3797,10 @@
         <v>3194</v>
       </c>
       <c r="C80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>3193</v>
+        <v>3194</v>
       </c>
       <c r="E80" t="n">
         <v>28</v>
@@ -3827,7 +3827,7 @@
         <v>1718</v>
       </c>
       <c r="M80" t="n">
-        <v>211039</v>
+        <v>211036</v>
       </c>
     </row>
     <row r="81">
@@ -3870,7 +3870,7 @@
         <v>1748</v>
       </c>
       <c r="M81" t="n">
-        <v>212970</v>
+        <v>212967</v>
       </c>
     </row>
     <row r="82">
@@ -3913,7 +3913,7 @@
         <v>1787</v>
       </c>
       <c r="M82" t="n">
-        <v>221366</v>
+        <v>221363</v>
       </c>
     </row>
     <row r="83">
@@ -3956,7 +3956,7 @@
         <v>1816</v>
       </c>
       <c r="M83" t="n">
-        <v>228503</v>
+        <v>228500</v>
       </c>
     </row>
     <row r="84">
@@ -3999,7 +3999,7 @@
         <v>1847</v>
       </c>
       <c r="M84" t="n">
-        <v>235297</v>
+        <v>235294</v>
       </c>
     </row>
     <row r="85">
@@ -4042,7 +4042,7 @@
         <v>1884</v>
       </c>
       <c r="M85" t="n">
-        <v>243006</v>
+        <v>243003</v>
       </c>
     </row>
     <row r="86">
@@ -4085,7 +4085,7 @@
         <v>1902</v>
       </c>
       <c r="M86" t="n">
-        <v>251362</v>
+        <v>251359</v>
       </c>
     </row>
     <row r="87">
@@ -4128,7 +4128,7 @@
         <v>1926</v>
       </c>
       <c r="M87" t="n">
-        <v>254219</v>
+        <v>254216</v>
       </c>
     </row>
     <row r="88">
@@ -4171,7 +4171,7 @@
         <v>1941</v>
       </c>
       <c r="M88" t="n">
-        <v>256096</v>
+        <v>256093</v>
       </c>
     </row>
     <row r="89">
@@ -4214,7 +4214,7 @@
         <v>1962</v>
       </c>
       <c r="M89" t="n">
-        <v>257922</v>
+        <v>257919</v>
       </c>
     </row>
     <row r="90">
@@ -4257,7 +4257,7 @@
         <v>1981</v>
       </c>
       <c r="M90" t="n">
-        <v>265922</v>
+        <v>265919</v>
       </c>
     </row>
     <row r="91">
@@ -4300,7 +4300,7 @@
         <v>1995</v>
       </c>
       <c r="M91" t="n">
-        <v>272457</v>
+        <v>272454</v>
       </c>
     </row>
     <row r="92">
@@ -4343,7 +4343,7 @@
         <v>2013</v>
       </c>
       <c r="M92" t="n">
-        <v>279650</v>
+        <v>279647</v>
       </c>
     </row>
     <row r="93">
@@ -4386,7 +4386,7 @@
         <v>2034</v>
       </c>
       <c r="M93" t="n">
-        <v>287482</v>
+        <v>287479</v>
       </c>
     </row>
     <row r="94">
@@ -4429,7 +4429,7 @@
         <v>2055</v>
       </c>
       <c r="M94" t="n">
-        <v>290376</v>
+        <v>290373</v>
       </c>
     </row>
     <row r="95">
@@ -4472,7 +4472,7 @@
         <v>2071</v>
       </c>
       <c r="M95" t="n">
-        <v>292199</v>
+        <v>292196</v>
       </c>
     </row>
     <row r="96">
@@ -4515,7 +4515,7 @@
         <v>2091</v>
       </c>
       <c r="M96" t="n">
-        <v>300337</v>
+        <v>300334</v>
       </c>
     </row>
     <row r="97">
@@ -4558,7 +4558,7 @@
         <v>2106</v>
       </c>
       <c r="M97" t="n">
-        <v>306062</v>
+        <v>306059</v>
       </c>
     </row>
     <row r="98">
@@ -4568,10 +4568,10 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6768</v>
+        <v>6774</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D98" t="n">
         <v>6768</v>
@@ -4601,7 +4601,7 @@
         <v>2130</v>
       </c>
       <c r="M98" t="n">
-        <v>312830</v>
+        <v>312833</v>
       </c>
     </row>
     <row r="99">
@@ -4611,10 +4611,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>6980</v>
+        <v>6982</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
         <v>6980</v>
@@ -4644,7 +4644,7 @@
         <v>2152</v>
       </c>
       <c r="M99" t="n">
-        <v>319810</v>
+        <v>319815</v>
       </c>
     </row>
     <row r="100">
@@ -4654,10 +4654,10 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>7946</v>
+        <v>7947</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="n">
         <v>7946</v>
@@ -4687,7 +4687,7 @@
         <v>2173</v>
       </c>
       <c r="M100" t="n">
-        <v>327756</v>
+        <v>327762</v>
       </c>
     </row>
     <row r="101">
@@ -4730,7 +4730,7 @@
         <v>2181</v>
       </c>
       <c r="M101" t="n">
-        <v>331474</v>
+        <v>331480</v>
       </c>
     </row>
     <row r="102">
@@ -4773,7 +4773,7 @@
         <v>2196</v>
       </c>
       <c r="M102" t="n">
-        <v>333468</v>
+        <v>333474</v>
       </c>
     </row>
     <row r="103">
@@ -4816,7 +4816,7 @@
         <v>2212</v>
       </c>
       <c r="M103" t="n">
-        <v>343174</v>
+        <v>343180</v>
       </c>
     </row>
     <row r="104">
@@ -4859,7 +4859,7 @@
         <v>2236</v>
       </c>
       <c r="M104" t="n">
-        <v>349808</v>
+        <v>349814</v>
       </c>
     </row>
     <row r="105">
@@ -4869,10 +4869,10 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>8063</v>
+        <v>8067</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D105" t="n">
         <v>8063</v>
@@ -4902,7 +4902,7 @@
         <v>2253</v>
       </c>
       <c r="M105" t="n">
-        <v>357871</v>
+        <v>357881</v>
       </c>
     </row>
     <row r="106">
@@ -4912,10 +4912,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>9850</v>
+        <v>9854</v>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D106" t="n">
         <v>9850</v>
@@ -4945,7 +4945,7 @@
         <v>2268</v>
       </c>
       <c r="M106" t="n">
-        <v>367721</v>
+        <v>367735</v>
       </c>
     </row>
     <row r="107">
@@ -4955,13 +4955,13 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>10090</v>
+        <v>10089</v>
       </c>
       <c r="C107" t="n">
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>10090</v>
+        <v>10089</v>
       </c>
       <c r="E107" t="n">
         <v>13</v>
@@ -4988,7 +4988,7 @@
         <v>2281</v>
       </c>
       <c r="M107" t="n">
-        <v>377811</v>
+        <v>377824</v>
       </c>
     </row>
     <row r="108">
@@ -5031,7 +5031,7 @@
         <v>2290</v>
       </c>
       <c r="M108" t="n">
-        <v>382748</v>
+        <v>382761</v>
       </c>
     </row>
     <row r="109">
@@ -5074,7 +5074,7 @@
         <v>2311</v>
       </c>
       <c r="M109" t="n">
-        <v>384655</v>
+        <v>384668</v>
       </c>
     </row>
     <row r="110">
@@ -5084,13 +5084,13 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>11387</v>
+        <v>11386</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>11387</v>
+        <v>11386</v>
       </c>
       <c r="E110" t="n">
         <v>13</v>
@@ -5117,7 +5117,7 @@
         <v>2324</v>
       </c>
       <c r="M110" t="n">
-        <v>396042</v>
+        <v>396054</v>
       </c>
     </row>
     <row r="111">
@@ -5160,7 +5160,7 @@
         <v>2337</v>
       </c>
       <c r="M111" t="n">
-        <v>405830</v>
+        <v>405842</v>
       </c>
     </row>
     <row r="112">
@@ -5173,10 +5173,10 @@
         <v>10167</v>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>10166</v>
+        <v>10167</v>
       </c>
       <c r="E112" t="n">
         <v>17</v>
@@ -5203,7 +5203,7 @@
         <v>2354</v>
       </c>
       <c r="M112" t="n">
-        <v>415997</v>
+        <v>416009</v>
       </c>
     </row>
     <row r="113">
@@ -5213,13 +5213,13 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>10126</v>
+        <v>10125</v>
       </c>
       <c r="C113" t="n">
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>10126</v>
+        <v>10125</v>
       </c>
       <c r="E113" t="n">
         <v>23</v>
@@ -5246,7 +5246,7 @@
         <v>2377</v>
       </c>
       <c r="M113" t="n">
-        <v>426123</v>
+        <v>426134</v>
       </c>
     </row>
     <row r="114">
@@ -5256,13 +5256,13 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>10220</v>
+        <v>10219</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>10220</v>
+        <v>10219</v>
       </c>
       <c r="E114" t="n">
         <v>13</v>
@@ -5289,7 +5289,7 @@
         <v>2390</v>
       </c>
       <c r="M114" t="n">
-        <v>436343</v>
+        <v>436353</v>
       </c>
     </row>
     <row r="115">
@@ -5299,13 +5299,13 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>4411</v>
+        <v>4410</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>4411</v>
+        <v>4410</v>
       </c>
       <c r="E115" t="n">
         <v>10</v>
@@ -5332,7 +5332,7 @@
         <v>2400</v>
       </c>
       <c r="M115" t="n">
-        <v>440754</v>
+        <v>440763</v>
       </c>
     </row>
     <row r="116">
@@ -5375,7 +5375,7 @@
         <v>2411</v>
       </c>
       <c r="M116" t="n">
-        <v>442596</v>
+        <v>442605</v>
       </c>
     </row>
     <row r="117">
@@ -5385,13 +5385,13 @@
         </is>
       </c>
       <c r="B117" t="n">
+        <v>10682</v>
+      </c>
+      <c r="C117" t="n">
+        <v>45</v>
+      </c>
+      <c r="D117" t="n">
         <v>10637</v>
-      </c>
-      <c r="C117" t="n">
-        <v>1</v>
-      </c>
-      <c r="D117" t="n">
-        <v>10636</v>
       </c>
       <c r="E117" t="n">
         <v>14</v>
@@ -5418,7 +5418,7 @@
         <v>2425</v>
       </c>
       <c r="M117" t="n">
-        <v>453233</v>
+        <v>453287</v>
       </c>
     </row>
     <row r="118">
@@ -5428,13 +5428,13 @@
         </is>
       </c>
       <c r="B118" t="n">
+        <v>9707</v>
+      </c>
+      <c r="C118" t="n">
+        <v>43</v>
+      </c>
+      <c r="D118" t="n">
         <v>9664</v>
-      </c>
-      <c r="C118" t="n">
-        <v>19</v>
-      </c>
-      <c r="D118" t="n">
-        <v>9645</v>
       </c>
       <c r="E118" t="n">
         <v>5</v>
@@ -5461,7 +5461,7 @@
         <v>2430</v>
       </c>
       <c r="M118" t="n">
-        <v>462897</v>
+        <v>462994</v>
       </c>
     </row>
     <row r="119">
@@ -5471,13 +5471,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>9085</v>
+        <v>9102</v>
       </c>
       <c r="C119" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D119" t="n">
-        <v>9080</v>
+        <v>9084</v>
       </c>
       <c r="E119" t="n">
         <v>10</v>
@@ -5504,7 +5504,7 @@
         <v>2440</v>
       </c>
       <c r="M119" t="n">
-        <v>471982</v>
+        <v>472096</v>
       </c>
     </row>
     <row r="120">
@@ -5514,13 +5514,13 @@
         </is>
       </c>
       <c r="B120" t="n">
+        <v>9359</v>
+      </c>
+      <c r="C120" t="n">
+        <v>52</v>
+      </c>
+      <c r="D120" t="n">
         <v>9307</v>
-      </c>
-      <c r="C120" t="n">
-        <v>3</v>
-      </c>
-      <c r="D120" t="n">
-        <v>9304</v>
       </c>
       <c r="E120" t="n">
         <v>12</v>
@@ -5547,7 +5547,7 @@
         <v>2452</v>
       </c>
       <c r="M120" t="n">
-        <v>481289</v>
+        <v>481455</v>
       </c>
     </row>
     <row r="121">
@@ -5557,10 +5557,10 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>9743</v>
+        <v>9835</v>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D121" t="n">
         <v>9742</v>
@@ -5590,7 +5590,7 @@
         <v>2464</v>
       </c>
       <c r="M121" t="n">
-        <v>491032</v>
+        <v>491290</v>
       </c>
     </row>
     <row r="122">
@@ -5633,7 +5633,7 @@
         <v>2474</v>
       </c>
       <c r="M122" t="n">
-        <v>495084</v>
+        <v>495342</v>
       </c>
     </row>
     <row r="123">
@@ -5676,7 +5676,7 @@
         <v>2484</v>
       </c>
       <c r="M123" t="n">
-        <v>498054</v>
+        <v>498312</v>
       </c>
     </row>
     <row r="124">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>10235</v>
+        <v>10273</v>
       </c>
       <c r="C124" t="n">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D124" t="n">
-        <v>10174</v>
+        <v>10238</v>
       </c>
       <c r="E124" t="n">
         <v>8</v>
@@ -5719,7 +5719,7 @@
         <v>2492</v>
       </c>
       <c r="M124" t="n">
-        <v>508289</v>
+        <v>508585</v>
       </c>
     </row>
     <row r="125">
@@ -5729,13 +5729,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>8772</v>
+        <v>8915</v>
       </c>
       <c r="C125" t="n">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="D125" t="n">
-        <v>8724</v>
+        <v>8767</v>
       </c>
       <c r="E125" t="n">
         <v>7</v>
@@ -5762,7 +5762,7 @@
         <v>2499</v>
       </c>
       <c r="M125" t="n">
-        <v>517061</v>
+        <v>517500</v>
       </c>
     </row>
     <row r="126">
@@ -5772,13 +5772,13 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>7851</v>
+        <v>7990</v>
       </c>
       <c r="C126" t="n">
-        <v>28</v>
+        <v>142</v>
       </c>
       <c r="D126" t="n">
-        <v>7823</v>
+        <v>7848</v>
       </c>
       <c r="E126" t="n">
         <v>11</v>
@@ -5805,7 +5805,7 @@
         <v>2510</v>
       </c>
       <c r="M126" t="n">
-        <v>524912</v>
+        <v>525490</v>
       </c>
     </row>
     <row r="127">
@@ -5815,13 +5815,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>9039</v>
+        <v>9081</v>
       </c>
       <c r="C127" t="n">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D127" t="n">
-        <v>9031</v>
+        <v>9038</v>
       </c>
       <c r="E127" t="n">
         <v>8</v>
@@ -5848,7 +5848,7 @@
         <v>2518</v>
       </c>
       <c r="M127" t="n">
-        <v>533951</v>
+        <v>534571</v>
       </c>
     </row>
     <row r="128">
@@ -5858,13 +5858,13 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>5151</v>
+        <v>5214</v>
       </c>
       <c r="C128" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D128" t="n">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="E128" t="n">
         <v>9</v>
@@ -5891,7 +5891,7 @@
         <v>2527</v>
       </c>
       <c r="M128" t="n">
-        <v>539102</v>
+        <v>539785</v>
       </c>
     </row>
     <row r="129">
@@ -5934,7 +5934,7 @@
         <v>2535</v>
       </c>
       <c r="M129" t="n">
-        <v>541194</v>
+        <v>541877</v>
       </c>
     </row>
     <row r="130">
@@ -5977,7 +5977,7 @@
         <v>2546</v>
       </c>
       <c r="M130" t="n">
-        <v>543901</v>
+        <v>544584</v>
       </c>
     </row>
     <row r="131">
@@ -5987,13 +5987,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>11228</v>
+        <v>11264</v>
       </c>
       <c r="C131" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D131" t="n">
-        <v>11226</v>
+        <v>11230</v>
       </c>
       <c r="E131" t="n">
         <v>14</v>
@@ -6020,7 +6020,7 @@
         <v>2560</v>
       </c>
       <c r="M131" t="n">
-        <v>555129</v>
+        <v>555848</v>
       </c>
     </row>
     <row r="132">
@@ -6030,13 +6030,13 @@
         </is>
       </c>
       <c r="B132" t="n">
+        <v>9845</v>
+      </c>
+      <c r="C132" t="n">
+        <v>20</v>
+      </c>
+      <c r="D132" t="n">
         <v>9825</v>
-      </c>
-      <c r="C132" t="n">
-        <v>3</v>
-      </c>
-      <c r="D132" t="n">
-        <v>9822</v>
       </c>
       <c r="E132" t="n">
         <v>6</v>
@@ -6063,7 +6063,7 @@
         <v>2566</v>
       </c>
       <c r="M132" t="n">
-        <v>564954</v>
+        <v>565693</v>
       </c>
     </row>
     <row r="133">
@@ -6073,13 +6073,13 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>8832</v>
+        <v>8996</v>
       </c>
       <c r="C133" t="n">
-        <v>3</v>
+        <v>163</v>
       </c>
       <c r="D133" t="n">
-        <v>8829</v>
+        <v>8833</v>
       </c>
       <c r="E133" t="n">
         <v>8</v>
@@ -6106,7 +6106,7 @@
         <v>2574</v>
       </c>
       <c r="M133" t="n">
-        <v>573786</v>
+        <v>574689</v>
       </c>
     </row>
     <row r="134">
@@ -6116,13 +6116,13 @@
         </is>
       </c>
       <c r="B134" t="n">
+        <v>8942</v>
+      </c>
+      <c r="C134" t="n">
+        <v>255</v>
+      </c>
+      <c r="D134" t="n">
         <v>8687</v>
-      </c>
-      <c r="C134" t="n">
-        <v>9</v>
-      </c>
-      <c r="D134" t="n">
-        <v>8678</v>
       </c>
       <c r="E134" t="n">
         <v>10</v>
@@ -6149,7 +6149,7 @@
         <v>2584</v>
       </c>
       <c r="M134" t="n">
-        <v>582473</v>
+        <v>583631</v>
       </c>
     </row>
     <row r="135">
@@ -6159,13 +6159,13 @@
         </is>
       </c>
       <c r="B135" t="n">
+        <v>10251</v>
+      </c>
+      <c r="C135" t="n">
+        <v>226</v>
+      </c>
+      <c r="D135" t="n">
         <v>10025</v>
-      </c>
-      <c r="C135" t="n">
-        <v>9</v>
-      </c>
-      <c r="D135" t="n">
-        <v>10016</v>
       </c>
       <c r="E135" t="n">
         <v>7</v>
@@ -6192,7 +6192,7 @@
         <v>2591</v>
       </c>
       <c r="M135" t="n">
-        <v>592498</v>
+        <v>593882</v>
       </c>
     </row>
     <row r="136">
@@ -6202,13 +6202,13 @@
         </is>
       </c>
       <c r="B136" t="n">
+        <v>4820</v>
+      </c>
+      <c r="C136" t="n">
+        <v>133</v>
+      </c>
+      <c r="D136" t="n">
         <v>4687</v>
-      </c>
-      <c r="C136" t="n">
-        <v>5</v>
-      </c>
-      <c r="D136" t="n">
-        <v>4682</v>
       </c>
       <c r="E136" t="n">
         <v>8</v>
@@ -6235,7 +6235,7 @@
         <v>2599</v>
       </c>
       <c r="M136" t="n">
-        <v>597185</v>
+        <v>598702</v>
       </c>
     </row>
     <row r="137">
@@ -6245,13 +6245,13 @@
         </is>
       </c>
       <c r="B137" t="n">
+        <v>3480</v>
+      </c>
+      <c r="C137" t="n">
+        <v>25</v>
+      </c>
+      <c r="D137" t="n">
         <v>3455</v>
-      </c>
-      <c r="C137" t="n">
-        <v>8</v>
-      </c>
-      <c r="D137" t="n">
-        <v>3447</v>
       </c>
       <c r="E137" t="n">
         <v>13</v>
@@ -6278,7 +6278,7 @@
         <v>2612</v>
       </c>
       <c r="M137" t="n">
-        <v>600640</v>
+        <v>602182</v>
       </c>
     </row>
     <row r="138">
@@ -6288,13 +6288,13 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>12256</v>
+        <v>12336</v>
       </c>
       <c r="C138" t="n">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="D138" t="n">
-        <v>12201</v>
+        <v>12250</v>
       </c>
       <c r="E138" t="n">
         <v>9</v>
@@ -6321,7 +6321,7 @@
         <v>2621</v>
       </c>
       <c r="M138" t="n">
-        <v>612896</v>
+        <v>614518</v>
       </c>
     </row>
     <row r="139">
@@ -6331,13 +6331,13 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>11490</v>
+        <v>11669</v>
       </c>
       <c r="C139" t="n">
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="D139" t="n">
-        <v>11473</v>
+        <v>11489</v>
       </c>
       <c r="E139" t="n">
         <v>5</v>
@@ -6364,7 +6364,7 @@
         <v>2626</v>
       </c>
       <c r="M139" t="n">
-        <v>624386</v>
+        <v>626187</v>
       </c>
     </row>
     <row r="140">
@@ -6374,13 +6374,13 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>10994</v>
+        <v>11218</v>
       </c>
       <c r="C140" t="n">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="D140" t="n">
-        <v>10982</v>
+        <v>10992</v>
       </c>
       <c r="E140" t="n">
         <v>10</v>
@@ -6407,7 +6407,7 @@
         <v>2636</v>
       </c>
       <c r="M140" t="n">
-        <v>635380</v>
+        <v>637405</v>
       </c>
     </row>
     <row r="141">
@@ -6417,13 +6417,13 @@
         </is>
       </c>
       <c r="B141" t="n">
+        <v>12769</v>
+      </c>
+      <c r="C141" t="n">
+        <v>282</v>
+      </c>
+      <c r="D141" t="n">
         <v>12487</v>
-      </c>
-      <c r="C141" t="n">
-        <v>4</v>
-      </c>
-      <c r="D141" t="n">
-        <v>12483</v>
       </c>
       <c r="E141" t="n">
         <v>9</v>
@@ -6450,7 +6450,7 @@
         <v>2645</v>
       </c>
       <c r="M141" t="n">
-        <v>647867</v>
+        <v>650174</v>
       </c>
     </row>
     <row r="142">
@@ -6460,13 +6460,13 @@
         </is>
       </c>
       <c r="B142" t="n">
+        <v>13112</v>
+      </c>
+      <c r="C142" t="n">
+        <v>182</v>
+      </c>
+      <c r="D142" t="n">
         <v>12930</v>
-      </c>
-      <c r="C142" t="n">
-        <v>7</v>
-      </c>
-      <c r="D142" t="n">
-        <v>12923</v>
       </c>
       <c r="E142" t="n">
         <v>9</v>
@@ -6493,7 +6493,7 @@
         <v>2654</v>
       </c>
       <c r="M142" t="n">
-        <v>660797</v>
+        <v>663286</v>
       </c>
     </row>
     <row r="143">
@@ -6503,13 +6503,13 @@
         </is>
       </c>
       <c r="B143" t="n">
+        <v>5541</v>
+      </c>
+      <c r="C143" t="n">
+        <v>47</v>
+      </c>
+      <c r="D143" t="n">
         <v>5494</v>
-      </c>
-      <c r="C143" t="n">
-        <v>3</v>
-      </c>
-      <c r="D143" t="n">
-        <v>5491</v>
       </c>
       <c r="E143" t="n">
         <v>6</v>
@@ -6536,7 +6536,7 @@
         <v>2660</v>
       </c>
       <c r="M143" t="n">
-        <v>666291</v>
+        <v>668827</v>
       </c>
     </row>
     <row r="144">
@@ -6546,10 +6546,10 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>3067</v>
+        <v>3070</v>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D144" t="n">
         <v>3067</v>
@@ -6579,7 +6579,7 @@
         <v>2668</v>
       </c>
       <c r="M144" t="n">
-        <v>669358</v>
+        <v>671897</v>
       </c>
     </row>
     <row r="145">
@@ -6589,13 +6589,13 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>12884</v>
+        <v>12886</v>
       </c>
       <c r="C145" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D145" t="n">
-        <v>12864</v>
+        <v>12880</v>
       </c>
       <c r="E145" t="n">
         <v>13</v>
@@ -6622,7 +6622,7 @@
         <v>2681</v>
       </c>
       <c r="M145" t="n">
-        <v>682242</v>
+        <v>684783</v>
       </c>
     </row>
     <row r="146">
@@ -6632,13 +6632,13 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>12496</v>
+        <v>12499</v>
       </c>
       <c r="C146" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D146" t="n">
-        <v>12466</v>
+        <v>12495</v>
       </c>
       <c r="E146" t="n">
         <v>9</v>
@@ -6665,7 +6665,7 @@
         <v>2690</v>
       </c>
       <c r="M146" t="n">
-        <v>694738</v>
+        <v>697282</v>
       </c>
     </row>
     <row r="147">
@@ -6675,13 +6675,13 @@
         </is>
       </c>
       <c r="B147" t="n">
+        <v>11918</v>
+      </c>
+      <c r="C147" t="n">
+        <v>46</v>
+      </c>
+      <c r="D147" t="n">
         <v>11872</v>
-      </c>
-      <c r="C147" t="n">
-        <v>12</v>
-      </c>
-      <c r="D147" t="n">
-        <v>11860</v>
       </c>
       <c r="E147" t="n">
         <v>12</v>
@@ -6708,7 +6708,7 @@
         <v>2702</v>
       </c>
       <c r="M147" t="n">
-        <v>706610</v>
+        <v>709200</v>
       </c>
     </row>
     <row r="148">
@@ -6718,13 +6718,13 @@
         </is>
       </c>
       <c r="B148" t="n">
+        <v>11946</v>
+      </c>
+      <c r="C148" t="n">
+        <v>47</v>
+      </c>
+      <c r="D148" t="n">
         <v>11899</v>
-      </c>
-      <c r="C148" t="n">
-        <v>38</v>
-      </c>
-      <c r="D148" t="n">
-        <v>11861</v>
       </c>
       <c r="E148" t="n">
         <v>10</v>
@@ -6751,7 +6751,7 @@
         <v>2712</v>
       </c>
       <c r="M148" t="n">
-        <v>718509</v>
+        <v>721146</v>
       </c>
     </row>
     <row r="149">
@@ -6761,13 +6761,13 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>12083</v>
+        <v>12112</v>
       </c>
       <c r="C149" t="n">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="D149" t="n">
-        <v>11994</v>
+        <v>12082</v>
       </c>
       <c r="E149" t="n">
         <v>9</v>
@@ -6794,7 +6794,7 @@
         <v>2721</v>
       </c>
       <c r="M149" t="n">
-        <v>730592</v>
+        <v>733258</v>
       </c>
     </row>
     <row r="150">
@@ -6804,13 +6804,13 @@
         </is>
       </c>
       <c r="B150" t="n">
+        <v>4885</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1</v>
+      </c>
+      <c r="D150" t="n">
         <v>4884</v>
-      </c>
-      <c r="C150" t="n">
-        <v>90</v>
-      </c>
-      <c r="D150" t="n">
-        <v>4794</v>
       </c>
       <c r="E150" t="n">
         <v>8</v>
@@ -6837,7 +6837,7 @@
         <v>2729</v>
       </c>
       <c r="M150" t="n">
-        <v>735476</v>
+        <v>738143</v>
       </c>
     </row>
     <row r="151">
@@ -6850,10 +6850,10 @@
         <v>2466</v>
       </c>
       <c r="C151" t="n">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>2344</v>
+        <v>2466</v>
       </c>
       <c r="E151" t="n">
         <v>8</v>
@@ -6880,7 +6880,7 @@
         <v>2737</v>
       </c>
       <c r="M151" t="n">
-        <v>737942</v>
+        <v>740609</v>
       </c>
     </row>
     <row r="152">
@@ -6890,13 +6890,13 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>12135</v>
+        <v>12133</v>
       </c>
       <c r="C152" t="n">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D152" t="n">
-        <v>12098</v>
+        <v>12127</v>
       </c>
       <c r="E152" t="n">
         <v>4</v>
@@ -6923,7 +6923,7 @@
         <v>2741</v>
       </c>
       <c r="M152" t="n">
-        <v>750077</v>
+        <v>752742</v>
       </c>
     </row>
     <row r="153">
@@ -6933,13 +6933,13 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>12016</v>
+        <v>12041</v>
       </c>
       <c r="C153" t="n">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D153" t="n">
-        <v>11917</v>
+        <v>12011</v>
       </c>
       <c r="E153" t="n">
         <v>6</v>
@@ -6966,7 +6966,7 @@
         <v>2747</v>
       </c>
       <c r="M153" t="n">
-        <v>762093</v>
+        <v>764783</v>
       </c>
     </row>
     <row r="154">
@@ -6976,13 +6976,13 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>10706</v>
+        <v>10744</v>
       </c>
       <c r="C154" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D154" t="n">
-        <v>10662</v>
+        <v>10704</v>
       </c>
       <c r="E154" t="n">
         <v>19</v>
@@ -7009,7 +7009,7 @@
         <v>2766</v>
       </c>
       <c r="M154" t="n">
-        <v>772799</v>
+        <v>775527</v>
       </c>
     </row>
     <row r="155">
@@ -7019,13 +7019,13 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>10428</v>
+        <v>10430</v>
       </c>
       <c r="C155" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D155" t="n">
-        <v>10393</v>
+        <v>10421</v>
       </c>
       <c r="E155" t="n">
         <v>9</v>
@@ -7052,7 +7052,7 @@
         <v>2775</v>
       </c>
       <c r="M155" t="n">
-        <v>783227</v>
+        <v>785957</v>
       </c>
     </row>
     <row r="156">
@@ -7062,13 +7062,13 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>11164</v>
+        <v>11241</v>
       </c>
       <c r="C156" t="n">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D156" t="n">
-        <v>11125</v>
+        <v>11163</v>
       </c>
       <c r="E156" t="n">
         <v>8</v>
@@ -7095,7 +7095,7 @@
         <v>2783</v>
       </c>
       <c r="M156" t="n">
-        <v>794391</v>
+        <v>797198</v>
       </c>
     </row>
     <row r="157">
@@ -7105,13 +7105,13 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>4227</v>
+        <v>4433</v>
       </c>
       <c r="C157" t="n">
-        <v>111</v>
+        <v>199</v>
       </c>
       <c r="D157" t="n">
-        <v>4116</v>
+        <v>4234</v>
       </c>
       <c r="E157" t="n">
         <v>10</v>
@@ -7138,7 +7138,7 @@
         <v>2793</v>
       </c>
       <c r="M157" t="n">
-        <v>798618</v>
+        <v>801631</v>
       </c>
     </row>
     <row r="158">
@@ -7148,13 +7148,13 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>2408</v>
+        <v>2443</v>
       </c>
       <c r="C158" t="n">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="D158" t="n">
-        <v>2317</v>
+        <v>2411</v>
       </c>
       <c r="E158" t="n">
         <v>9</v>
@@ -7181,7 +7181,7 @@
         <v>2802</v>
       </c>
       <c r="M158" t="n">
-        <v>801026</v>
+        <v>804074</v>
       </c>
     </row>
     <row r="159">
@@ -7191,13 +7191,13 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>11197</v>
+        <v>11558</v>
       </c>
       <c r="C159" t="n">
-        <v>496</v>
+        <v>363</v>
       </c>
       <c r="D159" t="n">
-        <v>10701</v>
+        <v>11195</v>
       </c>
       <c r="E159" t="n">
         <v>7</v>
@@ -7224,7 +7224,7 @@
         <v>2809</v>
       </c>
       <c r="M159" t="n">
-        <v>812223</v>
+        <v>815632</v>
       </c>
     </row>
     <row r="160">
@@ -7234,13 +7234,13 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>10594</v>
+        <v>10857</v>
       </c>
       <c r="C160" t="n">
-        <v>1053</v>
+        <v>276</v>
       </c>
       <c r="D160" t="n">
-        <v>9541</v>
+        <v>10581</v>
       </c>
       <c r="E160" t="n">
         <v>7</v>
@@ -7267,7 +7267,7 @@
         <v>2816</v>
       </c>
       <c r="M160" t="n">
-        <v>822817</v>
+        <v>826489</v>
       </c>
     </row>
     <row r="161">
@@ -7277,13 +7277,13 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>9064</v>
+        <v>9722</v>
       </c>
       <c r="C161" t="n">
-        <v>2350</v>
+        <v>665</v>
       </c>
       <c r="D161" t="n">
-        <v>6714</v>
+        <v>9057</v>
       </c>
       <c r="E161" t="n">
         <v>3</v>
@@ -7310,7 +7310,7 @@
         <v>2819</v>
       </c>
       <c r="M161" t="n">
-        <v>831881</v>
+        <v>836211</v>
       </c>
     </row>
     <row r="162">
@@ -7320,13 +7320,13 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>7695</v>
+        <v>9300</v>
       </c>
       <c r="C162" t="n">
-        <v>6244</v>
+        <v>1686</v>
       </c>
       <c r="D162" t="n">
-        <v>1451</v>
+        <v>7614</v>
       </c>
       <c r="E162" t="n">
         <v>9</v>
@@ -7338,22 +7338,22 @@
         <v>9</v>
       </c>
       <c r="H162" t="n">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="I162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J162" t="n">
         <v>1251</v>
       </c>
       <c r="K162" t="n">
-        <v>72254</v>
+        <v>72253</v>
       </c>
       <c r="L162" t="n">
         <v>2828</v>
       </c>
       <c r="M162" t="n">
-        <v>839576</v>
+        <v>845511</v>
       </c>
     </row>
     <row r="163">
@@ -7363,40 +7363,40 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>1389</v>
+        <v>5382</v>
       </c>
       <c r="C163" t="n">
-        <v>1291</v>
+        <v>4009</v>
       </c>
       <c r="D163" t="n">
-        <v>98</v>
+        <v>1373</v>
       </c>
       <c r="E163" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G163" t="n">
         <v>6</v>
       </c>
       <c r="H163" t="n">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J163" t="n">
         <v>1027</v>
       </c>
       <c r="K163" t="n">
-        <v>73282</v>
+        <v>73280</v>
       </c>
       <c r="L163" t="n">
-        <v>2834</v>
+        <v>2835</v>
       </c>
       <c r="M163" t="n">
-        <v>840965</v>
+        <v>850893</v>
       </c>
     </row>
     <row r="164">
@@ -7406,40 +7406,83 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>160</v>
+        <v>1115</v>
       </c>
       <c r="C164" t="n">
-        <v>160</v>
+        <v>956</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="E164" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F164" t="n">
         <v>1</v>
       </c>
       <c r="G164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H164" t="n">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="I164" t="n">
-        <v>1046</v>
+        <v>0</v>
       </c>
       <c r="J164" t="n">
-        <v>0</v>
+        <v>1039</v>
       </c>
       <c r="K164" t="n">
-        <v>74328</v>
+        <v>74319</v>
       </c>
       <c r="L164" t="n">
-        <v>2835</v>
+        <v>2837</v>
       </c>
       <c r="M164" t="n">
-        <v>841125</v>
+        <v>852008</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2020-08-09</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>103</v>
+      </c>
+      <c r="C165" t="n">
+        <v>103</v>
+      </c>
+      <c r="D165" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1</v>
+      </c>
+      <c r="G165" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" t="n">
+        <v>673</v>
+      </c>
+      <c r="I165" t="n">
+        <v>673</v>
+      </c>
+      <c r="J165" t="n">
+        <v>0</v>
+      </c>
+      <c r="K165" t="n">
+        <v>74992</v>
+      </c>
+      <c r="L165" t="n">
+        <v>2838</v>
+      </c>
+      <c r="M165" t="n">
+        <v>852111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding process-demog-data script and associates
</commit_message>
<xml_diff>
--- a/data/test-case-trend.xlsx
+++ b/data/test-case-trend.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:M167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2120,10 +2120,10 @@
         <v>2798</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="E41" t="n">
         <v>36</v>
@@ -3192,13 +3192,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3336</v>
+        <v>3335</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>3336</v>
+        <v>3335</v>
       </c>
       <c r="E66" t="n">
         <v>44</v>
@@ -3225,7 +3225,7 @@
         <v>1234</v>
       </c>
       <c r="M66" t="n">
-        <v>129772</v>
+        <v>129771</v>
       </c>
     </row>
     <row r="67">
@@ -3268,7 +3268,7 @@
         <v>1266</v>
       </c>
       <c r="M67" t="n">
-        <v>131613</v>
+        <v>131612</v>
       </c>
     </row>
     <row r="68">
@@ -3311,7 +3311,7 @@
         <v>1304</v>
       </c>
       <c r="M68" t="n">
-        <v>137474</v>
+        <v>137473</v>
       </c>
     </row>
     <row r="69">
@@ -3321,13 +3321,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>6615</v>
+        <v>6614</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>6615</v>
+        <v>6614</v>
       </c>
       <c r="E69" t="n">
         <v>38</v>
@@ -3354,7 +3354,7 @@
         <v>1342</v>
       </c>
       <c r="M69" t="n">
-        <v>144089</v>
+        <v>144087</v>
       </c>
     </row>
     <row r="70">
@@ -3367,10 +3367,10 @@
         <v>6043</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>6043</v>
+        <v>6042</v>
       </c>
       <c r="E70" t="n">
         <v>43</v>
@@ -3397,7 +3397,7 @@
         <v>1385</v>
       </c>
       <c r="M70" t="n">
-        <v>150132</v>
+        <v>150130</v>
       </c>
     </row>
     <row r="71">
@@ -3407,13 +3407,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>6704</v>
+        <v>6703</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>6704</v>
+        <v>6703</v>
       </c>
       <c r="E71" t="n">
         <v>34</v>
@@ -3440,7 +3440,7 @@
         <v>1419</v>
       </c>
       <c r="M71" t="n">
-        <v>156836</v>
+        <v>156833</v>
       </c>
     </row>
     <row r="72">
@@ -3483,7 +3483,7 @@
         <v>1444</v>
       </c>
       <c r="M72" t="n">
-        <v>163587</v>
+        <v>163584</v>
       </c>
     </row>
     <row r="73">
@@ -3526,7 +3526,7 @@
         <v>1476</v>
       </c>
       <c r="M73" t="n">
-        <v>166944</v>
+        <v>166941</v>
       </c>
     </row>
     <row r="74">
@@ -3569,7 +3569,7 @@
         <v>1510</v>
       </c>
       <c r="M74" t="n">
-        <v>168269</v>
+        <v>168266</v>
       </c>
     </row>
     <row r="75">
@@ -3612,7 +3612,7 @@
         <v>1551</v>
       </c>
       <c r="M75" t="n">
-        <v>175492</v>
+        <v>175489</v>
       </c>
     </row>
     <row r="76">
@@ -3622,13 +3622,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>7059</v>
+        <v>7001</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>7059</v>
+        <v>6999</v>
       </c>
       <c r="E76" t="n">
         <v>38</v>
@@ -3655,7 +3655,7 @@
         <v>1589</v>
       </c>
       <c r="M76" t="n">
-        <v>182551</v>
+        <v>182490</v>
       </c>
     </row>
     <row r="77">
@@ -3665,13 +3665,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>7302</v>
+        <v>7296</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>7301</v>
+        <v>7296</v>
       </c>
       <c r="E77" t="n">
         <v>27</v>
@@ -3698,7 +3698,7 @@
         <v>1616</v>
       </c>
       <c r="M77" t="n">
-        <v>189853</v>
+        <v>189786</v>
       </c>
     </row>
     <row r="78">
@@ -3708,13 +3708,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>8195</v>
+        <v>8157</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>8195</v>
+        <v>8157</v>
       </c>
       <c r="E78" t="n">
         <v>42</v>
@@ -3741,7 +3741,7 @@
         <v>1658</v>
       </c>
       <c r="M78" t="n">
-        <v>198048</v>
+        <v>197943</v>
       </c>
     </row>
     <row r="79">
@@ -3751,13 +3751,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>9787</v>
+        <v>9774</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>9787</v>
+        <v>9774</v>
       </c>
       <c r="E79" t="n">
         <v>32</v>
@@ -3784,7 +3784,7 @@
         <v>1690</v>
       </c>
       <c r="M79" t="n">
-        <v>207835</v>
+        <v>207717</v>
       </c>
     </row>
     <row r="80">
@@ -3794,13 +3794,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3193</v>
+        <v>3177</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>3193</v>
+        <v>3177</v>
       </c>
       <c r="E80" t="n">
         <v>28</v>
@@ -3827,7 +3827,7 @@
         <v>1718</v>
       </c>
       <c r="M80" t="n">
-        <v>211028</v>
+        <v>210894</v>
       </c>
     </row>
     <row r="81">
@@ -3870,7 +3870,7 @@
         <v>1748</v>
       </c>
       <c r="M81" t="n">
-        <v>212959</v>
+        <v>212825</v>
       </c>
     </row>
     <row r="82">
@@ -3880,13 +3880,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>8396</v>
+        <v>8390</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>8396</v>
+        <v>8390</v>
       </c>
       <c r="E82" t="n">
         <v>39</v>
@@ -3913,7 +3913,7 @@
         <v>1787</v>
       </c>
       <c r="M82" t="n">
-        <v>221355</v>
+        <v>221215</v>
       </c>
     </row>
     <row r="83">
@@ -3923,13 +3923,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>7134</v>
+        <v>7121</v>
       </c>
       <c r="C83" t="n">
         <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>7134</v>
+        <v>7121</v>
       </c>
       <c r="E83" t="n">
         <v>29</v>
@@ -3956,7 +3956,7 @@
         <v>1816</v>
       </c>
       <c r="M83" t="n">
-        <v>228489</v>
+        <v>228336</v>
       </c>
     </row>
     <row r="84">
@@ -3966,13 +3966,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>6794</v>
+        <v>6792</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>6794</v>
+        <v>6792</v>
       </c>
       <c r="E84" t="n">
         <v>31</v>
@@ -3999,7 +3999,7 @@
         <v>1847</v>
       </c>
       <c r="M84" t="n">
-        <v>235283</v>
+        <v>235128</v>
       </c>
     </row>
     <row r="85">
@@ -4009,13 +4009,13 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>7709</v>
+        <v>7687</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>7709</v>
+        <v>7687</v>
       </c>
       <c r="E85" t="n">
         <v>37</v>
@@ -4042,7 +4042,7 @@
         <v>1884</v>
       </c>
       <c r="M85" t="n">
-        <v>242992</v>
+        <v>242815</v>
       </c>
     </row>
     <row r="86">
@@ -4052,13 +4052,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>8354</v>
+        <v>8343</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>8354</v>
+        <v>8343</v>
       </c>
       <c r="E86" t="n">
         <v>18</v>
@@ -4085,7 +4085,7 @@
         <v>1902</v>
       </c>
       <c r="M86" t="n">
-        <v>251346</v>
+        <v>251158</v>
       </c>
     </row>
     <row r="87">
@@ -4128,7 +4128,7 @@
         <v>1926</v>
       </c>
       <c r="M87" t="n">
-        <v>254203</v>
+        <v>254015</v>
       </c>
     </row>
     <row r="88">
@@ -4138,13 +4138,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E88" t="n">
         <v>15</v>
@@ -4171,7 +4171,7 @@
         <v>1941</v>
       </c>
       <c r="M88" t="n">
-        <v>256080</v>
+        <v>255891</v>
       </c>
     </row>
     <row r="89">
@@ -4214,7 +4214,7 @@
         <v>1962</v>
       </c>
       <c r="M89" t="n">
-        <v>257906</v>
+        <v>257717</v>
       </c>
     </row>
     <row r="90">
@@ -4224,13 +4224,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>8000</v>
+        <v>7996</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>8000</v>
+        <v>7996</v>
       </c>
       <c r="E90" t="n">
         <v>19</v>
@@ -4257,7 +4257,7 @@
         <v>1981</v>
       </c>
       <c r="M90" t="n">
-        <v>265906</v>
+        <v>265713</v>
       </c>
     </row>
     <row r="91">
@@ -4267,13 +4267,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>6533</v>
+        <v>6518</v>
       </c>
       <c r="C91" t="n">
         <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>6533</v>
+        <v>6518</v>
       </c>
       <c r="E91" t="n">
         <v>14</v>
@@ -4300,7 +4300,7 @@
         <v>1995</v>
       </c>
       <c r="M91" t="n">
-        <v>272439</v>
+        <v>272231</v>
       </c>
     </row>
     <row r="92">
@@ -4310,13 +4310,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>7193</v>
+        <v>7189</v>
       </c>
       <c r="C92" t="n">
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>7193</v>
+        <v>7189</v>
       </c>
       <c r="E92" t="n">
         <v>18</v>
@@ -4343,7 +4343,7 @@
         <v>2013</v>
       </c>
       <c r="M92" t="n">
-        <v>279632</v>
+        <v>279420</v>
       </c>
     </row>
     <row r="93">
@@ -4353,13 +4353,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>7832</v>
+        <v>7825</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>7832</v>
+        <v>7825</v>
       </c>
       <c r="E93" t="n">
         <v>21</v>
@@ -4386,7 +4386,7 @@
         <v>2034</v>
       </c>
       <c r="M93" t="n">
-        <v>287464</v>
+        <v>287245</v>
       </c>
     </row>
     <row r="94">
@@ -4396,13 +4396,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="E94" t="n">
         <v>21</v>
@@ -4429,7 +4429,7 @@
         <v>2055</v>
       </c>
       <c r="M94" t="n">
-        <v>290358</v>
+        <v>290138</v>
       </c>
     </row>
     <row r="95">
@@ -4472,7 +4472,7 @@
         <v>2071</v>
       </c>
       <c r="M95" t="n">
-        <v>292181</v>
+        <v>291961</v>
       </c>
     </row>
     <row r="96">
@@ -4482,13 +4482,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>8138</v>
+        <v>8134</v>
       </c>
       <c r="C96" t="n">
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>8138</v>
+        <v>8134</v>
       </c>
       <c r="E96" t="n">
         <v>20</v>
@@ -4515,7 +4515,7 @@
         <v>2091</v>
       </c>
       <c r="M96" t="n">
-        <v>300319</v>
+        <v>300095</v>
       </c>
     </row>
     <row r="97">
@@ -4525,13 +4525,13 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>5725</v>
+        <v>5721</v>
       </c>
       <c r="C97" t="n">
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>5725</v>
+        <v>5721</v>
       </c>
       <c r="E97" t="n">
         <v>15</v>
@@ -4558,7 +4558,7 @@
         <v>2106</v>
       </c>
       <c r="M97" t="n">
-        <v>306044</v>
+        <v>305816</v>
       </c>
     </row>
     <row r="98">
@@ -4568,13 +4568,13 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6774</v>
+        <v>6762</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>6774</v>
+        <v>6762</v>
       </c>
       <c r="E98" t="n">
         <v>24</v>
@@ -4601,7 +4601,7 @@
         <v>2130</v>
       </c>
       <c r="M98" t="n">
-        <v>312818</v>
+        <v>312578</v>
       </c>
     </row>
     <row r="99">
@@ -4611,10 +4611,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>6983</v>
+        <v>6982</v>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
         <v>6982</v>
@@ -4644,7 +4644,7 @@
         <v>2152</v>
       </c>
       <c r="M99" t="n">
-        <v>319801</v>
+        <v>319560</v>
       </c>
     </row>
     <row r="100">
@@ -4654,13 +4654,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>7948</v>
+        <v>7944</v>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>7947</v>
+        <v>7944</v>
       </c>
       <c r="E100" t="n">
         <v>21</v>
@@ -4687,7 +4687,7 @@
         <v>2173</v>
       </c>
       <c r="M100" t="n">
-        <v>327749</v>
+        <v>327504</v>
       </c>
     </row>
     <row r="101">
@@ -4730,7 +4730,7 @@
         <v>2181</v>
       </c>
       <c r="M101" t="n">
-        <v>331467</v>
+        <v>331222</v>
       </c>
     </row>
     <row r="102">
@@ -4773,7 +4773,7 @@
         <v>2196</v>
       </c>
       <c r="M102" t="n">
-        <v>333461</v>
+        <v>333216</v>
       </c>
     </row>
     <row r="103">
@@ -4783,13 +4783,13 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>9706</v>
+        <v>9705</v>
       </c>
       <c r="C103" t="n">
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>9706</v>
+        <v>9705</v>
       </c>
       <c r="E103" t="n">
         <v>16</v>
@@ -4816,7 +4816,7 @@
         <v>2212</v>
       </c>
       <c r="M103" t="n">
-        <v>343167</v>
+        <v>342921</v>
       </c>
     </row>
     <row r="104">
@@ -4859,7 +4859,7 @@
         <v>2236</v>
       </c>
       <c r="M104" t="n">
-        <v>349801</v>
+        <v>349555</v>
       </c>
     </row>
     <row r="105">
@@ -4902,7 +4902,7 @@
         <v>2253</v>
       </c>
       <c r="M105" t="n">
-        <v>357868</v>
+        <v>357622</v>
       </c>
     </row>
     <row r="106">
@@ -4945,7 +4945,7 @@
         <v>2268</v>
       </c>
       <c r="M106" t="n">
-        <v>367722</v>
+        <v>367476</v>
       </c>
     </row>
     <row r="107">
@@ -4988,7 +4988,7 @@
         <v>2281</v>
       </c>
       <c r="M107" t="n">
-        <v>377811</v>
+        <v>377565</v>
       </c>
     </row>
     <row r="108">
@@ -5031,7 +5031,7 @@
         <v>2290</v>
       </c>
       <c r="M108" t="n">
-        <v>382748</v>
+        <v>382502</v>
       </c>
     </row>
     <row r="109">
@@ -5074,7 +5074,7 @@
         <v>2311</v>
       </c>
       <c r="M109" t="n">
-        <v>384655</v>
+        <v>384409</v>
       </c>
     </row>
     <row r="110">
@@ -5117,7 +5117,7 @@
         <v>2324</v>
       </c>
       <c r="M110" t="n">
-        <v>396041</v>
+        <v>395795</v>
       </c>
     </row>
     <row r="111">
@@ -5127,13 +5127,13 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>9788</v>
+        <v>9785</v>
       </c>
       <c r="C111" t="n">
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>9788</v>
+        <v>9785</v>
       </c>
       <c r="E111" t="n">
         <v>13</v>
@@ -5160,7 +5160,7 @@
         <v>2337</v>
       </c>
       <c r="M111" t="n">
-        <v>405829</v>
+        <v>405580</v>
       </c>
     </row>
     <row r="112">
@@ -5170,13 +5170,13 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>10168</v>
+        <v>10166</v>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>10167</v>
+        <v>10166</v>
       </c>
       <c r="E112" t="n">
         <v>17</v>
@@ -5203,7 +5203,7 @@
         <v>2354</v>
       </c>
       <c r="M112" t="n">
-        <v>415997</v>
+        <v>415746</v>
       </c>
     </row>
     <row r="113">
@@ -5246,7 +5246,7 @@
         <v>2377</v>
       </c>
       <c r="M113" t="n">
-        <v>426122</v>
+        <v>425871</v>
       </c>
     </row>
     <row r="114">
@@ -5289,7 +5289,7 @@
         <v>2390</v>
       </c>
       <c r="M114" t="n">
-        <v>436340</v>
+        <v>436089</v>
       </c>
     </row>
     <row r="115">
@@ -5332,7 +5332,7 @@
         <v>2400</v>
       </c>
       <c r="M115" t="n">
-        <v>440750</v>
+        <v>440499</v>
       </c>
     </row>
     <row r="116">
@@ -5375,7 +5375,7 @@
         <v>2411</v>
       </c>
       <c r="M116" t="n">
-        <v>442592</v>
+        <v>442341</v>
       </c>
     </row>
     <row r="117">
@@ -5385,13 +5385,13 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>10682</v>
+        <v>10680</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>10682</v>
+        <v>10680</v>
       </c>
       <c r="E117" t="n">
         <v>14</v>
@@ -5418,7 +5418,7 @@
         <v>2425</v>
       </c>
       <c r="M117" t="n">
-        <v>453274</v>
+        <v>453021</v>
       </c>
     </row>
     <row r="118">
@@ -5428,13 +5428,13 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>9707</v>
+        <v>9706</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>9707</v>
+        <v>9706</v>
       </c>
       <c r="E118" t="n">
         <v>5</v>
@@ -5461,7 +5461,7 @@
         <v>2430</v>
       </c>
       <c r="M118" t="n">
-        <v>462981</v>
+        <v>462727</v>
       </c>
     </row>
     <row r="119">
@@ -5471,13 +5471,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>9102</v>
+        <v>9101</v>
       </c>
       <c r="C119" t="n">
         <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>9102</v>
+        <v>9101</v>
       </c>
       <c r="E119" t="n">
         <v>10</v>
@@ -5504,7 +5504,7 @@
         <v>2440</v>
       </c>
       <c r="M119" t="n">
-        <v>472083</v>
+        <v>471828</v>
       </c>
     </row>
     <row r="120">
@@ -5517,10 +5517,10 @@
         <v>9359</v>
       </c>
       <c r="C120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D120" t="n">
-        <v>9359</v>
+        <v>9358</v>
       </c>
       <c r="E120" t="n">
         <v>12</v>
@@ -5547,7 +5547,7 @@
         <v>2452</v>
       </c>
       <c r="M120" t="n">
-        <v>481442</v>
+        <v>481187</v>
       </c>
     </row>
     <row r="121">
@@ -5560,10 +5560,10 @@
         <v>9835</v>
       </c>
       <c r="C121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D121" t="n">
-        <v>9835</v>
+        <v>9834</v>
       </c>
       <c r="E121" t="n">
         <v>12</v>
@@ -5590,7 +5590,7 @@
         <v>2464</v>
       </c>
       <c r="M121" t="n">
-        <v>491277</v>
+        <v>491022</v>
       </c>
     </row>
     <row r="122">
@@ -5633,7 +5633,7 @@
         <v>2474</v>
       </c>
       <c r="M122" t="n">
-        <v>495329</v>
+        <v>495074</v>
       </c>
     </row>
     <row r="123">
@@ -5676,7 +5676,7 @@
         <v>2484</v>
       </c>
       <c r="M123" t="n">
-        <v>498299</v>
+        <v>498044</v>
       </c>
     </row>
     <row r="124">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>10272</v>
+        <v>10271</v>
       </c>
       <c r="C124" t="n">
         <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>10272</v>
+        <v>10271</v>
       </c>
       <c r="E124" t="n">
         <v>8</v>
@@ -5719,7 +5719,7 @@
         <v>2492</v>
       </c>
       <c r="M124" t="n">
-        <v>508571</v>
+        <v>508315</v>
       </c>
     </row>
     <row r="125">
@@ -5729,13 +5729,13 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>8915</v>
+        <v>8914</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>8915</v>
+        <v>8914</v>
       </c>
       <c r="E125" t="n">
         <v>7</v>
@@ -5762,7 +5762,7 @@
         <v>2499</v>
       </c>
       <c r="M125" t="n">
-        <v>517486</v>
+        <v>517229</v>
       </c>
     </row>
     <row r="126">
@@ -5772,13 +5772,13 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>7990</v>
+        <v>7988</v>
       </c>
       <c r="C126" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D126" t="n">
-        <v>7988</v>
+        <v>7987</v>
       </c>
       <c r="E126" t="n">
         <v>11</v>
@@ -5805,7 +5805,7 @@
         <v>2510</v>
       </c>
       <c r="M126" t="n">
-        <v>525476</v>
+        <v>525217</v>
       </c>
     </row>
     <row r="127">
@@ -5815,13 +5815,13 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>9079</v>
+        <v>9080</v>
       </c>
       <c r="C127" t="n">
         <v>2</v>
       </c>
       <c r="D127" t="n">
-        <v>9077</v>
+        <v>9078</v>
       </c>
       <c r="E127" t="n">
         <v>8</v>
@@ -5848,7 +5848,7 @@
         <v>2518</v>
       </c>
       <c r="M127" t="n">
-        <v>534555</v>
+        <v>534297</v>
       </c>
     </row>
     <row r="128">
@@ -5891,7 +5891,7 @@
         <v>2527</v>
       </c>
       <c r="M128" t="n">
-        <v>539769</v>
+        <v>539511</v>
       </c>
     </row>
     <row r="129">
@@ -5934,7 +5934,7 @@
         <v>2535</v>
       </c>
       <c r="M129" t="n">
-        <v>541861</v>
+        <v>541603</v>
       </c>
     </row>
     <row r="130">
@@ -5947,10 +5947,10 @@
         <v>2707</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>2706</v>
+        <v>2707</v>
       </c>
       <c r="E130" t="n">
         <v>11</v>
@@ -5977,7 +5977,7 @@
         <v>2546</v>
       </c>
       <c r="M130" t="n">
-        <v>544568</v>
+        <v>544310</v>
       </c>
     </row>
     <row r="131">
@@ -5990,10 +5990,10 @@
         <v>11266</v>
       </c>
       <c r="C131" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>11264</v>
+        <v>11266</v>
       </c>
       <c r="E131" t="n">
         <v>14</v>
@@ -6020,7 +6020,7 @@
         <v>2560</v>
       </c>
       <c r="M131" t="n">
-        <v>555834</v>
+        <v>555576</v>
       </c>
     </row>
     <row r="132">
@@ -6030,13 +6030,13 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>9850</v>
+        <v>9851</v>
       </c>
       <c r="C132" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D132" t="n">
-        <v>9846</v>
+        <v>9849</v>
       </c>
       <c r="E132" t="n">
         <v>6</v>
@@ -6063,7 +6063,7 @@
         <v>2566</v>
       </c>
       <c r="M132" t="n">
-        <v>565684</v>
+        <v>565427</v>
       </c>
     </row>
     <row r="133">
@@ -6073,13 +6073,13 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>9002</v>
+        <v>9005</v>
       </c>
       <c r="C133" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D133" t="n">
-        <v>8997</v>
+        <v>9003</v>
       </c>
       <c r="E133" t="n">
         <v>8</v>
@@ -6106,7 +6106,7 @@
         <v>2574</v>
       </c>
       <c r="M133" t="n">
-        <v>574686</v>
+        <v>574432</v>
       </c>
     </row>
     <row r="134">
@@ -6119,10 +6119,10 @@
         <v>8950</v>
       </c>
       <c r="C134" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D134" t="n">
-        <v>8941</v>
+        <v>8948</v>
       </c>
       <c r="E134" t="n">
         <v>10</v>
@@ -6149,7 +6149,7 @@
         <v>2584</v>
       </c>
       <c r="M134" t="n">
-        <v>583636</v>
+        <v>583382</v>
       </c>
     </row>
     <row r="135">
@@ -6159,13 +6159,13 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>10262</v>
+        <v>10266</v>
       </c>
       <c r="C135" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D135" t="n">
-        <v>10251</v>
+        <v>10261</v>
       </c>
       <c r="E135" t="n">
         <v>7</v>
@@ -6192,7 +6192,7 @@
         <v>2591</v>
       </c>
       <c r="M135" t="n">
-        <v>593898</v>
+        <v>593648</v>
       </c>
     </row>
     <row r="136">
@@ -6202,10 +6202,10 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>4820</v>
+        <v>4828</v>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D136" t="n">
         <v>4820</v>
@@ -6235,7 +6235,7 @@
         <v>2599</v>
       </c>
       <c r="M136" t="n">
-        <v>598718</v>
+        <v>598476</v>
       </c>
     </row>
     <row r="137">
@@ -6245,13 +6245,13 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>3480</v>
+        <v>3483</v>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137" t="n">
-        <v>3480</v>
+        <v>3482</v>
       </c>
       <c r="E137" t="n">
         <v>13</v>
@@ -6278,7 +6278,7 @@
         <v>2612</v>
       </c>
       <c r="M137" t="n">
-        <v>602198</v>
+        <v>601959</v>
       </c>
     </row>
     <row r="138">
@@ -6288,13 +6288,13 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>12380</v>
+        <v>12389</v>
       </c>
       <c r="C138" t="n">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D138" t="n">
-        <v>12338</v>
+        <v>12378</v>
       </c>
       <c r="E138" t="n">
         <v>9</v>
@@ -6321,7 +6321,7 @@
         <v>2621</v>
       </c>
       <c r="M138" t="n">
-        <v>614578</v>
+        <v>614348</v>
       </c>
     </row>
     <row r="139">
@@ -6331,13 +6331,13 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>11677</v>
+        <v>11686</v>
       </c>
       <c r="C139" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D139" t="n">
-        <v>11668</v>
+        <v>11675</v>
       </c>
       <c r="E139" t="n">
         <v>5</v>
@@ -6364,7 +6364,7 @@
         <v>2626</v>
       </c>
       <c r="M139" t="n">
-        <v>626255</v>
+        <v>626034</v>
       </c>
     </row>
     <row r="140">
@@ -6374,13 +6374,13 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>11274</v>
+        <v>11276</v>
       </c>
       <c r="C140" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D140" t="n">
-        <v>11224</v>
+        <v>11273</v>
       </c>
       <c r="E140" t="n">
         <v>10</v>
@@ -6392,22 +6392,22 @@
         <v>10</v>
       </c>
       <c r="H140" t="n">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I140" t="n">
         <v>0</v>
       </c>
       <c r="J140" t="n">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K140" t="n">
-        <v>54029</v>
+        <v>54028</v>
       </c>
       <c r="L140" t="n">
         <v>2636</v>
       </c>
       <c r="M140" t="n">
-        <v>637529</v>
+        <v>637310</v>
       </c>
     </row>
     <row r="141">
@@ -6417,13 +6417,13 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>12769</v>
+        <v>12773</v>
       </c>
       <c r="C141" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D141" t="n">
-        <v>12766</v>
+        <v>12763</v>
       </c>
       <c r="E141" t="n">
         <v>9</v>
@@ -6444,13 +6444,13 @@
         <v>738</v>
       </c>
       <c r="K141" t="n">
-        <v>54767</v>
+        <v>54766</v>
       </c>
       <c r="L141" t="n">
         <v>2645</v>
       </c>
       <c r="M141" t="n">
-        <v>650298</v>
+        <v>650083</v>
       </c>
     </row>
     <row r="142">
@@ -6460,13 +6460,13 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>13112</v>
+        <v>13109</v>
       </c>
       <c r="C142" t="n">
         <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>13112</v>
+        <v>13109</v>
       </c>
       <c r="E142" t="n">
         <v>9</v>
@@ -6487,13 +6487,13 @@
         <v>833</v>
       </c>
       <c r="K142" t="n">
-        <v>55600</v>
+        <v>55599</v>
       </c>
       <c r="L142" t="n">
         <v>2654</v>
       </c>
       <c r="M142" t="n">
-        <v>663410</v>
+        <v>663192</v>
       </c>
     </row>
     <row r="143">
@@ -6503,13 +6503,13 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>5541</v>
+        <v>5540</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>5541</v>
+        <v>5540</v>
       </c>
       <c r="E143" t="n">
         <v>6</v>
@@ -6530,13 +6530,13 @@
         <v>910</v>
       </c>
       <c r="K143" t="n">
-        <v>56510</v>
+        <v>56509</v>
       </c>
       <c r="L143" t="n">
         <v>2660</v>
       </c>
       <c r="M143" t="n">
-        <v>668951</v>
+        <v>668732</v>
       </c>
     </row>
     <row r="144">
@@ -6573,13 +6573,13 @@
         <v>640</v>
       </c>
       <c r="K144" t="n">
-        <v>57150</v>
+        <v>57149</v>
       </c>
       <c r="L144" t="n">
         <v>2668</v>
       </c>
       <c r="M144" t="n">
-        <v>672021</v>
+        <v>671802</v>
       </c>
     </row>
     <row r="145">
@@ -6589,13 +6589,13 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>12888</v>
+        <v>12884</v>
       </c>
       <c r="C145" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>12886</v>
+        <v>12884</v>
       </c>
       <c r="E145" t="n">
         <v>13</v>
@@ -6616,13 +6616,13 @@
         <v>713</v>
       </c>
       <c r="K145" t="n">
-        <v>57863</v>
+        <v>57862</v>
       </c>
       <c r="L145" t="n">
         <v>2681</v>
       </c>
       <c r="M145" t="n">
-        <v>684909</v>
+        <v>684686</v>
       </c>
     </row>
     <row r="146">
@@ -6635,10 +6635,10 @@
         <v>12499</v>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146" t="n">
-        <v>12498</v>
+        <v>12497</v>
       </c>
       <c r="E146" t="n">
         <v>9</v>
@@ -6659,13 +6659,13 @@
         <v>736</v>
       </c>
       <c r="K146" t="n">
-        <v>58599</v>
+        <v>58598</v>
       </c>
       <c r="L146" t="n">
         <v>2690</v>
       </c>
       <c r="M146" t="n">
-        <v>697408</v>
+        <v>697185</v>
       </c>
     </row>
     <row r="147">
@@ -6675,22 +6675,22 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>11915</v>
+        <v>11912</v>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>11914</v>
+        <v>11912</v>
       </c>
       <c r="E147" t="n">
         <v>13</v>
       </c>
       <c r="F147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G147" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H147" t="n">
         <v>935</v>
@@ -6702,13 +6702,13 @@
         <v>935</v>
       </c>
       <c r="K147" t="n">
-        <v>59534</v>
+        <v>59533</v>
       </c>
       <c r="L147" t="n">
         <v>2703</v>
       </c>
       <c r="M147" t="n">
-        <v>709323</v>
+        <v>709097</v>
       </c>
     </row>
     <row r="148">
@@ -6718,13 +6718,13 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>11950</v>
+        <v>11952</v>
       </c>
       <c r="C148" t="n">
         <v>5</v>
       </c>
       <c r="D148" t="n">
-        <v>11945</v>
+        <v>11947</v>
       </c>
       <c r="E148" t="n">
         <v>10</v>
@@ -6745,13 +6745,13 @@
         <v>997</v>
       </c>
       <c r="K148" t="n">
-        <v>60531</v>
+        <v>60530</v>
       </c>
       <c r="L148" t="n">
         <v>2713</v>
       </c>
       <c r="M148" t="n">
-        <v>721273</v>
+        <v>721049</v>
       </c>
     </row>
     <row r="149">
@@ -6761,13 +6761,13 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>12111</v>
+        <v>12113</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D149" t="n">
-        <v>12111</v>
+        <v>12109</v>
       </c>
       <c r="E149" t="n">
         <v>9</v>
@@ -6788,13 +6788,13 @@
         <v>915</v>
       </c>
       <c r="K149" t="n">
-        <v>61446</v>
+        <v>61445</v>
       </c>
       <c r="L149" t="n">
         <v>2722</v>
       </c>
       <c r="M149" t="n">
-        <v>733384</v>
+        <v>733162</v>
       </c>
     </row>
     <row r="150">
@@ -6804,13 +6804,13 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>4896</v>
+        <v>4901</v>
       </c>
       <c r="C150" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D150" t="n">
-        <v>4885</v>
+        <v>4889</v>
       </c>
       <c r="E150" t="n">
         <v>8</v>
@@ -6822,22 +6822,22 @@
         <v>8</v>
       </c>
       <c r="H150" t="n">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="K150" t="n">
-        <v>62281</v>
+        <v>62279</v>
       </c>
       <c r="L150" t="n">
         <v>2730</v>
       </c>
       <c r="M150" t="n">
-        <v>738280</v>
+        <v>738063</v>
       </c>
     </row>
     <row r="151">
@@ -6850,10 +6850,10 @@
         <v>2467</v>
       </c>
       <c r="C151" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D151" t="n">
-        <v>2464</v>
+        <v>2465</v>
       </c>
       <c r="E151" t="n">
         <v>8</v>
@@ -6874,13 +6874,13 @@
         <v>551</v>
       </c>
       <c r="K151" t="n">
-        <v>62832</v>
+        <v>62830</v>
       </c>
       <c r="L151" t="n">
         <v>2738</v>
       </c>
       <c r="M151" t="n">
-        <v>740747</v>
+        <v>740530</v>
       </c>
     </row>
     <row r="152">
@@ -6890,13 +6890,13 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>12216</v>
+        <v>12215</v>
       </c>
       <c r="C152" t="n">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D152" t="n">
-        <v>12138</v>
+        <v>12199</v>
       </c>
       <c r="E152" t="n">
         <v>4</v>
@@ -6917,13 +6917,13 @@
         <v>801</v>
       </c>
       <c r="K152" t="n">
-        <v>63633</v>
+        <v>63631</v>
       </c>
       <c r="L152" t="n">
         <v>2742</v>
       </c>
       <c r="M152" t="n">
-        <v>752963</v>
+        <v>752745</v>
       </c>
     </row>
     <row r="153">
@@ -6933,13 +6933,13 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>12077</v>
+        <v>12067</v>
       </c>
       <c r="C153" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D153" t="n">
-        <v>12039</v>
+        <v>12061</v>
       </c>
       <c r="E153" t="n">
         <v>6</v>
@@ -6960,13 +6960,13 @@
         <v>615</v>
       </c>
       <c r="K153" t="n">
-        <v>64248</v>
+        <v>64246</v>
       </c>
       <c r="L153" t="n">
         <v>2748</v>
       </c>
       <c r="M153" t="n">
-        <v>765040</v>
+        <v>764812</v>
       </c>
     </row>
     <row r="154">
@@ -6976,13 +6976,13 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>10805</v>
+        <v>10786</v>
       </c>
       <c r="C154" t="n">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="D154" t="n">
-        <v>10745</v>
+        <v>10773</v>
       </c>
       <c r="E154" t="n">
         <v>19</v>
@@ -7003,13 +7003,13 @@
         <v>942</v>
       </c>
       <c r="K154" t="n">
-        <v>65190</v>
+        <v>65188</v>
       </c>
       <c r="L154" t="n">
         <v>2767</v>
       </c>
       <c r="M154" t="n">
-        <v>775845</v>
+        <v>775598</v>
       </c>
     </row>
     <row r="155">
@@ -7019,13 +7019,13 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>10507</v>
+        <v>10528</v>
       </c>
       <c r="C155" t="n">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="D155" t="n">
-        <v>10433</v>
+        <v>10501</v>
       </c>
       <c r="E155" t="n">
         <v>9</v>
@@ -7046,13 +7046,13 @@
         <v>890</v>
       </c>
       <c r="K155" t="n">
-        <v>66080</v>
+        <v>66078</v>
       </c>
       <c r="L155" t="n">
         <v>2776</v>
       </c>
       <c r="M155" t="n">
-        <v>786352</v>
+        <v>786126</v>
       </c>
     </row>
     <row r="156">
@@ -7062,13 +7062,13 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>11300</v>
+        <v>11324</v>
       </c>
       <c r="C156" t="n">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="D156" t="n">
-        <v>11238</v>
+        <v>11296</v>
       </c>
       <c r="E156" t="n">
         <v>8</v>
@@ -7080,22 +7080,22 @@
         <v>8</v>
       </c>
       <c r="H156" t="n">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J156" t="n">
         <v>976</v>
       </c>
       <c r="K156" t="n">
-        <v>67057</v>
+        <v>67054</v>
       </c>
       <c r="L156" t="n">
         <v>2784</v>
       </c>
       <c r="M156" t="n">
-        <v>797652</v>
+        <v>797450</v>
       </c>
     </row>
     <row r="157">
@@ -7105,13 +7105,13 @@
         </is>
       </c>
       <c r="B157" t="n">
+        <v>4504</v>
+      </c>
+      <c r="C157" t="n">
+        <v>22</v>
+      </c>
+      <c r="D157" t="n">
         <v>4482</v>
-      </c>
-      <c r="C157" t="n">
-        <v>46</v>
-      </c>
-      <c r="D157" t="n">
-        <v>4436</v>
       </c>
       <c r="E157" t="n">
         <v>10</v>
@@ -7132,13 +7132,13 @@
         <v>778</v>
       </c>
       <c r="K157" t="n">
-        <v>67835</v>
+        <v>67832</v>
       </c>
       <c r="L157" t="n">
         <v>2794</v>
       </c>
       <c r="M157" t="n">
-        <v>802134</v>
+        <v>801954</v>
       </c>
     </row>
     <row r="158">
@@ -7148,13 +7148,13 @@
         </is>
       </c>
       <c r="B158" t="n">
+        <v>2522</v>
+      </c>
+      <c r="C158" t="n">
+        <v>4</v>
+      </c>
+      <c r="D158" t="n">
         <v>2518</v>
-      </c>
-      <c r="C158" t="n">
-        <v>74</v>
-      </c>
-      <c r="D158" t="n">
-        <v>2444</v>
       </c>
       <c r="E158" t="n">
         <v>9</v>
@@ -7175,13 +7175,13 @@
         <v>574</v>
       </c>
       <c r="K158" t="n">
-        <v>68409</v>
+        <v>68406</v>
       </c>
       <c r="L158" t="n">
         <v>2803</v>
       </c>
       <c r="M158" t="n">
-        <v>804652</v>
+        <v>804476</v>
       </c>
     </row>
     <row r="159">
@@ -7191,22 +7191,22 @@
         </is>
       </c>
       <c r="B159" t="n">
+        <v>11810</v>
+      </c>
+      <c r="C159" t="n">
+        <v>114</v>
+      </c>
+      <c r="D159" t="n">
         <v>11696</v>
       </c>
-      <c r="C159" t="n">
-        <v>145</v>
-      </c>
-      <c r="D159" t="n">
-        <v>11551</v>
-      </c>
       <c r="E159" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F159" t="n">
         <v>1</v>
       </c>
       <c r="G159" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H159" t="n">
         <v>825</v>
@@ -7218,13 +7218,13 @@
         <v>825</v>
       </c>
       <c r="K159" t="n">
-        <v>69234</v>
+        <v>69231</v>
       </c>
       <c r="L159" t="n">
-        <v>2811</v>
+        <v>2812</v>
       </c>
       <c r="M159" t="n">
-        <v>816348</v>
+        <v>816286</v>
       </c>
     </row>
     <row r="160">
@@ -7234,13 +7234,13 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>11332</v>
+        <v>11492</v>
       </c>
       <c r="C160" t="n">
-        <v>470</v>
+        <v>163</v>
       </c>
       <c r="D160" t="n">
-        <v>10862</v>
+        <v>11329</v>
       </c>
       <c r="E160" t="n">
         <v>7</v>
@@ -7261,13 +7261,13 @@
         <v>729</v>
       </c>
       <c r="K160" t="n">
-        <v>69963</v>
+        <v>69960</v>
       </c>
       <c r="L160" t="n">
-        <v>2818</v>
+        <v>2819</v>
       </c>
       <c r="M160" t="n">
-        <v>827680</v>
+        <v>827778</v>
       </c>
     </row>
     <row r="161">
@@ -7277,40 +7277,40 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>10268</v>
+        <v>10655</v>
       </c>
       <c r="C161" t="n">
-        <v>559</v>
+        <v>385</v>
       </c>
       <c r="D161" t="n">
-        <v>9709</v>
+        <v>10270</v>
       </c>
       <c r="E161" t="n">
         <v>4</v>
       </c>
       <c r="F161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H161" t="n">
         <v>1038</v>
       </c>
       <c r="I161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J161" t="n">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="K161" t="n">
-        <v>71001</v>
+        <v>70998</v>
       </c>
       <c r="L161" t="n">
-        <v>2822</v>
+        <v>2823</v>
       </c>
       <c r="M161" t="n">
-        <v>837948</v>
+        <v>838433</v>
       </c>
     </row>
     <row r="162">
@@ -7320,40 +7320,40 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>10020</v>
+        <v>10775</v>
       </c>
       <c r="C162" t="n">
-        <v>733</v>
+        <v>762</v>
       </c>
       <c r="D162" t="n">
-        <v>9287</v>
+        <v>10013</v>
       </c>
       <c r="E162" t="n">
+        <v>12</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1</v>
+      </c>
+      <c r="G162" t="n">
         <v>11</v>
-      </c>
-      <c r="F162" t="n">
-        <v>2</v>
-      </c>
-      <c r="G162" t="n">
-        <v>9</v>
       </c>
       <c r="H162" t="n">
         <v>1249</v>
       </c>
       <c r="I162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J162" t="n">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="K162" t="n">
-        <v>72250</v>
+        <v>72247</v>
       </c>
       <c r="L162" t="n">
-        <v>2833</v>
+        <v>2835</v>
       </c>
       <c r="M162" t="n">
-        <v>847968</v>
+        <v>849208</v>
       </c>
     </row>
     <row r="163">
@@ -7363,40 +7363,40 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>9971</v>
+        <v>10866</v>
       </c>
       <c r="C163" t="n">
-        <v>4598</v>
+        <v>915</v>
       </c>
       <c r="D163" t="n">
-        <v>5373</v>
+        <v>9951</v>
       </c>
       <c r="E163" t="n">
+        <v>12</v>
+      </c>
+      <c r="F163" t="n">
+        <v>1</v>
+      </c>
+      <c r="G163" t="n">
         <v>11</v>
       </c>
-      <c r="F163" t="n">
-        <v>4</v>
-      </c>
-      <c r="G163" t="n">
-        <v>7</v>
-      </c>
       <c r="H163" t="n">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="I163" t="n">
         <v>1</v>
       </c>
       <c r="J163" t="n">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="K163" t="n">
-        <v>73277</v>
+        <v>73276</v>
       </c>
       <c r="L163" t="n">
-        <v>2844</v>
+        <v>2847</v>
       </c>
       <c r="M163" t="n">
-        <v>857939</v>
+        <v>860074</v>
       </c>
     </row>
     <row r="164">
@@ -7406,40 +7406,40 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>2828</v>
+        <v>3391</v>
       </c>
       <c r="C164" t="n">
-        <v>1719</v>
+        <v>567</v>
       </c>
       <c r="D164" t="n">
-        <v>1109</v>
+        <v>2824</v>
       </c>
       <c r="E164" t="n">
+        <v>7</v>
+      </c>
+      <c r="F164" t="n">
+        <v>1</v>
+      </c>
+      <c r="G164" t="n">
         <v>6</v>
       </c>
-      <c r="F164" t="n">
-        <v>4</v>
-      </c>
-      <c r="G164" t="n">
-        <v>2</v>
-      </c>
       <c r="H164" t="n">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="K164" t="n">
-        <v>74313</v>
+        <v>74311</v>
       </c>
       <c r="L164" t="n">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="M164" t="n">
-        <v>860767</v>
+        <v>863465</v>
       </c>
     </row>
     <row r="165">
@@ -7449,40 +7449,40 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>710</v>
+        <v>1450</v>
       </c>
       <c r="C165" t="n">
-        <v>608</v>
+        <v>744</v>
       </c>
       <c r="D165" t="n">
-        <v>102</v>
+        <v>706</v>
       </c>
       <c r="E165" t="n">
         <v>6</v>
       </c>
       <c r="F165" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G165" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H165" t="n">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I165" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J165" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="K165" t="n">
-        <v>74982</v>
+        <v>74979</v>
       </c>
       <c r="L165" t="n">
-        <v>2856</v>
+        <v>2860</v>
       </c>
       <c r="M165" t="n">
-        <v>861477</v>
+        <v>864915</v>
       </c>
     </row>
     <row r="166">
@@ -7492,40 +7492,83 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>178</v>
+        <v>1875</v>
       </c>
       <c r="C166" t="n">
-        <v>178</v>
+        <v>1701</v>
       </c>
       <c r="D166" t="n">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="E166" t="n">
+        <v>15</v>
+      </c>
+      <c r="F166" t="n">
+        <v>8</v>
+      </c>
+      <c r="G166" t="n">
         <v>7</v>
       </c>
-      <c r="F166" t="n">
-        <v>7</v>
-      </c>
-      <c r="G166" t="n">
-        <v>0</v>
-      </c>
       <c r="H166" t="n">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="I166" t="n">
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="J166" t="n">
-        <v>0</v>
+        <v>876</v>
       </c>
       <c r="K166" t="n">
-        <v>75862</v>
+        <v>75855</v>
       </c>
       <c r="L166" t="n">
-        <v>2863</v>
+        <v>2875</v>
       </c>
       <c r="M166" t="n">
-        <v>861655</v>
+        <v>866790</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2020-08-11</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>204</v>
+      </c>
+      <c r="C167" t="n">
+        <v>204</v>
+      </c>
+      <c r="D167" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" t="n">
+        <v>3</v>
+      </c>
+      <c r="F167" t="n">
+        <v>3</v>
+      </c>
+      <c r="G167" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" t="n">
+        <v>667</v>
+      </c>
+      <c r="I167" t="n">
+        <v>667</v>
+      </c>
+      <c r="J167" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" t="n">
+        <v>76522</v>
+      </c>
+      <c r="L167" t="n">
+        <v>2878</v>
+      </c>
+      <c r="M167" t="n">
+        <v>866994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>